<commit_message>
update in press and submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="411">
   <si>
     <t>title</t>
   </si>
@@ -1231,10 +1231,25 @@
     <t>Braae, Uffe Christian; Devleesschauwer, Brecht; Sithole, Fortune; Wang, Ziqi; Willingham, Arve Lee</t>
   </si>
   <si>
-    <t>Am. J. Trop. Med. Hyg.</t>
-  </si>
-  <si>
-    <t>The American Journal of Tropical Medicine and Hygiene</t>
+    <t>Contribution of fortified foods and supplements to the adequacy of fat soluble vitamin intake in the Belgian population</t>
+  </si>
+  <si>
+    <t>Moyersoen, Isabelle; Devleesschauwer, Brecht; Dekkers, Arnold; De Ridder, Karin; Tafforeau, Jean; Van Camp, John; Van Oyen, Herman; Lachat, Carl</t>
+  </si>
+  <si>
+    <t>Nutrients</t>
+  </si>
+  <si>
+    <t>Malaria Journal</t>
+  </si>
+  <si>
+    <t>Malar. J.</t>
+  </si>
+  <si>
+    <t>True malaria prevalence in children under five: Bayesian estimation using data of malaria household surveys from three sub-Saharan countries</t>
+  </si>
+  <si>
+    <t>Mfueni, Elvire; Devleesschauwer, Brecht; Van Malderen, Carine; Rosas-Aguirre, Angel; Brandt, Patrick; Dorsey, Grant; Ogutu, Bernhards; Snow, Robert W; Tshilolo, Léon; Zurovac, Dejan; Vanderelst, Dieter; Speybroeck, Niko</t>
   </si>
 </sst>
 </file>
@@ -1630,8 +1645,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:Q64" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
-  <autoFilter ref="A1:Q64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:Q65" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:Q65"/>
   <sortState ref="A2:Q61">
     <sortCondition ref="K1:K61"/>
   </sortState>
@@ -1681,8 +1696,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:F16"/>
   <sortState ref="A2:F17">
     <sortCondition ref="E1:E17"/>
   </sortState>
@@ -2013,11 +2028,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4060,7 +4073,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>134</v>
       </c>
@@ -4109,7 +4122,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>131</v>
       </c>
@@ -4207,7 +4220,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>163</v>
       </c>
@@ -4256,7 +4269,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>155</v>
       </c>
@@ -4354,7 +4367,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>178</v>
       </c>
@@ -4452,7 +4465,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>375</v>
       </c>
@@ -4501,7 +4514,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>302</v>
       </c>
@@ -4548,7 +4561,7 @@
       <c r="P50" s="28"/>
       <c r="Q50" s="29"/>
     </row>
-    <row r="51" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>169</v>
       </c>
@@ -4687,7 +4700,7 @@
       <c r="P53" s="28"/>
       <c r="Q53" s="29"/>
     </row>
-    <row r="54" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>135</v>
       </c>
@@ -4732,7 +4745,7 @@
       <c r="P54" s="28"/>
       <c r="Q54" s="29"/>
     </row>
-    <row r="55" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>352</v>
       </c>
@@ -4826,7 +4839,7 @@
       <c r="P56" s="28"/>
       <c r="Q56" s="29"/>
     </row>
-    <row r="57" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>250</v>
       </c>
@@ -4922,7 +4935,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>347</v>
       </c>
@@ -4967,7 +4980,7 @@
       <c r="P59" s="28"/>
       <c r="Q59" s="29"/>
     </row>
-    <row r="60" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>359</v>
       </c>
@@ -5012,7 +5025,7 @@
       <c r="P60" s="28"/>
       <c r="Q60" s="29"/>
     </row>
-    <row r="61" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="14" t="s">
         <v>369</v>
       </c>
@@ -5057,7 +5070,7 @@
       <c r="P61" s="31"/>
       <c r="Q61" s="14"/>
     </row>
-    <row r="62" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="39" t="s">
         <v>355</v>
       </c>
@@ -5143,7 +5156,7 @@
       <c r="P63" s="31"/>
       <c r="Q63" s="14"/>
     </row>
-    <row r="64" spans="1:17" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="14" t="s">
         <v>298</v>
       </c>
@@ -5185,6 +5198,49 @@
       <c r="O64" s="14"/>
       <c r="P64" s="31"/>
       <c r="Q64" s="14"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B65" s="39" t="s">
+        <v>395</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E65" s="15">
+        <v>2017</v>
+      </c>
+      <c r="F65" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K65" s="42">
+        <v>43106</v>
+      </c>
+      <c r="L65" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="M65" s="18"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="31"/>
+      <c r="Q65" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5345,9 +5401,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5394,8 +5450,8 @@
         <v>41904</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F15" ca="1" si="0">TODAY()-E2</f>
-        <v>1005</v>
+        <f t="shared" ref="F2:F16" ca="1" si="0">TODAY()-E2</f>
+        <v>1008</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5416,7 +5472,7 @@
       </c>
       <c r="F3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>568</v>
+        <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5437,7 +5493,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5458,7 +5514,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5479,7 +5535,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5500,7 +5556,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5521,7 +5577,7 @@
       </c>
       <c r="F8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5542,7 +5598,7 @@
       </c>
       <c r="F9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5563,7 +5619,7 @@
       </c>
       <c r="F10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5584,7 +5640,7 @@
       </c>
       <c r="F11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5605,7 +5661,7 @@
       </c>
       <c r="F12" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
@@ -5626,15 +5682,15 @@
       </c>
       <c r="F13" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>26</v>
@@ -5643,32 +5699,53 @@
         <v>29</v>
       </c>
       <c r="E14" s="10">
-        <v>42839</v>
+        <v>42911</v>
       </c>
       <c r="F14" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E15" s="10">
-        <v>42909</v>
+        <v>42914</v>
       </c>
       <c r="F15" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E16" s="10">
+        <v>42913</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -5774,7 +5851,7 @@
       </c>
       <c r="L2" s="13">
         <f t="shared" ref="L2:L3" ca="1" si="0">TODAY()-K2</f>
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -5813,7 +5890,7 @@
       </c>
       <c r="L3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -5838,7 +5915,7 @@
       <c r="K4" s="22"/>
       <c r="L4" s="10">
         <f ca="1">TODAY()-K4</f>
-        <v>42909</v>
+        <v>42912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add doi, new submission
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="231" windowWidth="14811" windowHeight="7894"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="submitted" sheetId="4" r:id="rId3"/>
     <sheet name="zzz" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="466">
   <si>
     <t>title</t>
   </si>
@@ -1327,9 +1327,6 @@
     <t>10.1007/978-3-319-67664-7_15</t>
   </si>
   <si>
-    <t>Preliminary assessment of the computer-based Taenia solium educational program `The Vicious Worm' on knowledge uptake in primary school children in rural areas in eastern Zambia</t>
-  </si>
-  <si>
     <t>10.1371/journal.pone.0183641</t>
   </si>
   <si>
@@ -1400,12 +1397,30 @@
   </si>
   <si>
     <t>10.1016/j.vetpar.2018.01.001</t>
+  </si>
+  <si>
+    <t>Preliminary assessment of the computer-based Taenia solium educational program 'The Vicious Worm' on knowledge uptake in primary school children in rural areas in eastern Zambia</t>
+  </si>
+  <si>
+    <t>10.1111/tmi.13029</t>
+  </si>
+  <si>
+    <t>BMC Veterinary Research</t>
+  </si>
+  <si>
+    <t>BMC Vet. Res.</t>
+  </si>
+  <si>
+    <t>Do current fortification and supplementation programs assure adequate intake of fat soluble vitamins in Belgian infants, toddlers, and pregnant and lactating women?</t>
+  </si>
+  <si>
+    <t>Moyersoen, Isabelle; Lachat, Carl; Cuypers, Koenraad; De Ridder, Karin; Devleesschauwer, Brecht; Tafforeau, Jean; Vandevijvere, Stefanie; Vansteenland, Margot; De Meulenaer, Bruno; Van Camp, John; Van Oyen, Herman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1636,9 +1651,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="53">
     <dxf>
@@ -1876,10 +1891,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:F9"/>
-  <sortState ref="A2:F16">
-    <sortCondition ref="E1:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F10" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:F10"/>
+  <sortState ref="A2:F10">
+    <sortCondition ref="E1:E10"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="title" dataDxfId="19"/>
@@ -1922,9 +1937,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1962,9 +1977,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1997,26 +2012,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2049,26 +2047,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2244,26 +2225,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.69140625" customWidth="1"/>
-    <col min="3" max="3" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.07421875" style="1"/>
-    <col min="8" max="8" width="9.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.07421875" style="2"/>
-    <col min="11" max="11" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.3046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="2"/>
+    <col min="11" max="11" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2300,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2369,7 +2350,7 @@
       </c>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>40</v>
       </c>
@@ -2421,7 +2402,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -2473,7 +2454,7 @@
       </c>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2525,7 +2506,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2577,7 +2558,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2608,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
@@ -2679,7 +2660,7 @@
       </c>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -2731,7 +2712,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -2783,7 +2764,7 @@
       </c>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -2835,7 +2816,7 @@
       </c>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
@@ -2887,7 +2868,7 @@
       </c>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -2939,7 +2920,7 @@
       </c>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
@@ -2991,7 +2972,7 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3024,7 @@
       </c>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -3095,7 +3076,7 @@
       </c>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -3147,7 +3128,7 @@
       </c>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -3199,7 +3180,7 @@
       </c>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>76</v>
       </c>
@@ -3251,7 +3232,7 @@
       </c>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>92</v>
       </c>
@@ -3303,7 +3284,7 @@
       </c>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>75</v>
       </c>
@@ -3355,7 +3336,7 @@
       </c>
       <c r="R21" s="7"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>74</v>
       </c>
@@ -3407,7 +3388,7 @@
       </c>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>106</v>
       </c>
@@ -3459,7 +3440,7 @@
       </c>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -3511,7 +3492,7 @@
       </c>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
         <v>130</v>
       </c>
@@ -3563,7 +3544,7 @@
       </c>
       <c r="R25" s="7"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -3615,7 +3596,7 @@
       </c>
       <c r="R26" s="7"/>
     </row>
-    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>100</v>
       </c>
@@ -3667,7 +3648,7 @@
       </c>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>141</v>
       </c>
@@ -3719,7 +3700,7 @@
       </c>
       <c r="R28" s="7"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
         <v>120</v>
       </c>
@@ -3771,7 +3752,7 @@
       </c>
       <c r="R29" s="7"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>113</v>
       </c>
@@ -3823,7 +3804,7 @@
       </c>
       <c r="R30" s="7"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>122</v>
       </c>
@@ -3875,7 +3856,7 @@
       </c>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A32" s="7" t="s">
         <v>194</v>
       </c>
@@ -3927,7 +3908,7 @@
       </c>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>128</v>
       </c>
@@ -3979,7 +3960,7 @@
       </c>
       <c r="R33" s="7"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>147</v>
       </c>
@@ -4031,7 +4012,7 @@
       </c>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>126</v>
       </c>
@@ -4083,7 +4064,7 @@
       </c>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>158</v>
       </c>
@@ -4135,7 +4116,7 @@
       </c>
       <c r="R36" s="7"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>168</v>
       </c>
@@ -4187,7 +4168,7 @@
       </c>
       <c r="R37" s="7"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -4239,7 +4220,7 @@
       </c>
       <c r="R38" s="7"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>144</v>
       </c>
@@ -4293,7 +4274,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>162</v>
       </c>
@@ -4347,7 +4328,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>134</v>
       </c>
@@ -4401,7 +4382,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
         <v>131</v>
       </c>
@@ -4455,7 +4436,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>171</v>
       </c>
@@ -4509,7 +4490,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>163</v>
       </c>
@@ -4563,7 +4544,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>155</v>
       </c>
@@ -4617,7 +4598,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>255</v>
       </c>
@@ -4671,7 +4652,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
         <v>178</v>
       </c>
@@ -4725,7 +4706,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>262</v>
       </c>
@@ -4779,7 +4760,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
         <v>365</v>
       </c>
@@ -4833,7 +4814,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
         <v>298</v>
       </c>
@@ -4885,7 +4866,7 @@
       </c>
       <c r="R50" s="7"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
         <v>169</v>
       </c>
@@ -4939,7 +4920,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>265</v>
       </c>
@@ -4993,7 +4974,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>139</v>
       </c>
@@ -5039,7 +5020,7 @@
       <c r="Q53" s="29"/>
       <c r="R53" s="7"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
         <v>135</v>
       </c>
@@ -5085,7 +5066,7 @@
       <c r="Q54" s="29"/>
       <c r="R54" s="7"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
         <v>345</v>
       </c>
@@ -5131,7 +5112,7 @@
       <c r="Q55" s="29"/>
       <c r="R55" s="7"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>273</v>
       </c>
@@ -5177,7 +5158,7 @@
       <c r="Q56" s="29"/>
       <c r="R56" s="7"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
         <v>249</v>
       </c>
@@ -5223,7 +5204,7 @@
       <c r="Q57" s="29"/>
       <c r="R57" s="7"/>
     </row>
-    <row r="58" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>271</v>
       </c>
@@ -5269,7 +5250,7 @@
       <c r="Q58" s="29"/>
       <c r="R58" s="7"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
         <v>351</v>
       </c>
@@ -5315,7 +5296,7 @@
       <c r="Q59" s="29"/>
       <c r="R59" s="7"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>420</v>
       </c>
@@ -5361,7 +5342,7 @@
       <c r="Q60" s="29"/>
       <c r="R60" s="7"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
         <v>430</v>
       </c>
@@ -5407,7 +5388,7 @@
       <c r="Q61" s="29"/>
       <c r="R61" s="7"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
         <v>359</v>
       </c>
@@ -5453,7 +5434,7 @@
       <c r="Q62" s="29"/>
       <c r="R62" s="7"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A63" s="7" t="s">
         <v>340</v>
       </c>
@@ -5499,7 +5480,7 @@
       <c r="Q63" s="29"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>424</v>
       </c>
@@ -5519,10 +5500,10 @@
         <v>12</v>
       </c>
       <c r="G64" s="41" t="s">
+        <v>437</v>
+      </c>
+      <c r="H64" s="41" t="s">
         <v>438</v>
-      </c>
-      <c r="H64" s="41" t="s">
-        <v>439</v>
       </c>
       <c r="I64" s="41" t="s">
         <v>14</v>
@@ -5538,14 +5519,14 @@
       </c>
       <c r="M64" s="7"/>
       <c r="N64" s="22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="O64" s="7"/>
       <c r="P64" s="28"/>
       <c r="Q64" s="29"/>
       <c r="R64" s="7"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A65" s="7" t="s">
         <v>388</v>
       </c>
@@ -5584,16 +5565,16 @@
       </c>
       <c r="M65" s="7"/>
       <c r="N65" s="22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="O65" s="7"/>
       <c r="P65" s="28"/>
       <c r="Q65" s="29"/>
       <c r="R65" s="7"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>348</v>
@@ -5630,14 +5611,14 @@
       </c>
       <c r="M66" s="7"/>
       <c r="N66" s="22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="O66" s="7"/>
       <c r="P66" s="28"/>
       <c r="Q66" s="29"/>
       <c r="R66" s="7"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A67" s="7" t="s">
         <v>369</v>
       </c>
@@ -5676,14 +5657,14 @@
       </c>
       <c r="M67" s="7"/>
       <c r="N67" s="22" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="O67" s="7"/>
       <c r="P67" s="28"/>
       <c r="Q67" s="29"/>
       <c r="R67" s="7"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>378</v>
       </c>
@@ -5729,7 +5710,7 @@
       <c r="Q68" s="29"/>
       <c r="R68" s="7"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>374</v>
       </c>
@@ -5775,12 +5756,12 @@
       <c r="Q69" s="29"/>
       <c r="R69" s="7"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>450</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>451</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>26</v>
@@ -5814,25 +5795,25 @@
       </c>
       <c r="M70" s="7"/>
       <c r="N70" s="22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="O70" s="7"/>
       <c r="P70" s="28"/>
       <c r="Q70" s="29"/>
       <c r="R70" s="7"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A71" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C71" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>453</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>454</v>
       </c>
       <c r="E71" s="7">
         <v>2017</v>
@@ -5860,25 +5841,25 @@
       </c>
       <c r="M71" s="11"/>
       <c r="N71" s="23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O71" s="7"/>
       <c r="P71" s="27"/>
       <c r="Q71" s="7"/>
       <c r="R71" s="7"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>433</v>
+        <v>294</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>295</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>59</v>
+        <v>296</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>60</v>
+        <v>339</v>
       </c>
       <c r="E72" s="15">
         <v>2018</v>
@@ -5899,78 +5880,78 @@
         <v>14</v>
       </c>
       <c r="K72" s="43">
-        <v>43471</v>
+        <v>43466</v>
       </c>
       <c r="L72" s="43" t="s">
         <v>282</v>
       </c>
       <c r="M72" s="18"/>
       <c r="N72" s="16" t="s">
-        <v>460</v>
+        <v>423</v>
       </c>
       <c r="O72" s="14"/>
       <c r="P72" s="31"/>
       <c r="Q72" s="14"/>
       <c r="R72" s="7"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="B73" s="32" t="s">
-        <v>295</v>
+        <v>397</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>398</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>296</v>
+        <v>418</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="E73" s="15">
         <v>2018</v>
       </c>
-      <c r="F73" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="G73" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="H73" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="I73" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="J73" s="53" t="s">
+      <c r="F73" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H73" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="44" t="s">
         <v>14</v>
       </c>
       <c r="K73" s="43">
-        <v>43466</v>
-      </c>
-      <c r="L73" s="55" t="s">
-        <v>282</v>
-      </c>
-      <c r="M73" s="18"/>
-      <c r="N73" s="16" t="s">
-        <v>423</v>
-      </c>
-      <c r="O73" s="14"/>
-      <c r="P73" s="31"/>
-      <c r="Q73" s="14"/>
+        <v>43467</v>
+      </c>
+      <c r="L73" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="M73" s="34"/>
+      <c r="N73" s="35" t="s">
+        <v>448</v>
+      </c>
+      <c r="O73" s="36"/>
+      <c r="P73" s="37"/>
+      <c r="Q73" s="36"/>
       <c r="R73" s="7"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="14" t="s">
-        <v>397</v>
+        <v>425</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>398</v>
+        <v>426</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="E74" s="15">
         <v>2018</v>
@@ -5991,32 +5972,32 @@
         <v>14</v>
       </c>
       <c r="K74" s="43">
-        <v>43467</v>
-      </c>
-      <c r="L74" s="46" t="s">
-        <v>282</v>
-      </c>
-      <c r="M74" s="34"/>
+        <v>43468</v>
+      </c>
+      <c r="L74" s="49" t="s">
+        <v>283</v>
+      </c>
+      <c r="M74" s="50"/>
       <c r="N74" s="35" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="O74" s="36"/>
       <c r="P74" s="37"/>
       <c r="Q74" s="36"/>
       <c r="R74" s="7"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="14" t="s">
-        <v>425</v>
+        <v>277</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>426</v>
+        <v>278</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="E75" s="15">
         <v>2018</v>
@@ -6037,7 +6018,7 @@
         <v>14</v>
       </c>
       <c r="K75" s="43">
-        <v>43468</v>
+        <v>43469</v>
       </c>
       <c r="L75" s="52" t="s">
         <v>283</v>
@@ -6051,18 +6032,18 @@
       <c r="Q75" s="36"/>
       <c r="R75" s="7"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="14" t="s">
-        <v>277</v>
+        <v>442</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>278</v>
+        <v>443</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="E76" s="15">
         <v>2018</v>
@@ -6083,12 +6064,12 @@
         <v>14</v>
       </c>
       <c r="K76" s="43">
-        <v>43469</v>
-      </c>
-      <c r="L76" s="49" t="s">
-        <v>283</v>
-      </c>
-      <c r="M76" s="50"/>
+        <v>43470</v>
+      </c>
+      <c r="L76" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="M76" s="34"/>
       <c r="N76" s="35" t="s">
         <v>458</v>
       </c>
@@ -6097,81 +6078,81 @@
       <c r="Q76" s="36"/>
       <c r="R76" s="7"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>441</v>
+        <v>59</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>442</v>
+        <v>60</v>
       </c>
       <c r="E77" s="15">
         <v>2018</v>
       </c>
-      <c r="F77" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="H77" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="J77" s="44" t="s">
+      <c r="F77" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G77" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="53" t="s">
         <v>14</v>
       </c>
       <c r="K77" s="43">
-        <v>43470</v>
-      </c>
-      <c r="L77" s="46" t="s">
-        <v>282</v>
-      </c>
-      <c r="M77" s="34"/>
-      <c r="N77" s="35" t="s">
+        <v>43471</v>
+      </c>
+      <c r="L77" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="M77" s="18"/>
+      <c r="N77" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="O77" s="36"/>
-      <c r="P77" s="37"/>
-      <c r="Q77" s="36"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="31"/>
+      <c r="Q77" s="14"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A78" s="14" t="s">
-        <v>346</v>
+        <v>460</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>347</v>
+        <v>434</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>349</v>
+        <v>422</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>350</v>
+        <v>56</v>
       </c>
       <c r="E78" s="15">
         <v>2018</v>
       </c>
-      <c r="F78" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="G78" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="H78" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="J78" s="44" t="s">
+      <c r="F78" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G78" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="J78" s="53" t="s">
         <v>14</v>
       </c>
       <c r="K78" s="43">
@@ -6181,41 +6162,43 @@
         <v>282</v>
       </c>
       <c r="M78" s="34"/>
-      <c r="N78" s="35"/>
+      <c r="N78" s="35" t="s">
+        <v>461</v>
+      </c>
       <c r="O78" s="36"/>
       <c r="P78" s="37"/>
       <c r="Q78" s="36"/>
       <c r="R78" s="7"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="14" t="s">
-        <v>436</v>
+        <v>346</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>434</v>
+        <v>347</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>422</v>
+        <v>349</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>56</v>
+        <v>350</v>
       </c>
       <c r="E79" s="15">
         <v>2018</v>
       </c>
-      <c r="F79" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="G79" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="H79" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="I79" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="J79" s="53" t="s">
+      <c r="F79" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J79" s="44" t="s">
         <v>14</v>
       </c>
       <c r="K79" s="43">
@@ -6245,20 +6228,20 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="30.69140625" customWidth="1"/>
-    <col min="4" max="4" width="24.07421875" customWidth="1"/>
-    <col min="6" max="7" width="8.84375" style="2"/>
-    <col min="8" max="8" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6290,7 +6273,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
@@ -6322,7 +6305,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>285</v>
       </c>
@@ -6352,7 +6335,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>286</v>
       </c>
@@ -6392,21 +6375,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="40.69140625" customWidth="1"/>
-    <col min="3" max="4" width="16.69140625" customWidth="1"/>
-    <col min="5" max="5" width="12.69140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6409,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>161</v>
       </c>
@@ -6443,11 +6426,11 @@
         <v>42502</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F9" ca="1" si="0">TODAY()-E2</f>
+        <f ca="1">TODAY()-E2</f>
         <v>602</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>264</v>
       </c>
@@ -6464,11 +6447,11 @@
         <v>42535</v>
       </c>
       <c r="F3" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">TODAY()-E3</f>
         <v>569</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>357</v>
       </c>
@@ -6485,11 +6468,11 @@
         <v>42717</v>
       </c>
       <c r="F4" s="13">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">TODAY()-E4</f>
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>382</v>
       </c>
@@ -6506,11 +6489,11 @@
         <v>42837</v>
       </c>
       <c r="F5" s="13">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">TODAY()-E5</f>
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>394</v>
       </c>
@@ -6527,11 +6510,11 @@
         <v>42913</v>
       </c>
       <c r="F6" s="13">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">TODAY()-E6</f>
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>400</v>
       </c>
@@ -6548,50 +6531,71 @@
         <v>42941</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">TODAY()-E7</f>
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="10">
+        <v>43000</v>
+      </c>
+      <c r="F8" s="12">
+        <f ca="1">TODAY()-E8</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="10">
-        <v>42989</v>
-      </c>
-      <c r="F8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>447</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>165</v>
+        <v>462</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>166</v>
+        <v>463</v>
       </c>
       <c r="E9" s="10">
-        <v>43000</v>
+        <v>43103</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <f ca="1">TODAY()-E9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="E10" s="10">
+        <v>43104</v>
+      </c>
+      <c r="F10" s="12">
+        <f ca="1">TODAY()-E10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6609,19 +6613,19 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.69140625" customWidth="1"/>
-    <col min="3" max="3" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.07421875" style="1"/>
-    <col min="8" max="10" width="9.07421875" style="2"/>
-    <col min="11" max="11" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="10" width="9.109375" style="2"/>
+    <col min="11" max="11" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6659,7 +6663,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>173</v>
       </c>
@@ -6698,7 +6702,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
new accepted / update PhD students
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="231" windowWidth="14811" windowHeight="7894"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="submitted" sheetId="4" r:id="rId3"/>
     <sheet name="zzz" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="492">
   <si>
     <t>title</t>
   </si>
@@ -1498,7 +1498,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1693,9 +1693,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="53">
     <dxf>
@@ -1881,8 +1881,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:R83" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
-  <autoFilter ref="A1:R83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:R84" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:R84"/>
   <sortState ref="A2:R83">
     <sortCondition ref="K1:K83"/>
   </sortState>
@@ -1933,8 +1933,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F13" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F12" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:F12"/>
   <sortState ref="A2:F14">
     <sortCondition ref="E1:E14"/>
   </sortState>
@@ -1979,7 +1979,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2021,7 +2021,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2054,26 +2054,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2106,23 +2089,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2299,28 +2265,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.69140625" customWidth="1"/>
-    <col min="3" max="3" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.07421875" style="1"/>
-    <col min="8" max="8" width="9.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.07421875" style="2"/>
-    <col min="11" max="11" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.3046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="2"/>
+    <col min="11" max="11" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2376,7 +2342,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2426,7 +2392,7 @@
       </c>
       <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>40</v>
       </c>
@@ -2478,7 +2444,7 @@
       </c>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -2530,7 +2496,7 @@
       </c>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2582,7 +2548,7 @@
       </c>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2634,7 +2600,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -2684,7 +2650,7 @@
       </c>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
@@ -2736,7 +2702,7 @@
       </c>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -2788,7 +2754,7 @@
       </c>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -2840,7 +2806,7 @@
       </c>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +2858,7 @@
       </c>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
@@ -2944,7 +2910,7 @@
       </c>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -2996,7 +2962,7 @@
       </c>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
@@ -3048,7 +3014,7 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
@@ -3100,7 +3066,7 @@
       </c>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -3152,7 +3118,7 @@
       </c>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>70</v>
       </c>
@@ -3204,7 +3170,7 @@
       </c>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
@@ -3256,7 +3222,7 @@
       </c>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>76</v>
       </c>
@@ -3308,7 +3274,7 @@
       </c>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>92</v>
       </c>
@@ -3360,7 +3326,7 @@
       </c>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>75</v>
       </c>
@@ -3412,7 +3378,7 @@
       </c>
       <c r="R21" s="7"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>74</v>
       </c>
@@ -3464,7 +3430,7 @@
       </c>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>106</v>
       </c>
@@ -3516,7 +3482,7 @@
       </c>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -3568,7 +3534,7 @@
       </c>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
         <v>130</v>
       </c>
@@ -3620,7 +3586,7 @@
       </c>
       <c r="R25" s="7"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -3672,7 +3638,7 @@
       </c>
       <c r="R26" s="7"/>
     </row>
-    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>100</v>
       </c>
@@ -3724,7 +3690,7 @@
       </c>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>141</v>
       </c>
@@ -3776,7 +3742,7 @@
       </c>
       <c r="R28" s="7"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
         <v>120</v>
       </c>
@@ -3828,7 +3794,7 @@
       </c>
       <c r="R29" s="7"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>113</v>
       </c>
@@ -3880,7 +3846,7 @@
       </c>
       <c r="R30" s="7"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>122</v>
       </c>
@@ -3932,7 +3898,7 @@
       </c>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A32" s="7" t="s">
         <v>194</v>
       </c>
@@ -3984,7 +3950,7 @@
       </c>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>128</v>
       </c>
@@ -4036,7 +4002,7 @@
       </c>
       <c r="R33" s="7"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>147</v>
       </c>
@@ -4088,7 +4054,7 @@
       </c>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>126</v>
       </c>
@@ -4140,7 +4106,7 @@
       </c>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>158</v>
       </c>
@@ -4192,7 +4158,7 @@
       </c>
       <c r="R36" s="7"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>168</v>
       </c>
@@ -4244,7 +4210,7 @@
       </c>
       <c r="R37" s="7"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -4296,7 +4262,7 @@
       </c>
       <c r="R38" s="7"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>144</v>
       </c>
@@ -4350,7 +4316,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>162</v>
       </c>
@@ -4404,7 +4370,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>134</v>
       </c>
@@ -4458,7 +4424,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
         <v>131</v>
       </c>
@@ -4512,7 +4478,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>171</v>
       </c>
@@ -4566,7 +4532,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>163</v>
       </c>
@@ -4620,7 +4586,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>155</v>
       </c>
@@ -4674,7 +4640,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>255</v>
       </c>
@@ -4728,7 +4694,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
         <v>178</v>
       </c>
@@ -4782,7 +4748,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>262</v>
       </c>
@@ -4836,7 +4802,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
         <v>363</v>
       </c>
@@ -4890,7 +4856,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
         <v>298</v>
       </c>
@@ -4942,7 +4908,7 @@
       </c>
       <c r="R50" s="7"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
         <v>169</v>
       </c>
@@ -4996,7 +4962,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>265</v>
       </c>
@@ -5050,7 +5016,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>139</v>
       </c>
@@ -5096,7 +5062,7 @@
       <c r="Q53" s="26"/>
       <c r="R53" s="7"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
         <v>135</v>
       </c>
@@ -5142,7 +5108,7 @@
       <c r="Q54" s="26"/>
       <c r="R54" s="7"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
         <v>345</v>
       </c>
@@ -5188,7 +5154,7 @@
       <c r="Q55" s="26"/>
       <c r="R55" s="7"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>273</v>
       </c>
@@ -5234,7 +5200,7 @@
       <c r="Q56" s="26"/>
       <c r="R56" s="7"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
         <v>249</v>
       </c>
@@ -5284,7 +5250,7 @@
       </c>
       <c r="R57" s="7"/>
     </row>
-    <row r="58" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>271</v>
       </c>
@@ -5330,7 +5296,7 @@
       <c r="Q58" s="26"/>
       <c r="R58" s="7"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
         <v>349</v>
       </c>
@@ -5376,7 +5342,7 @@
       <c r="Q59" s="26"/>
       <c r="R59" s="7"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>417</v>
       </c>
@@ -5422,7 +5388,7 @@
       <c r="Q60" s="26"/>
       <c r="R60" s="7"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
         <v>427</v>
       </c>
@@ -5468,7 +5434,7 @@
       <c r="Q61" s="26"/>
       <c r="R61" s="7"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
         <v>357</v>
       </c>
@@ -5514,7 +5480,7 @@
       <c r="Q62" s="26"/>
       <c r="R62" s="7"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A63" s="7" t="s">
         <v>340</v>
       </c>
@@ -5560,7 +5526,7 @@
       <c r="Q63" s="26"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>421</v>
       </c>
@@ -5606,7 +5572,7 @@
       <c r="Q64" s="26"/>
       <c r="R64" s="7"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A65" s="7" t="s">
         <v>465</v>
       </c>
@@ -5652,7 +5618,7 @@
       <c r="Q65" s="26"/>
       <c r="R65" s="7"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>441</v>
       </c>
@@ -5698,7 +5664,7 @@
       <c r="Q66" s="26"/>
       <c r="R66" s="7"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A67" s="7" t="s">
         <v>367</v>
       </c>
@@ -5744,7 +5710,7 @@
       <c r="Q67" s="26"/>
       <c r="R67" s="7"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>376</v>
       </c>
@@ -5794,7 +5760,7 @@
       </c>
       <c r="R68" s="7"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>372</v>
       </c>
@@ -5840,7 +5806,7 @@
       <c r="Q69" s="26"/>
       <c r="R69" s="7"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>445</v>
       </c>
@@ -5886,7 +5852,7 @@
       <c r="Q70" s="26"/>
       <c r="R70" s="7"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>422</v>
       </c>
@@ -5936,7 +5902,7 @@
       </c>
       <c r="R71" s="7"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A72" s="7" t="s">
         <v>196</v>
       </c>
@@ -5982,7 +5948,7 @@
       <c r="Q72" s="26"/>
       <c r="R72" s="7"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A73" s="7" t="s">
         <v>294</v>
       </c>
@@ -6028,7 +5994,7 @@
       <c r="Q73" s="26"/>
       <c r="R73" s="7"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>391</v>
       </c>
@@ -6074,7 +6040,7 @@
       <c r="Q74" s="26"/>
       <c r="R74" s="7"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>429</v>
       </c>
@@ -6120,7 +6086,7 @@
       <c r="Q75" s="26"/>
       <c r="R75" s="7"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A76" s="7" t="s">
         <v>482</v>
       </c>
@@ -6166,7 +6132,7 @@
       <c r="Q76" s="26"/>
       <c r="R76" s="7"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>487</v>
       </c>
@@ -6212,7 +6178,7 @@
       <c r="Q77" s="26"/>
       <c r="R77" s="7"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>456</v>
       </c>
@@ -6258,7 +6224,7 @@
       <c r="Q78" s="26"/>
       <c r="R78" s="7"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>397</v>
       </c>
@@ -6304,7 +6270,7 @@
       <c r="Q79" s="26"/>
       <c r="R79" s="7"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>464</v>
       </c>
@@ -6350,7 +6316,7 @@
       <c r="Q80" s="26"/>
       <c r="R80" s="7"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="14" t="s">
         <v>394</v>
       </c>
@@ -6396,7 +6362,7 @@
       <c r="Q81" s="30"/>
       <c r="R81" s="7"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="14" t="s">
         <v>277</v>
       </c>
@@ -6446,7 +6412,7 @@
       </c>
       <c r="R82" s="7"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
         <v>473</v>
       </c>
@@ -6478,7 +6444,7 @@
         <v>14</v>
       </c>
       <c r="K83" s="35">
-        <v>43471</v>
+        <v>43468</v>
       </c>
       <c r="L83" s="38" t="s">
         <v>282</v>
@@ -6489,6 +6455,50 @@
       <c r="P83" s="31"/>
       <c r="Q83" s="30"/>
       <c r="R83" s="7"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A84" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84" s="15">
+        <v>2018</v>
+      </c>
+      <c r="F84" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J84" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K84" s="35">
+        <v>43469</v>
+      </c>
+      <c r="L84" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="M84" s="28"/>
+      <c r="N84" s="29"/>
+      <c r="O84" s="30"/>
+      <c r="P84" s="31"/>
+      <c r="Q84" s="30"/>
+      <c r="R84" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6507,17 +6517,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="30.69140625" customWidth="1"/>
-    <col min="4" max="4" width="24.07421875" customWidth="1"/>
-    <col min="6" max="7" width="8.84375" style="2"/>
-    <col min="8" max="8" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6549,7 +6559,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
@@ -6581,7 +6591,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>285</v>
       </c>
@@ -6611,7 +6621,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>286</v>
       </c>
@@ -6651,21 +6661,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="40.69140625" customWidth="1"/>
-    <col min="3" max="4" width="16.69140625" customWidth="1"/>
-    <col min="5" max="5" width="12.69140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6685,7 +6693,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>161</v>
       </c>
@@ -6702,11 +6710,11 @@
         <v>42502</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F13" ca="1" si="0">TODAY()-E2</f>
-        <v>671</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+        <f t="shared" ref="F2:F12" ca="1" si="0">TODAY()-E2</f>
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>264</v>
       </c>
@@ -6724,10 +6732,10 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>638</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>380</v>
       </c>
@@ -6745,10 +6753,10 @@
       </c>
       <c r="F4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>99</v>
       </c>
@@ -6766,10 +6774,10 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>268</v>
       </c>
@@ -6787,154 +6795,133 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
       <c r="E7" s="10">
-        <v>43109</v>
-      </c>
-      <c r="F7" s="12">
+        <v>43124</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="E8" s="10">
-        <v>43124</v>
+        <v>43125</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>462</v>
+        <v>355</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>463</v>
+        <v>356</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="E9" s="10">
-        <v>43125</v>
+        <v>43130</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
-        <v>355</v>
+        <v>477</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>356</v>
+        <v>478</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>148</v>
+        <v>479</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>148</v>
+        <v>480</v>
       </c>
       <c r="E10" s="10">
-        <v>43130</v>
+        <v>43145</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>479</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>480</v>
+        <v>29</v>
       </c>
       <c r="E11" s="10">
-        <v>43145</v>
+        <v>43147</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>486</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="E12" s="10">
-        <v>43147</v>
+        <v>43149</v>
       </c>
       <c r="F12" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="E13" s="10">
-        <v>43149</v>
-      </c>
-      <c r="F13" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -6952,19 +6939,19 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.69140625" customWidth="1"/>
-    <col min="3" max="3" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.07421875" style="1"/>
-    <col min="8" max="10" width="9.07421875" style="2"/>
-    <col min="11" max="11" width="11.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="10" width="9.109375" style="2"/>
+    <col min="11" max="11" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="14.55" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7002,7 +6989,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>173</v>
       </c>
@@ -7038,10 +7025,10 @@
       </c>
       <c r="L2" s="13">
         <f t="shared" ref="L2:L3" ca="1" si="0">TODAY()-K2</f>
-        <v>865</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>174</v>
       </c>
@@ -7077,7 +7064,7 @@
       </c>
       <c r="L3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full published + doi
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="604">
   <si>
     <t>title</t>
   </si>
@@ -1826,6 +1826,9 @@
   </si>
   <si>
     <t>Van Wilder, Lisa; Rammant, Elke; Clays, Els; Devleesschauwer, Brecht; Pauwels, Nele; De Smedt, Delphine</t>
+  </si>
+  <si>
+    <t>10.1016/j.envres.2018.12.042</t>
   </si>
 </sst>
 </file>
@@ -2206,8 +2209,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:R103" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:R103"/>
-  <sortState ref="A2:R101">
-    <sortCondition ref="K1:K101"/>
+  <sortState ref="A2:R103">
+    <sortCondition ref="K1:K103"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" name="title" dataDxfId="44"/>
@@ -7420,44 +7423,44 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>525</v>
+        <v>566</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>519</v>
+        <v>82</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>520</v>
+        <v>83</v>
       </c>
       <c r="E97" s="7">
         <v>2019</v>
       </c>
       <c r="F97" s="32">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="H97" s="32" t="s">
         <v>14</v>
       </c>
       <c r="I97" s="32">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J97" s="32">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="K97" s="39">
-        <v>43497</v>
+        <v>43466</v>
       </c>
       <c r="L97" s="32" t="s">
         <v>279</v>
       </c>
       <c r="M97" s="7"/>
       <c r="N97" s="19" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="O97" s="7"/>
       <c r="P97" s="25"/>
@@ -7465,63 +7468,63 @@
       <c r="R97" s="7"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A98" s="14" t="s">
-        <v>391</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="E98" s="15">
-        <v>2018</v>
-      </c>
-      <c r="F98" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G98" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H98" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J98" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="K98" s="34">
-        <v>43831</v>
-      </c>
-      <c r="L98" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="M98" s="28"/>
-      <c r="N98" s="29" t="s">
-        <v>441</v>
-      </c>
-      <c r="O98" s="30"/>
+      <c r="A98" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="E98" s="7">
+        <v>2019</v>
+      </c>
+      <c r="F98" s="32">
+        <v>169</v>
+      </c>
+      <c r="G98" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="32">
+        <v>72</v>
+      </c>
+      <c r="J98" s="32">
+        <v>78</v>
+      </c>
+      <c r="K98" s="39">
+        <v>43497</v>
+      </c>
+      <c r="L98" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="M98" s="7"/>
+      <c r="N98" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="O98" s="7"/>
       <c r="P98" s="25"/>
       <c r="Q98" s="26"/>
       <c r="R98" s="7"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
-        <v>566</v>
+        <v>391</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>513</v>
+        <v>392</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>82</v>
+        <v>412</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>83</v>
+        <v>413</v>
       </c>
       <c r="E99" s="15">
         <v>2018</v>
@@ -7542,14 +7545,14 @@
         <v>14</v>
       </c>
       <c r="K99" s="34">
-        <v>43832</v>
+        <v>43831</v>
       </c>
       <c r="L99" s="37" t="s">
         <v>279</v>
       </c>
       <c r="M99" s="28"/>
       <c r="N99" s="29" t="s">
-        <v>567</v>
+        <v>441</v>
       </c>
       <c r="O99" s="30"/>
       <c r="P99" s="25"/>
@@ -7682,7 +7685,9 @@
         <v>279</v>
       </c>
       <c r="M102" s="28"/>
-      <c r="N102" s="29"/>
+      <c r="N102" s="29" t="s">
+        <v>603</v>
+      </c>
       <c r="O102" s="30"/>
       <c r="P102" s="25"/>
       <c r="Q102" s="26"/>
@@ -7897,10 +7902,14 @@
       <c r="E5" s="19">
         <v>2018</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="19">
+        <v>83</v>
+      </c>
+      <c r="G5" s="19">
+        <v>106</v>
+      </c>
       <c r="H5" s="10">
-        <v>43466</v>
+        <v>43455</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="20" t="s">
@@ -7923,10 +7932,14 @@
       <c r="E6" s="19">
         <v>2018</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="F6" s="19">
+        <v>107</v>
+      </c>
+      <c r="G6" s="19">
+        <v>122</v>
+      </c>
       <c r="H6" s="10">
-        <v>43466</v>
+        <v>43455</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="20" t="s">
@@ -7949,10 +7962,14 @@
       <c r="E7" s="19">
         <v>2018</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="F7" s="19">
+        <v>143</v>
+      </c>
+      <c r="G7" s="19">
+        <v>174</v>
+      </c>
       <c r="H7" s="10">
-        <v>43466</v>
+        <v>43455</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="20" t="s">

</xml_diff>

<commit_message>
new accepted & submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="640">
   <si>
     <t>title</t>
   </si>
@@ -1938,6 +1938,12 @@
   </si>
   <si>
     <t>Effects of 'The Vicious Worm' educational tool on Taenia solium knowledge retention in Zambian primary school students after one year</t>
+  </si>
+  <si>
+    <t>Epidemiology of Taenia saginata taeniosis/cysticercosis: a systematic review of the distribution in Western and Central Africa</t>
+  </si>
+  <si>
+    <t>Hendrickx, Emilie; Thomas, Lian F; Dorny, Pierre; Bobić, Branko; Braae, Uffe Christian; Devleesschauwer, Brecht; Eichenberger, Ramon M; Gabriël, Sarah; Saratsis, Anastasios; Torgerson, Paul R; Robertson, Lucy J; Dermauw, Veronique</t>
   </si>
 </sst>
 </file>
@@ -2359,8 +2365,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U117" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:U117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U118" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+  <autoFilter ref="A1:U118"/>
   <sortState ref="A2:U116">
     <sortCondition ref="K1:K116"/>
   </sortState>
@@ -2740,10 +2746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U117"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8941,7 +8947,7 @@
         <v>14</v>
       </c>
       <c r="K111" s="34">
-        <v>43833</v>
+        <v>43832</v>
       </c>
       <c r="L111" s="42" t="s">
         <v>276</v>
@@ -8990,7 +8996,7 @@
         <v>14</v>
       </c>
       <c r="K112" s="34">
-        <v>43834</v>
+        <v>43833</v>
       </c>
       <c r="L112" s="42" t="s">
         <v>276</v>
@@ -9041,7 +9047,7 @@
         <v>14</v>
       </c>
       <c r="K113" s="34">
-        <v>43835</v>
+        <v>43834</v>
       </c>
       <c r="L113" s="42" t="s">
         <v>276</v>
@@ -9092,7 +9098,7 @@
         <v>14</v>
       </c>
       <c r="K114" s="34">
-        <v>43836</v>
+        <v>43835</v>
       </c>
       <c r="L114" s="42" t="s">
         <v>276</v>
@@ -9141,7 +9147,7 @@
         <v>14</v>
       </c>
       <c r="K115" s="34">
-        <v>43837</v>
+        <v>43836</v>
       </c>
       <c r="L115" s="42" t="s">
         <v>276</v>
@@ -9190,7 +9196,7 @@
         <v>14</v>
       </c>
       <c r="K116" s="34">
-        <v>43838</v>
+        <v>43837</v>
       </c>
       <c r="L116" s="42" t="s">
         <v>276</v>
@@ -9239,7 +9245,7 @@
         <v>14</v>
       </c>
       <c r="K117" s="34">
-        <v>43839</v>
+        <v>43838</v>
       </c>
       <c r="L117" s="42" t="s">
         <v>276</v>
@@ -9255,6 +9261,53 @@
         <v>617</v>
       </c>
       <c r="U117" s="7"/>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A118" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E118" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F118" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G118" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H118" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I118" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J118" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K118" s="34">
+        <v>43839</v>
+      </c>
+      <c r="L118" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="M118" s="28"/>
+      <c r="N118" s="29"/>
+      <c r="O118" s="30"/>
+      <c r="P118" s="25"/>
+      <c r="Q118" s="26"/>
+      <c r="R118" s="7"/>
+      <c r="S118" s="7"/>
+      <c r="T118" s="7"/>
+      <c r="U118" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U1048576">
@@ -9523,7 +9576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9570,8 +9625,8 @@
         <v>42535</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F13" ca="1" si="0">TODAY()-E2</f>
-        <v>1016</v>
+        <f ca="1">TODAY()-E2</f>
+        <v>1028</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -9591,8 +9646,8 @@
         <v>43130</v>
       </c>
       <c r="F3" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>421</v>
+        <f ca="1">TODAY()-E3</f>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9612,8 +9667,8 @@
         <v>43393</v>
       </c>
       <c r="F4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <f ca="1">TODAY()-E4</f>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -9633,8 +9688,8 @@
         <v>43418</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>133</v>
+        <f ca="1">TODAY()-E5</f>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -9654,8 +9709,8 @@
         <v>43442</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <f ca="1">TODAY()-E6</f>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -9675,8 +9730,8 @@
         <v>43455</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <f ca="1">TODAY()-E7</f>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -9696,8 +9751,8 @@
         <v>43473</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <f ca="1">TODAY()-E8</f>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -9717,8 +9772,8 @@
         <v>43479</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <f ca="1">TODAY()-E9</f>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -9738,8 +9793,8 @@
         <v>43479</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <f ca="1">TODAY()-E10</f>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -9759,8 +9814,8 @@
         <v>43488</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <f ca="1">TODAY()-E11</f>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -9780,29 +9835,29 @@
         <v>43504</v>
       </c>
       <c r="F12" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <f ca="1">TODAY()-E12</f>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="A13" t="s">
+        <v>638</v>
+      </c>
+      <c r="B13" t="s">
+        <v>639</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="10">
-        <v>43516</v>
+        <v>43563</v>
       </c>
       <c r="F13" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <f ca="1">TODAY()-E13</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9867,7 +9922,7 @@
       </c>
       <c r="F2" s="13">
         <f ca="1">TODAY()-E2</f>
-        <v>1243</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -9888,7 +9943,7 @@
       </c>
       <c r="F3" s="13">
         <f ca="1">TODAY()-E3</f>
-        <v>1243</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9907,7 +9962,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="10">
         <f ca="1">TODAY()-E4</f>
-        <v>43551</v>
+        <v>43563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully published, new accepted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="649">
   <si>
     <t>title</t>
   </si>
@@ -1968,6 +1968,9 @@
   </si>
   <si>
     <t>10.1111/tbed.13214</t>
+  </si>
+  <si>
+    <t>e2034</t>
   </si>
 </sst>
 </file>
@@ -2179,7 +2182,87 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2340,46 +2423,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2394,65 +2437,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U122" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:U122"/>
-  <sortState ref="A2:U121">
-    <sortCondition ref="K1:K121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U123" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+  <autoFilter ref="A1:U123"/>
+  <sortState ref="A2:U122">
+    <sortCondition ref="K1:K122"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="47"/>
-    <tableColumn id="2" name="authors" dataDxfId="46"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
-    <tableColumn id="6" name="year" dataDxfId="43"/>
-    <tableColumn id="4" name="volume" dataDxfId="42"/>
-    <tableColumn id="5" name="issue" dataDxfId="41"/>
-    <tableColumn id="7" name="eID" dataDxfId="40"/>
-    <tableColumn id="8" name="from" dataDxfId="39"/>
-    <tableColumn id="9" name="to" dataDxfId="38"/>
-    <tableColumn id="10" name="date" dataDxfId="37"/>
-    <tableColumn id="14" name="classification" dataDxfId="36"/>
-    <tableColumn id="12" name="IF" dataDxfId="35"/>
-    <tableColumn id="13" name="DOI" dataDxfId="34"/>
-    <tableColumn id="15" name="WoS" dataDxfId="33"/>
-    <tableColumn id="16" name="rank" dataDxfId="32"/>
-    <tableColumn id="17" name="quartile" dataDxfId="31"/>
-    <tableColumn id="18" name="category" dataDxfId="30"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
-    <tableColumn id="20" name="SC" dataDxfId="28"/>
-    <tableColumn id="21" name="UGent" dataDxfId="27"/>
+    <tableColumn id="1" name="title" dataDxfId="55"/>
+    <tableColumn id="2" name="authors" dataDxfId="54"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="53"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="52"/>
+    <tableColumn id="6" name="year" dataDxfId="51"/>
+    <tableColumn id="4" name="volume" dataDxfId="50"/>
+    <tableColumn id="5" name="issue" dataDxfId="49"/>
+    <tableColumn id="7" name="eID" dataDxfId="48"/>
+    <tableColumn id="8" name="from" dataDxfId="47"/>
+    <tableColumn id="9" name="to" dataDxfId="46"/>
+    <tableColumn id="10" name="date" dataDxfId="45"/>
+    <tableColumn id="14" name="classification" dataDxfId="44"/>
+    <tableColumn id="12" name="IF" dataDxfId="43"/>
+    <tableColumn id="13" name="DOI" dataDxfId="42"/>
+    <tableColumn id="15" name="WoS" dataDxfId="41"/>
+    <tableColumn id="16" name="rank" dataDxfId="40"/>
+    <tableColumn id="17" name="quartile" dataDxfId="39"/>
+    <tableColumn id="18" name="category" dataDxfId="38"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="37"/>
+    <tableColumn id="20" name="SC" dataDxfId="36"/>
+    <tableColumn id="21" name="UGent" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:J7"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="25"/>
-    <tableColumn id="2" name="authors" dataDxfId="24"/>
-    <tableColumn id="3" name="editors" dataDxfId="23"/>
-    <tableColumn id="11" name="book" dataDxfId="22"/>
-    <tableColumn id="6" name="year" dataDxfId="21"/>
-    <tableColumn id="8" name="from" dataDxfId="20"/>
-    <tableColumn id="9" name="to" dataDxfId="19"/>
-    <tableColumn id="10" name="date" dataDxfId="18"/>
-    <tableColumn id="12" name="IF" dataDxfId="17"/>
-    <tableColumn id="13" name="DOI" dataDxfId="16"/>
+    <tableColumn id="1" name="title" dataDxfId="33"/>
+    <tableColumn id="2" name="authors" dataDxfId="32"/>
+    <tableColumn id="3" name="editors" dataDxfId="31"/>
+    <tableColumn id="11" name="book" dataDxfId="30"/>
+    <tableColumn id="6" name="year" dataDxfId="29"/>
+    <tableColumn id="8" name="from" dataDxfId="28"/>
+    <tableColumn id="9" name="to" dataDxfId="27"/>
+    <tableColumn id="10" name="date" dataDxfId="26"/>
+    <tableColumn id="12" name="IF" dataDxfId="25"/>
+    <tableColumn id="13" name="DOI" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F8"/>
   <sortState ref="A2:F19">
     <sortCondition ref="E1:E19"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="title" dataDxfId="21"/>
+    <tableColumn id="2" name="authors" dataDxfId="20"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="19"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="18"/>
+    <tableColumn id="10" name="date" dataDxfId="17"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="16">
+      <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F5"/>
+  <sortState ref="A2:K14">
+    <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="title" dataDxfId="13"/>
@@ -2461,26 +2524,6 @@
     <tableColumn id="11" name="journal_short" dataDxfId="10"/>
     <tableColumn id="10" name="date" dataDxfId="9"/>
     <tableColumn id="12" name="COUNT" dataDxfId="8">
-      <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F5"/>
-  <sortState ref="A2:K14">
-    <sortCondition ref="E1:E14"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="5"/>
-    <tableColumn id="2" name="authors" dataDxfId="4"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
-    <tableColumn id="10" name="date" dataDxfId="1"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="0">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2775,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U122"/>
+  <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9059,68 +9102,68 @@
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A113" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>389</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="E113" s="15">
+      <c r="A113" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="E113" s="7">
         <v>2019</v>
       </c>
-      <c r="F113" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G113" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H113" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I113" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J113" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K113" s="34">
-        <v>43831</v>
-      </c>
-      <c r="L113" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="M113" s="28"/>
-      <c r="N113" s="29" t="s">
-        <v>437</v>
-      </c>
-      <c r="O113" s="30"/>
+      <c r="F113" s="35">
+        <v>29</v>
+      </c>
+      <c r="G113" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="H113" s="35" t="s">
+        <v>648</v>
+      </c>
+      <c r="I113" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J113" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K113" s="36">
+        <v>43586</v>
+      </c>
+      <c r="L113" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="M113" s="7"/>
+      <c r="N113" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="O113" s="7"/>
       <c r="P113" s="25"/>
       <c r="Q113" s="26"/>
       <c r="R113" s="7"/>
       <c r="S113" s="7"/>
-      <c r="T113" s="7"/>
-      <c r="U113" s="7" t="s">
-        <v>616</v>
-      </c>
+      <c r="T113" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="U113" s="7"/>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
-        <v>516</v>
+        <v>388</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>517</v>
+        <v>389</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>514</v>
+        <v>409</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>515</v>
+        <v>410</v>
       </c>
       <c r="E114" s="15">
         <v>2019</v>
@@ -9141,14 +9184,14 @@
         <v>14</v>
       </c>
       <c r="K114" s="34">
-        <v>43832</v>
+        <v>43831</v>
       </c>
       <c r="L114" s="42" t="s">
         <v>276</v>
       </c>
       <c r="M114" s="28"/>
       <c r="N114" s="29" t="s">
-        <v>593</v>
+        <v>437</v>
       </c>
       <c r="O114" s="30"/>
       <c r="P114" s="25"/>
@@ -9156,20 +9199,22 @@
       <c r="R114" s="7"/>
       <c r="S114" s="7"/>
       <c r="T114" s="7"/>
-      <c r="U114" s="7"/>
+      <c r="U114" s="7" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
-        <v>470</v>
+        <v>516</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>471</v>
+        <v>517</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>472</v>
+        <v>514</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>473</v>
+        <v>515</v>
       </c>
       <c r="E115" s="15">
         <v>2019</v>
@@ -9190,23 +9235,21 @@
         <v>14</v>
       </c>
       <c r="K115" s="34">
-        <v>43833</v>
+        <v>43832</v>
       </c>
       <c r="L115" s="42" t="s">
         <v>276</v>
       </c>
       <c r="M115" s="28"/>
       <c r="N115" s="29" t="s">
-        <v>618</v>
+        <v>593</v>
       </c>
       <c r="O115" s="30"/>
       <c r="P115" s="25"/>
       <c r="Q115" s="26"/>
       <c r="R115" s="7"/>
       <c r="S115" s="7"/>
-      <c r="T115" s="7" t="s">
-        <v>615</v>
-      </c>
+      <c r="T115" s="7"/>
       <c r="U115" s="7"/>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
@@ -9241,7 +9284,7 @@
         <v>14</v>
       </c>
       <c r="K116" s="34">
-        <v>43834</v>
+        <v>43833</v>
       </c>
       <c r="L116" s="42" t="s">
         <v>276</v>
@@ -9290,7 +9333,7 @@
         <v>14</v>
       </c>
       <c r="K117" s="34">
-        <v>43835</v>
+        <v>43834</v>
       </c>
       <c r="L117" s="42" t="s">
         <v>276</v>
@@ -9341,7 +9384,7 @@
         <v>14</v>
       </c>
       <c r="K118" s="34">
-        <v>43836</v>
+        <v>43835</v>
       </c>
       <c r="L118" s="42" t="s">
         <v>276</v>
@@ -9390,7 +9433,7 @@
         <v>14</v>
       </c>
       <c r="K119" s="34">
-        <v>43837</v>
+        <v>43836</v>
       </c>
       <c r="L119" s="42" t="s">
         <v>276</v>
@@ -9439,7 +9482,7 @@
         <v>14</v>
       </c>
       <c r="K120" s="34">
-        <v>43838</v>
+        <v>43837</v>
       </c>
       <c r="L120" s="42" t="s">
         <v>276</v>
@@ -9488,7 +9531,7 @@
         <v>14</v>
       </c>
       <c r="K121" s="34">
-        <v>43839</v>
+        <v>43838</v>
       </c>
       <c r="L121" s="42" t="s">
         <v>276</v>
@@ -9535,7 +9578,7 @@
         <v>14</v>
       </c>
       <c r="K122" s="34">
-        <v>43840</v>
+        <v>43839</v>
       </c>
       <c r="L122" s="42" t="s">
         <v>276</v>
@@ -9550,20 +9593,83 @@
       <c r="T122" s="7"/>
       <c r="U122" s="7"/>
     </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A123" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="D123" s="14" t="s">
+        <v>603</v>
+      </c>
+      <c r="E123" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F123" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G123" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H123" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I123" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J123" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K123" s="34">
+        <v>43840</v>
+      </c>
+      <c r="L123" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="M123" s="28"/>
+      <c r="N123" s="29"/>
+      <c r="O123" s="30"/>
+      <c r="P123" s="25"/>
+      <c r="Q123" s="26"/>
+      <c r="R123" s="7"/>
+      <c r="S123" s="7"/>
+      <c r="T123" s="7"/>
+      <c r="U123" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="S1:U112 S114:U1048576">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+  <conditionalFormatting sqref="S1:U112 S114:U122 S124:U1048576">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S113:U113">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+  <conditionalFormatting sqref="T113:U113">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S113">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S123:U123">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9815,7 +9921,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -9864,8 +9970,8 @@
         <v>43130</v>
       </c>
       <c r="F2" s="13">
-        <f t="shared" ref="F2:F9" ca="1" si="0">TODAY()-E2</f>
-        <v>459</v>
+        <f t="shared" ref="F2:F8" ca="1" si="0">TODAY()-E2</f>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -9886,7 +9992,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9907,7 +10013,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -9928,91 +10034,70 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>602</v>
+        <v>90</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>603</v>
+        <v>90</v>
       </c>
       <c r="E6" s="10">
-        <v>43479</v>
+        <v>43488</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>608</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>90</v>
+      <c r="A7" t="s">
+        <v>636</v>
+      </c>
+      <c r="B7" t="s">
+        <v>637</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
       </c>
       <c r="E7" s="10">
-        <v>43488</v>
+        <v>43563</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>101</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>636</v>
-      </c>
-      <c r="B8" t="s">
-        <v>637</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
+      <c r="A8" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>646</v>
       </c>
       <c r="E8" s="10">
-        <v>43563</v>
+        <v>43585</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>644</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>645</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="E9" s="10">
-        <v>43585</v>
-      </c>
-      <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -10077,7 +10162,7 @@
       </c>
       <c r="F2" s="45">
         <f t="shared" ref="F2:F5" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>3.5095890410958903</v>
+        <v>3.5205479452054793</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -10098,7 +10183,7 @@
       </c>
       <c r="F3" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5095890410958903</v>
+        <v>3.5205479452054793</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -10117,7 +10202,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>119.42191780821918</v>
+        <v>119.43287671232876</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -10138,7 +10223,7 @@
       </c>
       <c r="F5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8876712328767122</v>
+        <v>2.8986301369863012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new accepted & fully published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="231" windowWidth="14808" windowHeight="7893"/>
+    <workbookView xWindow="245" yWindow="231" windowWidth="14808" windowHeight="7893" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="673">
   <si>
     <t>title</t>
   </si>
@@ -2040,6 +2040,9 @@
   </si>
   <si>
     <t>Birnie, Emma; Virk, Harjeet Singh; Savelkoel, Jelmer; Spijker, Rene; Bertherat, Eric; Dance, David A B; Limmathurotsakul, Direk; Devleesschauwer, Brecht; Haagsma, Juanita A; Wiersinga, W Joost</t>
+  </si>
+  <si>
+    <t>10.1186/s13012-019-0930-2</t>
   </si>
 </sst>
 </file>
@@ -2256,6 +2259,106 @@
   </cellStyles>
   <dxfs count="60">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2415,106 +2518,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2529,73 +2532,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U126" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:U126"/>
-  <sortState ref="A2:U126">
-    <sortCondition ref="K1:K126"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U127" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="A1:U127"/>
+  <sortState ref="A2:U127">
+    <sortCondition ref="K1:K127"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="47"/>
-    <tableColumn id="2" name="authors" dataDxfId="46"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
-    <tableColumn id="6" name="year" dataDxfId="43"/>
-    <tableColumn id="4" name="volume" dataDxfId="42"/>
-    <tableColumn id="5" name="issue" dataDxfId="41"/>
-    <tableColumn id="7" name="eID" dataDxfId="40"/>
-    <tableColumn id="8" name="from" dataDxfId="39"/>
-    <tableColumn id="9" name="to" dataDxfId="38"/>
-    <tableColumn id="10" name="date" dataDxfId="37"/>
-    <tableColumn id="14" name="classification" dataDxfId="36"/>
-    <tableColumn id="12" name="IF" dataDxfId="35"/>
-    <tableColumn id="13" name="DOI" dataDxfId="34"/>
-    <tableColumn id="15" name="WoS" dataDxfId="33"/>
-    <tableColumn id="16" name="rank" dataDxfId="32"/>
-    <tableColumn id="17" name="quartile" dataDxfId="31"/>
-    <tableColumn id="18" name="category" dataDxfId="30"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
-    <tableColumn id="20" name="SC" dataDxfId="28"/>
-    <tableColumn id="21" name="UGent" dataDxfId="27"/>
+    <tableColumn id="1" name="title" dataDxfId="57"/>
+    <tableColumn id="2" name="authors" dataDxfId="56"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="55"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="54"/>
+    <tableColumn id="6" name="year" dataDxfId="53"/>
+    <tableColumn id="4" name="volume" dataDxfId="52"/>
+    <tableColumn id="5" name="issue" dataDxfId="51"/>
+    <tableColumn id="7" name="eID" dataDxfId="50"/>
+    <tableColumn id="8" name="from" dataDxfId="49"/>
+    <tableColumn id="9" name="to" dataDxfId="48"/>
+    <tableColumn id="10" name="date" dataDxfId="47"/>
+    <tableColumn id="14" name="classification" dataDxfId="46"/>
+    <tableColumn id="12" name="IF" dataDxfId="45"/>
+    <tableColumn id="13" name="DOI" dataDxfId="44"/>
+    <tableColumn id="15" name="WoS" dataDxfId="43"/>
+    <tableColumn id="16" name="rank" dataDxfId="42"/>
+    <tableColumn id="17" name="quartile" dataDxfId="41"/>
+    <tableColumn id="18" name="category" dataDxfId="40"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="39"/>
+    <tableColumn id="20" name="SC" dataDxfId="38"/>
+    <tableColumn id="21" name="UGent" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:J7"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="25"/>
-    <tableColumn id="2" name="authors" dataDxfId="24"/>
-    <tableColumn id="3" name="editors" dataDxfId="23"/>
-    <tableColumn id="11" name="book" dataDxfId="22"/>
-    <tableColumn id="6" name="year" dataDxfId="21"/>
-    <tableColumn id="8" name="from" dataDxfId="20"/>
-    <tableColumn id="9" name="to" dataDxfId="19"/>
-    <tableColumn id="10" name="date" dataDxfId="18"/>
-    <tableColumn id="12" name="IF" dataDxfId="17"/>
-    <tableColumn id="13" name="DOI" dataDxfId="16"/>
+    <tableColumn id="1" name="title" dataDxfId="35"/>
+    <tableColumn id="2" name="authors" dataDxfId="34"/>
+    <tableColumn id="3" name="editors" dataDxfId="33"/>
+    <tableColumn id="11" name="book" dataDxfId="32"/>
+    <tableColumn id="6" name="year" dataDxfId="31"/>
+    <tableColumn id="8" name="from" dataDxfId="30"/>
+    <tableColumn id="9" name="to" dataDxfId="29"/>
+    <tableColumn id="10" name="date" dataDxfId="28"/>
+    <tableColumn id="12" name="IF" dataDxfId="27"/>
+    <tableColumn id="13" name="DOI" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:F8"/>
   <sortState ref="A2:F19">
     <sortCondition ref="E1:E19"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="13"/>
-    <tableColumn id="2" name="authors" dataDxfId="12"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
-    <tableColumn id="10" name="date" dataDxfId="9"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="8">
+    <tableColumn id="1" name="title" dataDxfId="23"/>
+    <tableColumn id="2" name="authors" dataDxfId="22"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="21"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="20"/>
+    <tableColumn id="10" name="date" dataDxfId="19"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="18">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2604,18 +2607,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="5"/>
-    <tableColumn id="2" name="authors" dataDxfId="4"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
-    <tableColumn id="10" name="date" dataDxfId="1"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="0">
+    <tableColumn id="1" name="title" dataDxfId="15"/>
+    <tableColumn id="2" name="authors" dataDxfId="14"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="13"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="12"/>
+    <tableColumn id="10" name="date" dataDxfId="11"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="10">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2910,10 +2913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U126"/>
+  <dimension ref="A1:U127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView topLeftCell="A95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9813,47 +9816,47 @@
       <c r="U123" s="7"/>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124" s="14" t="s">
-        <v>570</v>
-      </c>
-      <c r="B124" s="14" t="s">
-        <v>526</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>571</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>572</v>
-      </c>
-      <c r="E124" s="15">
+      <c r="A124" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E124" s="19">
         <v>2019</v>
       </c>
-      <c r="F124" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G124" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H124" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I124" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J124" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K124" s="34">
-        <v>43832</v>
-      </c>
-      <c r="L124" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="M124" s="28"/>
-      <c r="N124" s="29" t="s">
-        <v>646</v>
-      </c>
-      <c r="O124" s="30"/>
+      <c r="F124" s="19">
+        <v>19</v>
+      </c>
+      <c r="G124" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H124" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I124" s="19">
+        <v>892</v>
+      </c>
+      <c r="J124" s="19">
+        <v>902</v>
+      </c>
+      <c r="K124" s="10">
+        <v>43678</v>
+      </c>
+      <c r="L124" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="M124" s="11"/>
+      <c r="N124" s="20" t="s">
+        <v>662</v>
+      </c>
+      <c r="O124" s="7"/>
       <c r="P124" s="25"/>
       <c r="Q124" s="26"/>
       <c r="R124" s="7"/>
@@ -9864,47 +9867,47 @@
       <c r="U124" s="7"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125" s="14" t="s">
-        <v>599</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>601</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="E125" s="15">
+      <c r="A125" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="E125" s="19">
         <v>2019</v>
       </c>
-      <c r="F125" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H125" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I125" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J125" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="K125" s="34">
-        <v>43833</v>
-      </c>
-      <c r="L125" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="M125" s="28"/>
-      <c r="N125" s="29" t="s">
-        <v>658</v>
-      </c>
-      <c r="O125" s="30"/>
+      <c r="F125" s="19">
+        <v>14</v>
+      </c>
+      <c r="G125" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H125" s="19">
+        <v>79</v>
+      </c>
+      <c r="I125" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J125" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="K125" s="10">
+        <v>43690</v>
+      </c>
+      <c r="L125" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="M125" s="11"/>
+      <c r="N125" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="O125" s="7"/>
       <c r="P125" s="25"/>
       <c r="Q125" s="26"/>
       <c r="R125" s="7"/>
@@ -9914,16 +9917,16 @@
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
-        <v>529</v>
+        <v>570</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>671</v>
+        <v>526</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>81</v>
+        <v>571</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>82</v>
+        <v>572</v>
       </c>
       <c r="E126" s="15">
         <v>2019</v>
@@ -9944,14 +9947,14 @@
         <v>14</v>
       </c>
       <c r="K126" s="34">
-        <v>43834</v>
+        <v>43832</v>
       </c>
       <c r="L126" s="42" t="s">
         <v>276</v>
       </c>
       <c r="M126" s="28"/>
       <c r="N126" s="29" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="O126" s="30"/>
       <c r="P126" s="25"/>
@@ -9963,44 +9966,93 @@
       </c>
       <c r="U126" s="7"/>
     </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="E127" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F127" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G127" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H127" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I127" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J127" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K127" s="34">
+        <v>43833</v>
+      </c>
+      <c r="L127" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="M127" s="28"/>
+      <c r="N127" s="29" t="s">
+        <v>658</v>
+      </c>
+      <c r="O127" s="30"/>
+      <c r="P127" s="25"/>
+      <c r="Q127" s="26"/>
+      <c r="R127" s="7"/>
+      <c r="S127" s="7"/>
+      <c r="T127" s="7"/>
+      <c r="U127" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U1048576 U126">
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10252,9 +10304,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10301,155 +10353,134 @@
         <v>43130</v>
       </c>
       <c r="F2" s="13">
-        <f t="shared" ref="F2:F9" ca="1" si="0">TODAY()-E2</f>
-        <v>540</v>
+        <f t="shared" ref="F2:F8" ca="1" si="0">TODAY()-E2</f>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>551</v>
+        <v>589</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>552</v>
+        <v>587</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>556</v>
+        <v>588</v>
       </c>
       <c r="E3" s="10">
-        <v>43393</v>
+        <v>43455</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>277</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>586</v>
+        <v>607</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>589</v>
+        <v>608</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>587</v>
+        <v>90</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>588</v>
+        <v>90</v>
       </c>
       <c r="E4" s="10">
-        <v>43455</v>
+        <v>43488</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>607</v>
+        <v>643</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>608</v>
+        <v>644</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>90</v>
+        <v>645</v>
       </c>
       <c r="E5" s="10">
-        <v>43488</v>
+        <v>43585</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>643</v>
+        <v>665</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>644</v>
+        <v>666</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>645</v>
+        <v>82</v>
       </c>
       <c r="E6" s="10">
-        <v>43585</v>
+        <v>43599</v>
       </c>
       <c r="F6" s="12">
+        <f ca="1">TODAY()-E6</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E7" s="10">
+        <v>43642</v>
+      </c>
+      <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="10">
-        <v>43599</v>
-      </c>
-      <c r="F7" s="12">
-        <f ca="1">TODAY()-E7</f>
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>530</v>
+        <v>663</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>660</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>531</v>
+        <v>13</v>
       </c>
       <c r="E8" s="10">
-        <v>43642</v>
+        <v>43645</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="10">
-        <v>43645</v>
-      </c>
-      <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -10514,7 +10545,7 @@
       </c>
       <c r="F2" s="45">
         <f t="shared" ref="F2:F5" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>3.7315068493150685</v>
+        <v>3.7890410958904108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10535,7 +10566,7 @@
       </c>
       <c r="F3" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7315068493150685</v>
+        <v>3.7890410958904108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -10554,7 +10585,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>119.64383561643835</v>
+        <v>119.7013698630137</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10575,7 +10606,7 @@
       </c>
       <c r="F5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1095890410958904</v>
+        <v>3.1671232876712327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update training & publications
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="231" windowWidth="14808" windowHeight="7893" activeTab="2"/>
+    <workbookView xWindow="245" yWindow="231" windowWidth="14808" windowHeight="7893"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="673">
   <si>
     <t>title</t>
   </si>
@@ -1787,12 +1787,6 @@
     <t>A comprehensive catalogue of EQ-5D scores in chronic disease: results of a systematic review</t>
   </si>
   <si>
-    <t>Value in Health</t>
-  </si>
-  <si>
-    <t>Value Health</t>
-  </si>
-  <si>
     <t>Van Wilder, Lisa; Rammant, Elke; Clays, Els; Devleesschauwer, Brecht; Pauwels, Nele; De Smedt, Delphine</t>
   </si>
   <si>
@@ -2043,6 +2037,12 @@
   </si>
   <si>
     <t>10.1186/s13012-019-0930-2</t>
+  </si>
+  <si>
+    <t>Quality of Life Research</t>
+  </si>
+  <si>
+    <t>Qual. Life Res.</t>
   </si>
 </sst>
 </file>
@@ -2532,8 +2532,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U127" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <autoFilter ref="A1:U127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U128" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="A1:U128"/>
   <sortState ref="A2:U127">
     <sortCondition ref="K1:K127"/>
   </sortState>
@@ -2587,8 +2587,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A1:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:F7"/>
   <sortState ref="A2:F19">
     <sortCondition ref="E1:E19"/>
   </sortState>
@@ -2913,10 +2913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U127"/>
+  <dimension ref="A1:U128"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2992,13 +2992,13 @@
         <v>395</v>
       </c>
       <c r="S1" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="U1" s="17" t="s">
         <v>610</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>611</v>
-      </c>
-      <c r="U1" s="17" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -3053,7 +3053,7 @@
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -3167,7 +3167,7 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -3281,7 +3281,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -3336,7 +3336,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -3564,7 +3564,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -3621,7 +3621,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3735,7 +3735,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -3792,7 +3792,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -3906,7 +3906,7 @@
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -3963,7 +3963,7 @@
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -4020,7 +4020,7 @@
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -4077,12 +4077,12 @@
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>79</v>
@@ -4134,7 +4134,7 @@
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
       <c r="U22" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -4248,7 +4248,7 @@
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -4305,7 +4305,7 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -4362,7 +4362,7 @@
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
       <c r="U25" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -4419,7 +4419,7 @@
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="27" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
       <c r="U27" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -4533,12 +4533,12 @@
       <c r="S28" s="7"/>
       <c r="T28" s="7"/>
       <c r="U28" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>118</v>
@@ -4590,7 +4590,7 @@
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
       <c r="U30" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -4761,7 +4761,7 @@
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -4818,7 +4818,7 @@
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -4875,7 +4875,7 @@
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
       <c r="U34" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -4989,7 +4989,7 @@
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -5103,7 +5103,7 @@
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
       <c r="U38" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -5161,10 +5161,10 @@
       </c>
       <c r="S39" s="7"/>
       <c r="T39" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -5222,10 +5222,10 @@
       </c>
       <c r="S40" s="7"/>
       <c r="T40" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -5283,10 +5283,10 @@
       </c>
       <c r="S41" s="7"/>
       <c r="T41" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -5344,10 +5344,10 @@
       </c>
       <c r="S42" s="7"/>
       <c r="T42" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -5405,10 +5405,10 @@
       </c>
       <c r="S43" s="7"/>
       <c r="T43" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -5466,10 +5466,10 @@
       </c>
       <c r="S44" s="7"/>
       <c r="T44" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -5527,10 +5527,10 @@
       </c>
       <c r="S45" s="7"/>
       <c r="T45" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U45" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -5588,10 +5588,10 @@
       </c>
       <c r="S46" s="7"/>
       <c r="T46" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U46" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -5649,10 +5649,10 @@
       </c>
       <c r="S47" s="7"/>
       <c r="T47" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U47" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -5710,10 +5710,10 @@
       </c>
       <c r="S48" s="7"/>
       <c r="T48" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U48" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -5771,10 +5771,10 @@
       </c>
       <c r="S49" s="7"/>
       <c r="T49" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U49" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -5830,10 +5830,10 @@
       <c r="R50" s="7"/>
       <c r="S50" s="7"/>
       <c r="T50" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -5891,10 +5891,10 @@
       </c>
       <c r="S51" s="7"/>
       <c r="T51" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U51" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -5952,10 +5952,10 @@
       </c>
       <c r="S52" s="7"/>
       <c r="T52" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U52" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
@@ -6007,10 +6007,10 @@
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
       <c r="T53" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
@@ -6062,10 +6062,10 @@
       <c r="R54" s="7"/>
       <c r="S54" s="7"/>
       <c r="T54" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U54" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -6117,10 +6117,10 @@
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
       <c r="T55" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -6172,10 +6172,10 @@
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
       <c r="T56" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U56" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -6231,10 +6231,10 @@
       <c r="R57" s="7"/>
       <c r="S57" s="7"/>
       <c r="T57" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U57" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="58" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -6286,10 +6286,10 @@
       <c r="R58" s="7"/>
       <c r="S58" s="7"/>
       <c r="T58" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U58" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -6341,10 +6341,10 @@
       <c r="R59" s="7"/>
       <c r="S59" s="7"/>
       <c r="T59" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U59" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -6396,10 +6396,10 @@
       <c r="R60" s="7"/>
       <c r="S60" s="7"/>
       <c r="T60" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U60" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
@@ -6451,10 +6451,10 @@
       <c r="R61" s="7"/>
       <c r="S61" s="7"/>
       <c r="T61" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U61" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
@@ -6506,10 +6506,10 @@
       <c r="R62" s="7"/>
       <c r="S62" s="7"/>
       <c r="T62" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U62" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
@@ -6561,10 +6561,10 @@
       <c r="R63" s="7"/>
       <c r="S63" s="7"/>
       <c r="T63" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U63" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -6616,10 +6616,10 @@
       <c r="R64" s="7"/>
       <c r="S64" s="7"/>
       <c r="T64" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U64" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
@@ -6671,10 +6671,10 @@
       <c r="R65" s="7"/>
       <c r="S65" s="7"/>
       <c r="T65" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U65" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
@@ -6726,10 +6726,10 @@
       <c r="R66" s="7"/>
       <c r="S66" s="7"/>
       <c r="T66" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U66" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -6781,10 +6781,10 @@
       <c r="R67" s="7"/>
       <c r="S67" s="7"/>
       <c r="T67" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U67" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
@@ -6840,10 +6840,10 @@
       <c r="R68" s="7"/>
       <c r="S68" s="7"/>
       <c r="T68" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U68" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -6895,10 +6895,10 @@
       <c r="R69" s="7"/>
       <c r="S69" s="7"/>
       <c r="T69" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U69" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
@@ -6950,10 +6950,10 @@
       <c r="R70" s="7"/>
       <c r="S70" s="7"/>
       <c r="T70" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U70" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
@@ -7009,10 +7009,10 @@
       <c r="R71" s="7"/>
       <c r="S71" s="7"/>
       <c r="T71" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U71" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
@@ -7064,10 +7064,10 @@
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
       <c r="T72" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U72" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
@@ -7119,10 +7119,10 @@
       <c r="R73" s="7"/>
       <c r="S73" s="7"/>
       <c r="T73" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
@@ -7174,10 +7174,10 @@
       <c r="R74" s="7"/>
       <c r="S74" s="7"/>
       <c r="T74" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U74" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
@@ -7229,10 +7229,10 @@
       <c r="R75" s="7"/>
       <c r="S75" s="7"/>
       <c r="T75" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U75" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
@@ -7284,15 +7284,15 @@
       <c r="R76" s="7"/>
       <c r="S76" s="7"/>
       <c r="T76" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U76" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>480</v>
@@ -7339,10 +7339,10 @@
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
       <c r="T77" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U77" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
@@ -7394,10 +7394,10 @@
       <c r="R78" s="7"/>
       <c r="S78" s="7"/>
       <c r="T78" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U78" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -7449,10 +7449,10 @@
       <c r="R79" s="7"/>
       <c r="S79" s="7"/>
       <c r="T79" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
@@ -7504,10 +7504,10 @@
       <c r="R80" s="7"/>
       <c r="S80" s="7"/>
       <c r="T80" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U80" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
@@ -7559,10 +7559,10 @@
       <c r="R81" s="7"/>
       <c r="S81" s="7"/>
       <c r="T81" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U81" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
@@ -7614,10 +7614,10 @@
       <c r="R82" s="7"/>
       <c r="S82" s="7"/>
       <c r="T82" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
@@ -7669,10 +7669,10 @@
       <c r="R83" s="7"/>
       <c r="S83" s="7"/>
       <c r="T83" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
@@ -7724,10 +7724,10 @@
       <c r="R84" s="7"/>
       <c r="S84" s="7"/>
       <c r="T84" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U84" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
@@ -7783,10 +7783,10 @@
       <c r="R85" s="7"/>
       <c r="S85" s="7"/>
       <c r="T85" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U85" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
@@ -7838,10 +7838,10 @@
       <c r="R86" s="7"/>
       <c r="S86" s="7"/>
       <c r="T86" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U86" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -7893,10 +7893,10 @@
       <c r="R87" s="7"/>
       <c r="S87" s="7"/>
       <c r="T87" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U87" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
@@ -7948,10 +7948,10 @@
       <c r="R88" s="7"/>
       <c r="S88" s="7"/>
       <c r="T88" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U88" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -8003,10 +8003,10 @@
       <c r="R89" s="7"/>
       <c r="S89" s="7"/>
       <c r="T89" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U89" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
@@ -8058,10 +8058,10 @@
       <c r="R90" s="7"/>
       <c r="S90" s="7"/>
       <c r="T90" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U90" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
@@ -8113,10 +8113,10 @@
       <c r="R91" s="7"/>
       <c r="S91" s="7"/>
       <c r="T91" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U91" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
@@ -8168,10 +8168,10 @@
       <c r="R92" s="7"/>
       <c r="S92" s="7"/>
       <c r="T92" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U92" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -8223,10 +8223,10 @@
       <c r="R93" s="7"/>
       <c r="S93" s="7"/>
       <c r="T93" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U93" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -8278,10 +8278,10 @@
       <c r="R94" s="7"/>
       <c r="S94" s="7"/>
       <c r="T94" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U94" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
@@ -8333,10 +8333,10 @@
       <c r="R95" s="7"/>
       <c r="S95" s="7"/>
       <c r="T95" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U95" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
@@ -8388,10 +8388,10 @@
       <c r="R96" s="7"/>
       <c r="S96" s="7"/>
       <c r="T96" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U96" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
@@ -8441,18 +8441,18 @@
       <c r="R97" s="7"/>
       <c r="S97" s="7"/>
       <c r="T97" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U97" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>512</v>
@@ -8470,7 +8470,7 @@
         <v>14</v>
       </c>
       <c r="H98" s="32" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I98" s="32" t="s">
         <v>14</v>
@@ -8486,7 +8486,7 @@
       </c>
       <c r="M98" s="7"/>
       <c r="N98" s="19" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="O98" s="7"/>
       <c r="P98" s="25"/>
@@ -8494,10 +8494,10 @@
       <c r="R98" s="7"/>
       <c r="S98" s="7"/>
       <c r="T98" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U98" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
@@ -8523,7 +8523,7 @@
         <v>14</v>
       </c>
       <c r="H99" s="32" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="I99" s="32" t="s">
         <v>14</v>
@@ -8539,7 +8539,7 @@
       </c>
       <c r="M99" s="7"/>
       <c r="N99" s="19" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="O99" s="7"/>
       <c r="P99" s="25"/>
@@ -8547,10 +8547,10 @@
       <c r="R99" s="7"/>
       <c r="S99" s="7"/>
       <c r="T99" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U99" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
@@ -8600,10 +8600,10 @@
       <c r="R100" s="7"/>
       <c r="S100" s="7"/>
       <c r="T100" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U100" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="M101" s="7"/>
       <c r="N101" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="O101" s="7"/>
       <c r="P101" s="25"/>
@@ -8653,10 +8653,10 @@
       <c r="R101" s="7"/>
       <c r="S101" s="7"/>
       <c r="T101" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U101" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
@@ -8698,7 +8698,7 @@
       </c>
       <c r="M102" s="7"/>
       <c r="N102" s="19" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="O102" s="7"/>
       <c r="P102" s="25"/>
@@ -8706,10 +8706,10 @@
       <c r="R102" s="7"/>
       <c r="S102" s="7"/>
       <c r="T102" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U102" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
@@ -8735,7 +8735,7 @@
         <v>14</v>
       </c>
       <c r="H103" s="35" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="I103" s="35" t="s">
         <v>14</v>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="M103" s="7"/>
       <c r="N103" s="19" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="O103" s="7"/>
       <c r="P103" s="25"/>
@@ -8759,18 +8759,18 @@
       <c r="R103" s="7"/>
       <c r="S103" s="7"/>
       <c r="T103" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U103" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>26</v>
@@ -8804,7 +8804,7 @@
       </c>
       <c r="M104" s="7"/>
       <c r="N104" s="19" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="O104" s="7"/>
       <c r="P104" s="25"/>
@@ -8812,10 +8812,10 @@
       <c r="R104" s="7"/>
       <c r="S104" s="7"/>
       <c r="T104" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U104" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
@@ -8823,7 +8823,7 @@
         <v>559</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>512</v>
@@ -8841,7 +8841,7 @@
         <v>14</v>
       </c>
       <c r="H105" s="35" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="I105" s="35" t="s">
         <v>14</v>
@@ -8857,7 +8857,7 @@
       </c>
       <c r="M105" s="7"/>
       <c r="N105" s="19" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="O105" s="7"/>
       <c r="P105" s="25"/>
@@ -8865,10 +8865,10 @@
       <c r="R105" s="7"/>
       <c r="S105" s="7"/>
       <c r="T105" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U105" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
@@ -8910,7 +8910,7 @@
       </c>
       <c r="M106" s="7"/>
       <c r="N106" s="19" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="O106" s="7"/>
       <c r="P106" s="25"/>
@@ -8918,10 +8918,10 @@
       <c r="R106" s="7"/>
       <c r="S106" s="7"/>
       <c r="T106" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U106" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="M107" s="7"/>
       <c r="N107" s="19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="O107" s="7"/>
       <c r="P107" s="25"/>
@@ -8971,10 +8971,10 @@
       <c r="R107" s="7"/>
       <c r="S107" s="7"/>
       <c r="T107" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U107" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
@@ -9016,7 +9016,7 @@
       </c>
       <c r="M108" s="7"/>
       <c r="N108" s="19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="O108" s="7"/>
       <c r="P108" s="25"/>
@@ -9024,15 +9024,15 @@
       <c r="R108" s="7"/>
       <c r="S108" s="7"/>
       <c r="T108" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U108" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>542</v>
@@ -9053,7 +9053,7 @@
         <v>554</v>
       </c>
       <c r="H109" s="35" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="I109" s="35" t="s">
         <v>14</v>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="M109" s="7"/>
       <c r="N109" s="19" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="O109" s="7"/>
       <c r="P109" s="25"/>
@@ -9077,18 +9077,18 @@
       <c r="R109" s="7"/>
       <c r="S109" s="7"/>
       <c r="T109" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U109" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>26</v>
@@ -9122,7 +9122,7 @@
       </c>
       <c r="M110" s="7"/>
       <c r="N110" s="19" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="O110" s="7"/>
       <c r="P110" s="25"/>
@@ -9130,10 +9130,10 @@
       <c r="R110" s="7"/>
       <c r="S110" s="7"/>
       <c r="T110" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U110" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
@@ -9141,7 +9141,7 @@
         <v>535</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>255</v>
@@ -9175,7 +9175,7 @@
       </c>
       <c r="M111" s="7"/>
       <c r="N111" s="19" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="O111" s="7"/>
       <c r="P111" s="25"/>
@@ -9183,10 +9183,10 @@
       <c r="R111" s="7"/>
       <c r="S111" s="7"/>
       <c r="T111" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U111" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
@@ -9212,7 +9212,7 @@
         <v>92</v>
       </c>
       <c r="H112" s="35" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="I112" s="35" t="s">
         <v>14</v>
@@ -9228,7 +9228,7 @@
       </c>
       <c r="M112" s="7"/>
       <c r="N112" s="19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="O112" s="7"/>
       <c r="P112" s="25"/>
@@ -9236,10 +9236,10 @@
       <c r="R112" s="7"/>
       <c r="S112" s="7"/>
       <c r="T112" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U112" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="M113" s="7"/>
       <c r="N113" s="19" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="O113" s="7"/>
       <c r="P113" s="25"/>
@@ -9289,24 +9289,24 @@
       <c r="R113" s="7"/>
       <c r="S113" s="7"/>
       <c r="T113" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U113" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="D114" s="7" t="s">
         <v>653</v>
-      </c>
-      <c r="B114" s="7" t="s">
-        <v>657</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>655</v>
       </c>
       <c r="E114" s="19">
         <v>2019</v>
@@ -9334,7 +9334,7 @@
       </c>
       <c r="M114" s="11"/>
       <c r="N114" s="20" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="O114" s="7"/>
       <c r="P114" s="25"/>
@@ -9342,15 +9342,15 @@
       <c r="R114" s="7"/>
       <c r="S114" s="7"/>
       <c r="T114" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U114" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>534</v>
@@ -9371,7 +9371,7 @@
         <v>93</v>
       </c>
       <c r="H115" s="35" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="I115" s="35" t="s">
         <v>14</v>
@@ -9387,7 +9387,7 @@
       </c>
       <c r="M115" s="7"/>
       <c r="N115" s="19" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="O115" s="7"/>
       <c r="P115" s="25"/>
@@ -9395,15 +9395,15 @@
       <c r="R115" s="7"/>
       <c r="S115" s="7"/>
       <c r="T115" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U115" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>573</v>
@@ -9440,7 +9440,7 @@
       </c>
       <c r="M116" s="7"/>
       <c r="N116" s="19" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="O116" s="7"/>
       <c r="P116" s="25"/>
@@ -9448,10 +9448,10 @@
       <c r="R116" s="7"/>
       <c r="S116" s="7"/>
       <c r="T116" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U116" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
@@ -9501,18 +9501,18 @@
       <c r="R117" s="7"/>
       <c r="S117" s="7"/>
       <c r="T117" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U117" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>145</v>
@@ -9530,7 +9530,7 @@
         <v>112</v>
       </c>
       <c r="H118" s="35" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="I118" s="35" t="s">
         <v>14</v>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="M118" s="7"/>
       <c r="N118" s="19" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="O118" s="7"/>
       <c r="P118" s="25"/>
@@ -9555,15 +9555,15 @@
       <c r="S118" s="7"/>
       <c r="T118" s="7"/>
       <c r="U118" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>26</v>
@@ -9597,7 +9597,7 @@
       </c>
       <c r="M119" s="7"/>
       <c r="N119" s="19" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="O119" s="7"/>
       <c r="P119" s="25"/>
@@ -9605,10 +9605,10 @@
       <c r="R119" s="7"/>
       <c r="S119" s="7"/>
       <c r="T119" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U119" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="M120" s="7"/>
       <c r="N120" s="19" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="O120" s="7"/>
       <c r="P120" s="25"/>
@@ -9658,18 +9658,18 @@
       <c r="R120" s="7"/>
       <c r="S120" s="7"/>
       <c r="T120" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="U120" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>512</v>
@@ -9687,7 +9687,7 @@
         <v>14</v>
       </c>
       <c r="H121" s="35" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="I121" s="35" t="s">
         <v>14</v>
@@ -9703,7 +9703,7 @@
       </c>
       <c r="M121" s="7"/>
       <c r="N121" s="19" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="O121" s="7"/>
       <c r="P121" s="25"/>
@@ -9711,7 +9711,7 @@
       <c r="R121" s="7"/>
       <c r="S121" s="7"/>
       <c r="T121" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U121" s="7"/>
     </row>
@@ -9738,7 +9738,7 @@
         <v>14</v>
       </c>
       <c r="H122" s="35" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I122" s="35" t="s">
         <v>14</v>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="M122" s="7"/>
       <c r="N122" s="19" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="O122" s="7"/>
       <c r="P122" s="25"/>
@@ -9762,7 +9762,7 @@
       <c r="R122" s="7"/>
       <c r="S122" s="7"/>
       <c r="T122" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U122" s="7"/>
     </row>
@@ -9805,7 +9805,7 @@
       </c>
       <c r="M123" s="7"/>
       <c r="N123" s="19" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="O123" s="7"/>
       <c r="P123" s="25"/>
@@ -9820,7 +9820,7 @@
         <v>529</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>81</v>
@@ -9854,7 +9854,7 @@
       </c>
       <c r="M124" s="11"/>
       <c r="N124" s="20" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="O124" s="7"/>
       <c r="P124" s="25"/>
@@ -9862,7 +9862,7 @@
       <c r="R124" s="7"/>
       <c r="S124" s="7"/>
       <c r="T124" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U124" s="7"/>
     </row>
@@ -9905,7 +9905,7 @@
       </c>
       <c r="M125" s="11"/>
       <c r="N125" s="20" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="O125" s="7"/>
       <c r="P125" s="25"/>
@@ -9947,14 +9947,14 @@
         <v>14</v>
       </c>
       <c r="K126" s="34">
-        <v>43832</v>
+        <v>43831</v>
       </c>
       <c r="L126" s="42" t="s">
         <v>276</v>
       </c>
       <c r="M126" s="28"/>
       <c r="N126" s="29" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="O126" s="30"/>
       <c r="P126" s="25"/>
@@ -9962,22 +9962,22 @@
       <c r="R126" s="7"/>
       <c r="S126" s="7"/>
       <c r="T126" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="U126" s="7"/>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="C127" s="14" t="s">
         <v>599</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="D127" s="14" t="s">
         <v>600</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>601</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>602</v>
       </c>
       <c r="E127" s="15">
         <v>2019</v>
@@ -9998,14 +9998,14 @@
         <v>14</v>
       </c>
       <c r="K127" s="34">
-        <v>43833</v>
+        <v>43832</v>
       </c>
       <c r="L127" s="42" t="s">
         <v>276</v>
       </c>
       <c r="M127" s="28"/>
       <c r="N127" s="29" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="O127" s="30"/>
       <c r="P127" s="25"/>
@@ -10014,6 +10014,53 @@
       <c r="S127" s="7"/>
       <c r="T127" s="7"/>
       <c r="U127" s="7"/>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A128" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="E128" s="15">
+        <v>2019</v>
+      </c>
+      <c r="F128" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G128" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H128" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I128" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J128" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K128" s="34">
+        <v>43833</v>
+      </c>
+      <c r="L128" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="M128" s="28"/>
+      <c r="N128" s="29"/>
+      <c r="O128" s="30"/>
+      <c r="P128" s="25"/>
+      <c r="Q128" s="26"/>
+      <c r="R128" s="7"/>
+      <c r="S128" s="7"/>
+      <c r="T128" s="7"/>
+      <c r="U128" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U1048576 U126">
@@ -10304,9 +10351,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10353,134 +10400,113 @@
         <v>43130</v>
       </c>
       <c r="F2" s="13">
-        <f t="shared" ref="F2:F8" ca="1" si="0">TODAY()-E2</f>
-        <v>561</v>
+        <f t="shared" ref="F2:F7" ca="1" si="0">TODAY()-E2</f>
+        <v>592</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>586</v>
+        <v>605</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>589</v>
+        <v>606</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>587</v>
+        <v>90</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>588</v>
+        <v>90</v>
       </c>
       <c r="E3" s="10">
-        <v>43455</v>
+        <v>43488</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>607</v>
+        <v>641</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>608</v>
+        <v>642</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>90</v>
+        <v>643</v>
       </c>
       <c r="E4" s="10">
-        <v>43488</v>
+        <v>43585</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>643</v>
+        <v>663</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>644</v>
+        <v>664</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>645</v>
+        <v>82</v>
       </c>
       <c r="E5" s="10">
-        <v>43585</v>
+        <v>43599</v>
       </c>
       <c r="F5" s="12">
+        <f ca="1">TODAY()-E5</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E6" s="10">
+        <v>43642</v>
+      </c>
+      <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="10">
-        <v>43599</v>
-      </c>
-      <c r="F6" s="12">
-        <f ca="1">TODAY()-E6</f>
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>530</v>
+        <v>661</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>660</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>531</v>
+        <v>13</v>
       </c>
       <c r="E7" s="10">
-        <v>43642</v>
+        <v>43645</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="10">
-        <v>43645</v>
-      </c>
-      <c r="F8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -10545,7 +10571,7 @@
       </c>
       <c r="F2" s="45">
         <f t="shared" ref="F2:F5" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>3.7890410958904108</v>
+        <v>3.8739726027397259</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10566,7 +10592,7 @@
       </c>
       <c r="F3" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7890410958904108</v>
+        <v>3.8739726027397259</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -10585,7 +10611,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>119.7013698630137</v>
+        <v>119.78630136986301</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10606,7 +10632,7 @@
       </c>
       <c r="F5" s="45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1671232876712327</v>
+        <v>3.2520547945205478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update projects, publications, students
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="686">
   <si>
     <t>title</t>
   </si>
@@ -2076,6 +2076,12 @@
   </si>
   <si>
     <t>Van Goethem, Nina; Struelens Marc J; De Keersmaecker, Sigrid C J; Roosens, Nancy H C; Robert, Annie; Quoilin, Sophie; Van Oyen, Herman; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>A timely opportunity for identifying Taenia solium control strategies and targets beyond 2020</t>
+  </si>
+  <si>
+    <t>Dixon, Matthew Andrew; Braae, Uffe Christian; Winskill, Peter; Devleesschauwer, Brecht; Trevisan, Chiara; Van Damme, Inge; Walker, Martin; Hamley, Jonathan I D; Ramiandrasoa, Sylvia N; Schmidt, Veronika; Gabriël, Sarah; Harrison, Wendy; Basáñez, Maria-Gloria</t>
   </si>
 </sst>
 </file>
@@ -2289,106 +2295,6 @@
   </cellStyles>
   <dxfs count="60">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2548,6 +2454,106 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2562,73 +2568,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U130" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <autoFilter ref="A1:U130"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U131" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:U131"/>
   <sortState ref="A2:U130">
     <sortCondition ref="K1:K130"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="57"/>
-    <tableColumn id="2" name="authors" dataDxfId="56"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="55"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="54"/>
-    <tableColumn id="6" name="year" dataDxfId="53"/>
-    <tableColumn id="4" name="volume" dataDxfId="52"/>
-    <tableColumn id="5" name="issue" dataDxfId="51"/>
-    <tableColumn id="7" name="eID" dataDxfId="50"/>
-    <tableColumn id="8" name="from" dataDxfId="49"/>
-    <tableColumn id="9" name="to" dataDxfId="48"/>
-    <tableColumn id="10" name="date" dataDxfId="47"/>
-    <tableColumn id="14" name="classification" dataDxfId="46"/>
-    <tableColumn id="12" name="IF" dataDxfId="45"/>
-    <tableColumn id="13" name="DOI" dataDxfId="44"/>
-    <tableColumn id="15" name="WoS" dataDxfId="43"/>
-    <tableColumn id="16" name="rank" dataDxfId="42"/>
-    <tableColumn id="17" name="quartile" dataDxfId="41"/>
-    <tableColumn id="18" name="category" dataDxfId="40"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="39"/>
-    <tableColumn id="20" name="SC" dataDxfId="38"/>
-    <tableColumn id="21" name="UGent" dataDxfId="37"/>
+    <tableColumn id="1" name="title" dataDxfId="47"/>
+    <tableColumn id="2" name="authors" dataDxfId="46"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
+    <tableColumn id="6" name="year" dataDxfId="43"/>
+    <tableColumn id="4" name="volume" dataDxfId="42"/>
+    <tableColumn id="5" name="issue" dataDxfId="41"/>
+    <tableColumn id="7" name="eID" dataDxfId="40"/>
+    <tableColumn id="8" name="from" dataDxfId="39"/>
+    <tableColumn id="9" name="to" dataDxfId="38"/>
+    <tableColumn id="10" name="date" dataDxfId="37"/>
+    <tableColumn id="14" name="classification" dataDxfId="36"/>
+    <tableColumn id="12" name="IF" dataDxfId="35"/>
+    <tableColumn id="13" name="DOI" dataDxfId="34"/>
+    <tableColumn id="15" name="WoS" dataDxfId="33"/>
+    <tableColumn id="16" name="rank" dataDxfId="32"/>
+    <tableColumn id="17" name="quartile" dataDxfId="31"/>
+    <tableColumn id="18" name="category" dataDxfId="30"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
+    <tableColumn id="20" name="SC" dataDxfId="28"/>
+    <tableColumn id="21" name="UGent" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:J7"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="35"/>
-    <tableColumn id="2" name="authors" dataDxfId="34"/>
-    <tableColumn id="3" name="editors" dataDxfId="33"/>
-    <tableColumn id="11" name="book" dataDxfId="32"/>
-    <tableColumn id="6" name="year" dataDxfId="31"/>
-    <tableColumn id="8" name="from" dataDxfId="30"/>
-    <tableColumn id="9" name="to" dataDxfId="29"/>
-    <tableColumn id="10" name="date" dataDxfId="28"/>
-    <tableColumn id="12" name="IF" dataDxfId="27"/>
-    <tableColumn id="13" name="DOI" dataDxfId="26"/>
+    <tableColumn id="1" name="title" dataDxfId="25"/>
+    <tableColumn id="2" name="authors" dataDxfId="24"/>
+    <tableColumn id="3" name="editors" dataDxfId="23"/>
+    <tableColumn id="11" name="book" dataDxfId="22"/>
+    <tableColumn id="6" name="year" dataDxfId="21"/>
+    <tableColumn id="8" name="from" dataDxfId="20"/>
+    <tableColumn id="9" name="to" dataDxfId="19"/>
+    <tableColumn id="10" name="date" dataDxfId="18"/>
+    <tableColumn id="12" name="IF" dataDxfId="17"/>
+    <tableColumn id="13" name="DOI" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:F7"/>
   <sortState ref="A2:F7">
     <sortCondition ref="E1:E7"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="23"/>
-    <tableColumn id="2" name="authors" dataDxfId="22"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="21"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="20"/>
-    <tableColumn id="10" name="date" dataDxfId="19"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="18">
+    <tableColumn id="1" name="title" dataDxfId="13"/>
+    <tableColumn id="2" name="authors" dataDxfId="12"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
+    <tableColumn id="10" name="date" dataDxfId="9"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="8">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2637,18 +2643,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="15"/>
-    <tableColumn id="2" name="authors" dataDxfId="14"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="13"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="12"/>
-    <tableColumn id="10" name="date" dataDxfId="11"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="10">
+    <tableColumn id="1" name="title" dataDxfId="5"/>
+    <tableColumn id="2" name="authors" dataDxfId="4"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
+    <tableColumn id="10" name="date" dataDxfId="1"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="0">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2943,10 +2949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U130"/>
+  <dimension ref="A1:U131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10179,7 +10185,7 @@
         <v>14</v>
       </c>
       <c r="K130" s="33">
-        <v>43833</v>
+        <v>43832</v>
       </c>
       <c r="L130" s="41" t="s">
         <v>276</v>
@@ -10196,44 +10202,91 @@
       <c r="T130" s="7"/>
       <c r="U130" s="7"/>
     </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A131" s="13" t="s">
+        <v>684</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E131" s="14">
+        <v>2019</v>
+      </c>
+      <c r="F131" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G131" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H131" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I131" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J131" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K131" s="33">
+        <v>43833</v>
+      </c>
+      <c r="L131" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="M131" s="27"/>
+      <c r="N131" s="28"/>
+      <c r="O131" s="29"/>
+      <c r="P131" s="24"/>
+      <c r="Q131" s="25"/>
+      <c r="R131" s="7"/>
+      <c r="S131" s="7"/>
+      <c r="T131" s="7"/>
+      <c r="U131" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U1048576 U126">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10535,7 +10588,7 @@
       </c>
       <c r="F2" s="12">
         <f t="shared" ref="F2:F7" ca="1" si="0">TODAY()-E2</f>
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10556,7 +10609,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -10577,7 +10630,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10598,7 +10651,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -10619,7 +10672,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -10640,7 +10693,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -10705,7 +10758,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>4.1424657534246574</v>
+        <v>4.1643835616438354</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10726,7 +10779,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1424657534246574</v>
+        <v>4.1643835616438354</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -10747,7 +10800,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5205479452054793</v>
+        <v>3.5424657534246577</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10768,7 +10821,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>1.8904109589041096</v>
+        <v>1.9123287671232876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully published & new submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="704">
   <si>
     <t>title</t>
   </si>
@@ -2130,6 +2130,12 @@
   </si>
   <si>
     <t>10.2471/blt.19.238485</t>
+  </si>
+  <si>
+    <t>Conducting national burden of disease studies in small countries in Europe – A challenge or a feasibility?</t>
+  </si>
+  <si>
+    <t>Cuschieri, Sarah; Pallari, Elena; Terzic, Natasa; Alkerwi, Ala'a; Sigurvinsdottir, Rannveig; Sigfusdottir, Inga Dora; Devleesschauwer, Brecht</t>
   </si>
 </sst>
 </file>
@@ -2400,7 +2406,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2458,11 +2464,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2691,8 +2697,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F9"/>
   <sortState ref="A2:F10">
     <sortCondition descending="1" ref="F1:F10"/>
   </sortState>
@@ -3020,7 +3026,7 @@
   <dimension ref="A1:U135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10354,68 +10360,66 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A132" s="13" t="s">
-        <v>567</v>
-      </c>
-      <c r="B132" s="13" t="s">
-        <v>526</v>
-      </c>
-      <c r="C132" s="13" t="s">
-        <v>568</v>
-      </c>
-      <c r="D132" s="13" t="s">
-        <v>569</v>
-      </c>
-      <c r="E132" s="14">
+      <c r="A132" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="E132" s="18">
         <v>2020</v>
       </c>
-      <c r="F132" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G132" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H132" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I132" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J132" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K132" s="33">
-        <v>44197</v>
-      </c>
-      <c r="L132" s="41" t="s">
-        <v>276</v>
-      </c>
-      <c r="M132" s="27"/>
-      <c r="N132" s="28" t="s">
-        <v>637</v>
-      </c>
-      <c r="O132" s="29"/>
+      <c r="F132" s="18">
+        <v>63</v>
+      </c>
+      <c r="G132" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H132" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I132" s="18">
+        <v>500</v>
+      </c>
+      <c r="J132" s="18">
+        <v>508</v>
+      </c>
+      <c r="K132" s="10">
+        <v>43952</v>
+      </c>
+      <c r="L132" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="M132" s="11"/>
+      <c r="N132" s="19" t="s">
+        <v>697</v>
+      </c>
+      <c r="O132" s="7"/>
       <c r="P132" s="24"/>
       <c r="Q132" s="25"/>
       <c r="R132" s="7"/>
       <c r="S132" s="7"/>
-      <c r="T132" s="7" t="s">
-        <v>606</v>
-      </c>
+      <c r="T132" s="7"/>
       <c r="U132" s="7"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>670</v>
+        <v>567</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>671</v>
+        <v>526</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>676</v>
+        <v>568</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>676</v>
+        <v>569</v>
       </c>
       <c r="E133" s="14">
         <v>2020</v>
@@ -10436,21 +10440,23 @@
         <v>14</v>
       </c>
       <c r="K133" s="33">
-        <v>44199</v>
+        <v>44197</v>
       </c>
       <c r="L133" s="41" t="s">
         <v>276</v>
       </c>
       <c r="M133" s="27"/>
       <c r="N133" s="28" t="s">
-        <v>697</v>
+        <v>637</v>
       </c>
       <c r="O133" s="29"/>
       <c r="P133" s="24"/>
       <c r="Q133" s="25"/>
       <c r="R133" s="7"/>
       <c r="S133" s="7"/>
-      <c r="T133" s="7"/>
+      <c r="T133" s="7" t="s">
+        <v>606</v>
+      </c>
       <c r="U133" s="7"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
@@ -10846,7 +10852,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -10895,8 +10901,8 @@
         <v>43599</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F8" ca="1" si="0">TODAY()-E2</f>
-        <v>294</v>
+        <f t="shared" ref="F2:F9" ca="1" si="0">TODAY()-E2</f>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10917,7 +10923,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>133</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -10938,7 +10944,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10959,7 +10965,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -10980,7 +10986,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -11001,7 +11007,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -11022,7 +11028,28 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E9" s="10">
+        <v>43942</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11087,7 +11114,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>4.3424657534246576</v>
+        <v>4.4794520547945202</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11108,7 +11135,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3424657534246576</v>
+        <v>4.4794520547945202</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11129,7 +11156,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7205479452054795</v>
+        <v>3.8575342465753426</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -11150,7 +11177,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>2.0904109589041098</v>
+        <v>2.2273972602739724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new submission & new accepted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="706">
   <si>
     <t>title</t>
   </si>
@@ -2136,6 +2136,12 @@
   </si>
   <si>
     <t>Cuschieri, Sarah; Pallari, Elena; Terzic, Natasa; Alkerwi, Ala'a; Sigurvinsdottir, Rannveig; Sigfusdottir, Inga Dora; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Population vulnerability to COVID-19 in Europe: a burden of disease analysis</t>
+  </si>
+  <si>
+    <t>Wyper, Grant MA; Assunção, Ricardo MA; Cuschieri, Sarah; Devleeschauwer, Brecht; Fletcher, Eilidh; Haagsma, Juanita A; Hilderink, Henk; Idavain, Jane; Lesnik, Tina; Von der Lippe, Elena; Majdan, Marek; Santric-Milicevic, Milena; Pallari, Elena; Peñalvo, José L; Pires, Sara M; Plass, Dietrich; Santos, João V; Stockton, Diane L; Thomsen, Sofie T; Grant, Ian</t>
   </si>
 </sst>
 </file>
@@ -2642,8 +2648,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U137" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
-  <autoFilter ref="A1:U137"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U138" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="A1:U138"/>
   <sortState ref="A2:U137">
     <sortCondition ref="K1:K137"/>
   </sortState>
@@ -3023,10 +3029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U137"/>
+  <dimension ref="A1:U138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView topLeftCell="A101" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10648,6 +10654,53 @@
       <c r="S137" s="7"/>
       <c r="T137" s="7"/>
       <c r="U137" s="7"/>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
+        <v>686</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>687</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D138" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E138" s="14">
+        <v>2020</v>
+      </c>
+      <c r="F138" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G138" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H138" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I138" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J138" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K138" s="33">
+        <v>44202</v>
+      </c>
+      <c r="L138" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="M138" s="27"/>
+      <c r="N138" s="28"/>
+      <c r="O138" s="29"/>
+      <c r="P138" s="24"/>
+      <c r="Q138" s="25"/>
+      <c r="R138" s="7"/>
+      <c r="S138" s="7"/>
+      <c r="T138" s="7"/>
+      <c r="U138" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S136:U1048576">
@@ -10948,7 +11001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10995,8 +11050,8 @@
         <v>43803</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F7" ca="1" si="0">TODAY()-E2</f>
-        <v>140</v>
+        <f ca="1">TODAY()-E2</f>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11016,79 +11071,79 @@
         <v>43837</v>
       </c>
       <c r="F3" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <f ca="1">TODAY()-E3</f>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>686</v>
+        <v>694</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>687</v>
+        <v>695</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>26</v>
+        <v>270</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>29</v>
+        <v>271</v>
       </c>
       <c r="E4" s="10">
-        <v>43846</v>
+        <v>43860</v>
       </c>
       <c r="F4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <f ca="1">TODAY()-E4</f>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>270</v>
+        <v>692</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>271</v>
+        <v>693</v>
       </c>
       <c r="E5" s="10">
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <f ca="1">TODAY()-E5</f>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>688</v>
+        <v>703</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>692</v>
+        <v>270</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>693</v>
+        <v>271</v>
       </c>
       <c r="E6" s="10">
-        <v>43861</v>
+        <v>43942</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <f ca="1">TODAY()-E6</f>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>270</v>
@@ -11097,11 +11152,11 @@
         <v>271</v>
       </c>
       <c r="E7" s="10">
-        <v>43942</v>
+        <v>43956</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f ca="1">TODAY()-E7</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11166,7 +11221,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>4.4794520547945202</v>
+        <v>4.515068493150685</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11187,7 +11242,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4794520547945202</v>
+        <v>4.515068493150685</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11208,7 +11263,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8575342465753426</v>
+        <v>3.893150684931507</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -11229,7 +11284,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>2.2273972602739724</v>
+        <v>2.2630136986301368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new accepted and published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="748">
   <si>
     <t>title</t>
   </si>
@@ -2250,15 +2250,34 @@
   </si>
   <si>
     <t>Br. J. Nutr.</t>
+  </si>
+  <si>
+    <t>BMJ Open</t>
+  </si>
+  <si>
+    <t>Risk Metrics: Quantifying the Impact of Adverse Health Effects</t>
+  </si>
+  <si>
+    <t>Devleesschauwer, Brecht; Pires, Sara Monteiro; Kowalcyk, Barbara B; Scharff, Robert L; Havelaar, Arie H; Speybroeck, Niko</t>
+  </si>
+  <si>
+    <t>Pérez-Rodríguez, Fernando</t>
+  </si>
+  <si>
+    <t>Risk Assessment Methods for Biological and Chemical Hazards in Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1201/9780429083525 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2324,7 +2343,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2455,6 +2474,9 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2463,6 +2485,127 @@
   </cellStyles>
   <dxfs count="62">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2487,7 +2630,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2622,126 +2764,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2756,73 +2778,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U141" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:U141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U142" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="A1:U142"/>
   <sortState ref="A2:U141">
     <sortCondition ref="K1:K141"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="47"/>
-    <tableColumn id="2" name="authors" dataDxfId="46"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
-    <tableColumn id="6" name="year" dataDxfId="43"/>
-    <tableColumn id="4" name="volume" dataDxfId="42"/>
-    <tableColumn id="5" name="issue" dataDxfId="41"/>
-    <tableColumn id="7" name="eID" dataDxfId="40"/>
-    <tableColumn id="8" name="from" dataDxfId="39"/>
-    <tableColumn id="9" name="to" dataDxfId="38"/>
-    <tableColumn id="10" name="date" dataDxfId="37"/>
-    <tableColumn id="14" name="classification" dataDxfId="36"/>
-    <tableColumn id="12" name="IF" dataDxfId="35"/>
-    <tableColumn id="13" name="DOI" dataDxfId="34"/>
-    <tableColumn id="15" name="WoS" dataDxfId="33"/>
-    <tableColumn id="16" name="rank" dataDxfId="32"/>
-    <tableColumn id="17" name="quartile" dataDxfId="31"/>
-    <tableColumn id="18" name="category" dataDxfId="30"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
-    <tableColumn id="20" name="SC" dataDxfId="28"/>
-    <tableColumn id="21" name="UGent" dataDxfId="27"/>
+    <tableColumn id="1" name="title" dataDxfId="59"/>
+    <tableColumn id="2" name="authors" dataDxfId="58"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="57"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="56"/>
+    <tableColumn id="6" name="year" dataDxfId="55"/>
+    <tableColumn id="4" name="volume" dataDxfId="54"/>
+    <tableColumn id="5" name="issue" dataDxfId="53"/>
+    <tableColumn id="7" name="eID" dataDxfId="52"/>
+    <tableColumn id="8" name="from" dataDxfId="51"/>
+    <tableColumn id="9" name="to" dataDxfId="50"/>
+    <tableColumn id="10" name="date" dataDxfId="49"/>
+    <tableColumn id="14" name="classification" dataDxfId="48"/>
+    <tableColumn id="12" name="IF" dataDxfId="47"/>
+    <tableColumn id="13" name="DOI" dataDxfId="46"/>
+    <tableColumn id="15" name="WoS" dataDxfId="45"/>
+    <tableColumn id="16" name="rank" dataDxfId="44"/>
+    <tableColumn id="17" name="quartile" dataDxfId="43"/>
+    <tableColumn id="18" name="category" dataDxfId="42"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="41"/>
+    <tableColumn id="20" name="SC" dataDxfId="40"/>
+    <tableColumn id="21" name="UGent" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J7" totalsRowShown="0" headerRowDxfId="26">
-  <autoFilter ref="A1:J7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J8" totalsRowShown="0" headerRowDxfId="38">
+  <autoFilter ref="A1:J8"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="25"/>
-    <tableColumn id="2" name="authors" dataDxfId="24"/>
-    <tableColumn id="3" name="editors" dataDxfId="23"/>
-    <tableColumn id="11" name="book" dataDxfId="22"/>
-    <tableColumn id="6" name="year" dataDxfId="21"/>
-    <tableColumn id="8" name="from" dataDxfId="20"/>
-    <tableColumn id="9" name="to" dataDxfId="19"/>
-    <tableColumn id="10" name="date" dataDxfId="18"/>
-    <tableColumn id="12" name="IF" dataDxfId="17"/>
-    <tableColumn id="13" name="DOI" dataDxfId="16"/>
+    <tableColumn id="1" name="title" dataDxfId="37"/>
+    <tableColumn id="2" name="authors" dataDxfId="36"/>
+    <tableColumn id="3" name="editors" dataDxfId="35"/>
+    <tableColumn id="11" name="book" dataDxfId="34"/>
+    <tableColumn id="6" name="year" dataDxfId="33"/>
+    <tableColumn id="8" name="from" dataDxfId="32"/>
+    <tableColumn id="9" name="to" dataDxfId="31"/>
+    <tableColumn id="10" name="date" dataDxfId="30"/>
+    <tableColumn id="12" name="IF" dataDxfId="29"/>
+    <tableColumn id="13" name="DOI" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:F13"/>
   <sortState ref="A2:F10">
     <sortCondition descending="1" ref="F1:F10"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="5"/>
-    <tableColumn id="2" name="authors" dataDxfId="4"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
-    <tableColumn id="10" name="date" dataDxfId="1"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="0">
+    <tableColumn id="1" name="title" dataDxfId="25"/>
+    <tableColumn id="2" name="authors" dataDxfId="24"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="23"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="22"/>
+    <tableColumn id="10" name="date" dataDxfId="21"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="20">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2831,18 +2853,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="13"/>
-    <tableColumn id="2" name="authors" dataDxfId="12"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
-    <tableColumn id="10" name="date" dataDxfId="9"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="8">
+    <tableColumn id="1" name="title" dataDxfId="17"/>
+    <tableColumn id="2" name="authors" dataDxfId="16"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="15"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="14"/>
+    <tableColumn id="10" name="date" dataDxfId="13"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="12">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3137,10 +3159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U141"/>
+  <dimension ref="A1:U142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView topLeftCell="A107" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10734,93 +10756,95 @@
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>732</v>
+        <v>567</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>690</v>
+        <v>526</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>651</v>
+        <v>568</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>530</v>
+        <v>569</v>
       </c>
       <c r="E137" s="18">
         <v>2020</v>
       </c>
       <c r="F137" s="18">
-        <v>383</v>
+        <v>67</v>
       </c>
       <c r="G137" s="19" t="s">
-        <v>551</v>
+        <v>737</v>
       </c>
       <c r="H137" s="18" t="s">
         <v>14</v>
       </c>
       <c r="I137" s="18">
-        <v>396</v>
+        <v>69</v>
       </c>
       <c r="J137" s="18">
-        <v>397</v>
+        <v>81</v>
       </c>
       <c r="K137" s="10">
-        <v>44035</v>
+        <v>44013</v>
       </c>
       <c r="L137" s="10" t="s">
         <v>276</v>
       </c>
       <c r="M137" s="11"/>
       <c r="N137" s="19" t="s">
-        <v>733</v>
+        <v>637</v>
       </c>
       <c r="O137" s="7"/>
       <c r="P137" s="24"/>
       <c r="Q137" s="25"/>
       <c r="R137" s="7"/>
       <c r="S137" s="7"/>
-      <c r="T137" s="7"/>
+      <c r="T137" s="7" t="s">
+        <v>606</v>
+      </c>
       <c r="U137" s="7"/>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>734</v>
+        <v>711</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>735</v>
+        <v>712</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>271</v>
+        <v>13</v>
       </c>
       <c r="E138" s="18">
         <v>2020</v>
       </c>
       <c r="F138" s="18">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G138" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H138" s="18">
-        <v>68</v>
-      </c>
-      <c r="I138" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J138" s="18" t="s">
-        <v>14</v>
+      <c r="H138" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I138" s="18">
+        <v>719</v>
+      </c>
+      <c r="J138" s="18">
+        <v>720</v>
       </c>
       <c r="K138" s="10">
-        <v>44035</v>
+        <v>44032</v>
       </c>
       <c r="L138" s="10" t="s">
         <v>276</v>
       </c>
       <c r="M138" s="11"/>
       <c r="N138" s="19" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="O138" s="7"/>
       <c r="P138" s="24"/>
@@ -10832,97 +10856,95 @@
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>567</v>
+        <v>732</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>526</v>
+        <v>690</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>568</v>
+        <v>651</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>569</v>
+        <v>530</v>
       </c>
       <c r="E139" s="18">
         <v>2020</v>
       </c>
       <c r="F139" s="18">
-        <v>67</v>
+        <v>383</v>
       </c>
       <c r="G139" s="19" t="s">
-        <v>737</v>
+        <v>551</v>
       </c>
       <c r="H139" s="18" t="s">
         <v>14</v>
       </c>
       <c r="I139" s="18">
-        <v>69</v>
+        <v>396</v>
       </c>
       <c r="J139" s="18">
-        <v>81</v>
+        <v>397</v>
       </c>
       <c r="K139" s="10">
-        <v>44013</v>
+        <v>44035</v>
       </c>
       <c r="L139" s="10" t="s">
         <v>276</v>
       </c>
       <c r="M139" s="11"/>
       <c r="N139" s="19" t="s">
-        <v>637</v>
+        <v>733</v>
       </c>
       <c r="O139" s="7"/>
       <c r="P139" s="24"/>
       <c r="Q139" s="25"/>
       <c r="R139" s="7"/>
       <c r="S139" s="7"/>
-      <c r="T139" s="7" t="s">
-        <v>606</v>
-      </c>
+      <c r="T139" s="7"/>
       <c r="U139" s="7"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A140" s="13" t="s">
-        <v>711</v>
-      </c>
-      <c r="B140" s="13" t="s">
-        <v>712</v>
-      </c>
-      <c r="C140" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D140" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E140" s="14">
+      <c r="A140" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E140" s="18">
         <v>2020</v>
       </c>
-      <c r="F140" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G140" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H140" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I140" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J140" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K140" s="33">
-        <v>44198</v>
-      </c>
-      <c r="L140" s="41" t="s">
-        <v>276</v>
-      </c>
-      <c r="M140" s="27"/>
-      <c r="N140" s="28" t="s">
-        <v>727</v>
-      </c>
-      <c r="O140" s="29"/>
+      <c r="F140" s="18">
+        <v>78</v>
+      </c>
+      <c r="G140" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H140" s="18">
+        <v>68</v>
+      </c>
+      <c r="I140" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J140" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K140" s="10">
+        <v>44035</v>
+      </c>
+      <c r="L140" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="M140" s="11"/>
+      <c r="N140" s="19" t="s">
+        <v>736</v>
+      </c>
+      <c r="O140" s="7"/>
       <c r="P140" s="24"/>
       <c r="Q140" s="25"/>
       <c r="R140" s="7"/>
@@ -10962,7 +10984,7 @@
         <v>14</v>
       </c>
       <c r="K141" s="33">
-        <v>44199</v>
+        <v>44197</v>
       </c>
       <c r="L141" s="41" t="s">
         <v>276</v>
@@ -10977,52 +10999,99 @@
       <c r="T141" s="7"/>
       <c r="U141" s="7"/>
     </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A142" s="13" t="s">
+        <v>684</v>
+      </c>
+      <c r="B142" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="D142" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="E142" s="14">
+        <v>2020</v>
+      </c>
+      <c r="F142" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G142" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H142" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I142" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J142" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K142" s="33">
+        <v>44198</v>
+      </c>
+      <c r="L142" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="M142" s="27"/>
+      <c r="N142" s="28"/>
+      <c r="O142" s="29"/>
+      <c r="P142" s="24"/>
+      <c r="Q142" s="25"/>
+      <c r="R142" s="7"/>
+      <c r="S142" s="7"/>
+      <c r="T142" s="7"/>
+      <c r="U142" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S136:U1048576">
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11036,9 +11105,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11264,6 +11333,36 @@
         <v>506</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2021</v>
+      </c>
+      <c r="F8" s="18">
+        <v>47</v>
+      </c>
+      <c r="G8" s="18">
+        <v>78</v>
+      </c>
+      <c r="H8" s="46">
+        <v>44134</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="19" t="s">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -11274,7 +11373,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -11323,109 +11422,109 @@
         <v>43803</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F14" ca="1" si="0">TODAY()-E2</f>
-        <v>244</v>
+        <f t="shared" ref="F2:F13" ca="1" si="0">TODAY()-E2</f>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>90</v>
+        <v>271</v>
       </c>
       <c r="E3" s="10">
-        <v>43837</v>
+        <v>43860</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>270</v>
+        <v>691</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>271</v>
+        <v>692</v>
       </c>
       <c r="E4" s="10">
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>689</v>
+        <v>701</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>688</v>
+        <v>702</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>691</v>
+        <v>270</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>692</v>
+        <v>271</v>
       </c>
       <c r="E5" s="10">
-        <v>43861</v>
+        <v>43942</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>186</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>270</v>
+        <v>708</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>271</v>
+        <v>709</v>
       </c>
       <c r="E6" s="10">
-        <v>43942</v>
+        <v>43972</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>710</v>
+        <v>715</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>708</v>
+        <v>262</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>709</v>
+        <v>265</v>
       </c>
       <c r="E7" s="10">
-        <v>43972</v>
+        <v>43986</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
@@ -11434,149 +11533,128 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>262</v>
+        <v>161</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>265</v>
+        <v>162</v>
       </c>
       <c r="E8" s="10">
-        <v>43986</v>
+        <v>43990</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>161</v>
+        <v>270</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="E9" s="10">
-        <v>43990</v>
+        <v>43992</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>270</v>
+        <v>723</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>271</v>
+        <v>721</v>
       </c>
       <c r="E10" s="10">
-        <v>43992</v>
+        <v>44000</v>
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="E11" s="10">
-        <v>44000</v>
+        <v>44006</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="E12" s="10">
-        <v>44006</v>
+        <v>44014</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>728</v>
+        <v>738</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>729</v>
+        <v>740</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>730</v>
+        <v>741</v>
       </c>
       <c r="E13" s="10">
-        <v>44014</v>
+        <v>44047</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>738</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>740</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>741</v>
-      </c>
-      <c r="E14" s="10">
-        <v>44047</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -11641,7 +11719,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>4.7643835616438359</v>
+        <v>4.8027397260273972</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11662,7 +11740,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7643835616438359</v>
+        <v>4.8027397260273972</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11683,7 +11761,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1424657534246574</v>
+        <v>4.1808219178082195</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -11704,7 +11782,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>2.5123287671232877</v>
+        <v>2.5506849315068494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added doi + new submission
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="791">
   <si>
     <t>title</t>
   </si>
@@ -2382,6 +2382,21 @@
   </si>
   <si>
     <t>Reflections on key methodological decisions in national burden of disease assessments</t>
+  </si>
+  <si>
+    <t>10.1136/jech-2020-213791</t>
+  </si>
+  <si>
+    <t>The Global Burden of Animal Diseases rollout</t>
+  </si>
+  <si>
+    <t>Rushton, Jonathan; Huntington, Ben; Gilbert, William; Herrero, Mario; Torgerson, Paul R; Shaw, Alexandra P M; Bruce, Mieghan; Marsh, Tom L; Pendell, Dustin L; Bernardo, Theresa M; Stacey, Deborah; Grace, Delia; Watkins, Kevin; Bondad-Reantaso, Melba; Devleesschauwer, Brecht; Pigott, David M; Stone, Matthew; Mesenhowski, Shannon</t>
+  </si>
+  <si>
+    <t>The Lancet</t>
+  </si>
+  <si>
+    <t>Lancet</t>
   </si>
 </sst>
 </file>
@@ -2976,8 +2991,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F13" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F14"/>
   <sortState ref="A2:F10">
     <sortCondition descending="1" ref="F1:F10"/>
   </sortState>
@@ -3304,7 +3319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A123" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
@@ -11745,7 +11760,9 @@
         <v>274</v>
       </c>
       <c r="M153" s="49"/>
-      <c r="N153" s="48"/>
+      <c r="N153" s="48" t="s">
+        <v>786</v>
+      </c>
       <c r="O153" s="29"/>
       <c r="P153" s="24"/>
       <c r="Q153" s="25"/>
@@ -12091,9 +12108,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12141,7 +12158,7 @@
       </c>
       <c r="F2" s="12">
         <f t="shared" ref="F2:F13" ca="1" si="0">TODAY()-E2</f>
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12162,7 +12179,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12183,7 +12200,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12204,7 +12221,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -12225,7 +12242,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -12246,7 +12263,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -12267,7 +12284,7 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -12288,7 +12305,7 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -12309,7 +12326,7 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -12330,7 +12347,7 @@
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -12351,7 +12368,7 @@
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -12372,6 +12389,27 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="E14" s="10">
+        <v>44211</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" ref="F14" ca="1" si="1">TODAY()-E14</f>
         <v>0</v>
       </c>
     </row>
@@ -12437,7 +12475,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>5.1972602739726028</v>
+        <v>5.2136986301369861</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12458,7 +12496,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1972602739726028</v>
+        <v>5.2136986301369861</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12479,7 +12517,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5753424657534243</v>
+        <v>4.5917808219178085</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12500,7 +12538,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>2.9452054794520546</v>
+        <v>2.9616438356164383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully published + submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="801">
   <si>
     <t>title</t>
   </si>
@@ -2415,6 +2415,18 @@
   </si>
   <si>
     <t>10.1016/S0140-6736(21)00189-6</t>
+  </si>
+  <si>
+    <t>Assessing polypharmacy in the older population: comparison of a self-reported and prescription based method</t>
+  </si>
+  <si>
+    <t>Pharmacoepidemiology and Drug Safety</t>
+  </si>
+  <si>
+    <t>Pharmacoepidemiol. Drug Saf.</t>
+  </si>
+  <si>
+    <t>Van der Heyden, Johan; Berete, Finaba; Renard, Françoise; Vanoverloop, Johan; Devleesschauwer, Brecht; De Ridder, Karin; Bruyère, Olivier</t>
   </si>
 </sst>
 </file>
@@ -2641,146 +2653,6 @@
   </cellStyles>
   <dxfs count="64">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2940,6 +2812,146 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2954,73 +2966,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U155" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U155" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:U155"/>
-  <sortState ref="A2:U153">
-    <sortCondition ref="K1:K153"/>
+  <sortState ref="A2:U155">
+    <sortCondition ref="K1:K155"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="61"/>
-    <tableColumn id="2" name="authors" dataDxfId="60"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="59"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="58"/>
-    <tableColumn id="6" name="year" dataDxfId="57"/>
-    <tableColumn id="4" name="volume" dataDxfId="56"/>
-    <tableColumn id="5" name="issue" dataDxfId="55"/>
-    <tableColumn id="7" name="eID" dataDxfId="54"/>
-    <tableColumn id="8" name="from" dataDxfId="53"/>
-    <tableColumn id="9" name="to" dataDxfId="52"/>
-    <tableColumn id="10" name="date" dataDxfId="51"/>
-    <tableColumn id="14" name="classification" dataDxfId="50"/>
-    <tableColumn id="12" name="IF" dataDxfId="49"/>
-    <tableColumn id="13" name="DOI" dataDxfId="48"/>
-    <tableColumn id="15" name="WoS" dataDxfId="47"/>
-    <tableColumn id="16" name="rank" dataDxfId="46"/>
-    <tableColumn id="17" name="quartile" dataDxfId="45"/>
-    <tableColumn id="18" name="category" dataDxfId="44"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="43"/>
-    <tableColumn id="20" name="SC" dataDxfId="42"/>
-    <tableColumn id="21" name="UGent" dataDxfId="41"/>
+    <tableColumn id="1" name="title" dataDxfId="47"/>
+    <tableColumn id="2" name="authors" dataDxfId="46"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
+    <tableColumn id="6" name="year" dataDxfId="43"/>
+    <tableColumn id="4" name="volume" dataDxfId="42"/>
+    <tableColumn id="5" name="issue" dataDxfId="41"/>
+    <tableColumn id="7" name="eID" dataDxfId="40"/>
+    <tableColumn id="8" name="from" dataDxfId="39"/>
+    <tableColumn id="9" name="to" dataDxfId="38"/>
+    <tableColumn id="10" name="date" dataDxfId="37"/>
+    <tableColumn id="14" name="classification" dataDxfId="36"/>
+    <tableColumn id="12" name="IF" dataDxfId="35"/>
+    <tableColumn id="13" name="DOI" dataDxfId="34"/>
+    <tableColumn id="15" name="WoS" dataDxfId="33"/>
+    <tableColumn id="16" name="rank" dataDxfId="32"/>
+    <tableColumn id="17" name="quartile" dataDxfId="31"/>
+    <tableColumn id="18" name="category" dataDxfId="30"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
+    <tableColumn id="20" name="SC" dataDxfId="28"/>
+    <tableColumn id="21" name="UGent" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J8" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J8" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:J8"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="39"/>
-    <tableColumn id="2" name="authors" dataDxfId="38"/>
-    <tableColumn id="3" name="editors" dataDxfId="37"/>
-    <tableColumn id="11" name="book" dataDxfId="36"/>
-    <tableColumn id="6" name="year" dataDxfId="35"/>
-    <tableColumn id="8" name="from" dataDxfId="34"/>
-    <tableColumn id="9" name="to" dataDxfId="33"/>
-    <tableColumn id="10" name="date" dataDxfId="32"/>
-    <tableColumn id="12" name="IF" dataDxfId="31"/>
-    <tableColumn id="13" name="DOI" dataDxfId="30"/>
+    <tableColumn id="1" name="title" dataDxfId="25"/>
+    <tableColumn id="2" name="authors" dataDxfId="24"/>
+    <tableColumn id="3" name="editors" dataDxfId="23"/>
+    <tableColumn id="11" name="book" dataDxfId="22"/>
+    <tableColumn id="6" name="year" dataDxfId="21"/>
+    <tableColumn id="8" name="from" dataDxfId="20"/>
+    <tableColumn id="9" name="to" dataDxfId="19"/>
+    <tableColumn id="10" name="date" dataDxfId="18"/>
+    <tableColumn id="12" name="IF" dataDxfId="17"/>
+    <tableColumn id="13" name="DOI" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:F13"/>
-  <sortState ref="A2:F10">
-    <sortCondition descending="1" ref="F1:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F14"/>
+  <sortState ref="A2:F14">
+    <sortCondition descending="1" ref="F1:F14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="27"/>
-    <tableColumn id="2" name="authors" dataDxfId="26"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="25"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="24"/>
-    <tableColumn id="10" name="date" dataDxfId="23"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="22">
+    <tableColumn id="1" name="title" dataDxfId="13"/>
+    <tableColumn id="2" name="authors" dataDxfId="12"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
+    <tableColumn id="10" name="date" dataDxfId="9"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="8">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3029,18 +3041,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="19"/>
-    <tableColumn id="2" name="authors" dataDxfId="18"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="17"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="16"/>
-    <tableColumn id="10" name="date" dataDxfId="15"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="14">
+    <tableColumn id="1" name="title" dataDxfId="5"/>
+    <tableColumn id="2" name="authors" dataDxfId="4"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
+    <tableColumn id="10" name="date" dataDxfId="1"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="0">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3337,8 +3349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView topLeftCell="A123" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11541,47 +11553,47 @@
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A149" s="13" t="s">
-        <v>751</v>
-      </c>
-      <c r="B149" s="13" t="s">
-        <v>719</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>752</v>
-      </c>
-      <c r="D149" s="13" t="s">
-        <v>753</v>
-      </c>
-      <c r="E149" s="14">
+      <c r="A149" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>769</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>770</v>
+      </c>
+      <c r="E149" s="18">
         <v>2021</v>
       </c>
-      <c r="F149" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G149" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H149" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I149" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J149" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K149" s="33">
-        <v>44562</v>
-      </c>
-      <c r="L149" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="M149" s="27"/>
-      <c r="N149" s="28" t="s">
-        <v>754</v>
-      </c>
-      <c r="O149" s="29"/>
+      <c r="F149" s="18">
+        <v>39</v>
+      </c>
+      <c r="G149" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H149" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I149" s="18">
+        <v>152</v>
+      </c>
+      <c r="J149" s="18">
+        <v>159</v>
+      </c>
+      <c r="K149" s="10">
+        <v>44348</v>
+      </c>
+      <c r="L149" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="M149" s="11"/>
+      <c r="N149" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="O149" s="7"/>
       <c r="P149" s="24"/>
       <c r="Q149" s="25"/>
       <c r="R149" s="7"/>
@@ -11593,16 +11605,16 @@
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
-        <v>652</v>
+        <v>751</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>653</v>
+        <v>719</v>
       </c>
       <c r="C150" s="13" t="s">
-        <v>81</v>
+        <v>752</v>
       </c>
       <c r="D150" s="13" t="s">
-        <v>82</v>
+        <v>753</v>
       </c>
       <c r="E150" s="14">
         <v>2021</v>
@@ -11623,14 +11635,14 @@
         <v>14</v>
       </c>
       <c r="K150" s="33">
-        <v>44563</v>
+        <v>44562</v>
       </c>
       <c r="L150" s="41" t="s">
         <v>274</v>
       </c>
       <c r="M150" s="27"/>
       <c r="N150" s="28" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O150" s="29"/>
       <c r="P150" s="24"/>
@@ -11638,20 +11650,22 @@
       <c r="R150" s="7"/>
       <c r="S150" s="7"/>
       <c r="T150" s="7"/>
-      <c r="U150" s="7"/>
+      <c r="U150" s="7" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
-        <v>726</v>
+        <v>652</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>727</v>
+        <v>653</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>728</v>
+        <v>81</v>
       </c>
       <c r="D151" s="13" t="s">
-        <v>729</v>
+        <v>82</v>
       </c>
       <c r="E151" s="14">
         <v>2021</v>
@@ -11672,14 +11686,14 @@
         <v>14</v>
       </c>
       <c r="K151" s="33">
-        <v>44564</v>
+        <v>44563</v>
       </c>
       <c r="L151" s="41" t="s">
         <v>274</v>
       </c>
       <c r="M151" s="27"/>
       <c r="N151" s="28" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="O151" s="29"/>
       <c r="P151" s="24"/>
@@ -11691,44 +11705,44 @@
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
-        <v>763</v>
+        <v>726</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>764</v>
+        <v>727</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>765</v>
+        <v>728</v>
       </c>
       <c r="D152" s="13" t="s">
-        <v>766</v>
+        <v>729</v>
       </c>
       <c r="E152" s="14">
         <v>2021</v>
       </c>
-      <c r="F152" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G152" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H152" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I152" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="J152" s="47" t="s">
+      <c r="F152" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G152" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H152" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I152" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J152" s="39" t="s">
         <v>14</v>
       </c>
       <c r="K152" s="33">
-        <v>44565</v>
-      </c>
-      <c r="L152" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="M152" s="49"/>
-      <c r="N152" s="48" t="s">
-        <v>767</v>
+        <v>44564</v>
+      </c>
+      <c r="L152" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="M152" s="27"/>
+      <c r="N152" s="28" t="s">
+        <v>762</v>
       </c>
       <c r="O152" s="29"/>
       <c r="P152" s="24"/>
@@ -11736,22 +11750,20 @@
       <c r="R152" s="7"/>
       <c r="S152" s="7"/>
       <c r="T152" s="7"/>
-      <c r="U152" s="7" t="s">
-        <v>605</v>
-      </c>
+      <c r="U152" s="7"/>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
-        <v>709</v>
+        <v>763</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>710</v>
+        <v>764</v>
       </c>
       <c r="C153" s="13" t="s">
-        <v>260</v>
+        <v>765</v>
       </c>
       <c r="D153" s="13" t="s">
-        <v>263</v>
+        <v>766</v>
       </c>
       <c r="E153" s="14">
         <v>2021</v>
@@ -11772,14 +11784,14 @@
         <v>14</v>
       </c>
       <c r="K153" s="33">
-        <v>44566</v>
+        <v>44565</v>
       </c>
       <c r="L153" s="33" t="s">
         <v>274</v>
       </c>
       <c r="M153" s="49"/>
       <c r="N153" s="48" t="s">
-        <v>786</v>
+        <v>767</v>
       </c>
       <c r="O153" s="29"/>
       <c r="P153" s="24"/>
@@ -11787,20 +11799,22 @@
       <c r="R153" s="7"/>
       <c r="S153" s="7"/>
       <c r="T153" s="7"/>
-      <c r="U153" s="7"/>
+      <c r="U153" s="7" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
-        <v>768</v>
+        <v>709</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>771</v>
+        <v>710</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>769</v>
+        <v>260</v>
       </c>
       <c r="D154" s="13" t="s">
-        <v>770</v>
+        <v>263</v>
       </c>
       <c r="E154" s="14">
         <v>2021</v>
@@ -11821,14 +11835,14 @@
         <v>14</v>
       </c>
       <c r="K154" s="33">
-        <v>44567</v>
+        <v>44566</v>
       </c>
       <c r="L154" s="33" t="s">
         <v>274</v>
       </c>
       <c r="M154" s="49"/>
       <c r="N154" s="48" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="O154" s="29"/>
       <c r="P154" s="24"/>
@@ -11895,58 +11909,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S136:U146 S148:U1048576">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12230,9 +12244,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12279,8 +12293,8 @@
         <v>43861</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F13" ca="1" si="0">TODAY()-E2</f>
-        <v>371</v>
+        <f ca="1">TODAY()-E2</f>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12300,8 +12314,8 @@
         <v>43942</v>
       </c>
       <c r="F3" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>290</v>
+        <f ca="1">TODAY()-E3</f>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12321,8 +12335,8 @@
         <v>43972</v>
       </c>
       <c r="F4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>260</v>
+        <f ca="1">TODAY()-E4</f>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12342,8 +12356,8 @@
         <v>44000</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>232</v>
+        <f ca="1">TODAY()-E5</f>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -12363,8 +12377,8 @@
         <v>44006</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>226</v>
+        <f ca="1">TODAY()-E6</f>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -12384,8 +12398,8 @@
         <v>44078</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <f ca="1">TODAY()-E7</f>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -12405,8 +12419,8 @@
         <v>44123</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <f ca="1">TODAY()-E8</f>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -12426,8 +12440,8 @@
         <v>44181</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <f ca="1">TODAY()-E9</f>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -12447,8 +12461,8 @@
         <v>44191</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <f ca="1">TODAY()-E10</f>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -12468,50 +12482,71 @@
         <v>44192</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <f ca="1">TODAY()-E11</f>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="E12" s="10">
+        <v>44197</v>
+      </c>
+      <c r="F12" s="12">
+        <f ca="1">TODAY()-E12</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>783</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>784</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E13" s="10">
         <v>44205</v>
       </c>
-      <c r="F12" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="F13" s="12">
+        <f ca="1">TODAY()-E13</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>791</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E14" s="10">
         <v>44224</v>
       </c>
-      <c r="F13" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+      <c r="F14" s="12">
+        <f ca="1">TODAY()-E14</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -12576,7 +12611,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>5.2712328767123289</v>
+        <v>5.2767123287671236</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12597,7 +12632,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2712328767123289</v>
+        <v>5.2767123287671236</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12618,7 +12653,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6493150684931503</v>
+        <v>4.6547945205479451</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12639,7 +12674,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>3.0191780821917806</v>
+        <v>3.0246575342465754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new published and submitted
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="838">
   <si>
     <t>title</t>
   </si>
@@ -2523,6 +2523,21 @@
   </si>
   <si>
     <t>Kayiba Kalenda, Nadine; Yobi, Doudou Malekita; Devleesschauwer, Brecht; Mvumbi, Dieudonné Makaba; Kabututu, Pius Zakayi; Losimba, Joris Likwela; Azama, Lydie Kalindula; De Mol, Patrick; Hayette, Marrie-Pièrre; Mvumbi, Georges Lelo; Dikassa, Paul Lusamba; Beutels, Philippe; Rosas-Aguirre, Angel; Speybroeck, Niko</t>
+  </si>
+  <si>
+    <t>10.1186/s12936-021-03789-w</t>
+  </si>
+  <si>
+    <t>Estimating the direct Covid-19 disability-adjusted life years impact on the Malta population for the first full year</t>
+  </si>
+  <si>
+    <t>Journal of Public Health</t>
+  </si>
+  <si>
+    <t>J. Public Health</t>
+  </si>
+  <si>
+    <t>Cuschieri, Sarah; Calleja, Neville; Devleesschauwer, Brecht; Wyper, Grant M A</t>
   </si>
 </sst>
 </file>
@@ -3064,8 +3079,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U163" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:U163"/>
-  <sortState ref="A2:U159">
-    <sortCondition ref="K1:K159"/>
+  <sortState ref="A2:U163">
+    <sortCondition ref="K1:K163"/>
   </sortState>
   <tableColumns count="21">
     <tableColumn id="1" name="title" dataDxfId="47"/>
@@ -3117,8 +3132,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F15"/>
   <sortState ref="A2:F15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
@@ -3445,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView topLeftCell="A129" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12006,47 +12021,47 @@
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A156" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="B156" s="13" t="s">
-        <v>714</v>
-      </c>
-      <c r="C156" s="13" t="s">
-        <v>746</v>
-      </c>
-      <c r="D156" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="E156" s="14">
+      <c r="A156" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="E156" s="18">
         <v>2021</v>
       </c>
-      <c r="F156" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G156" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H156" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I156" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J156" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K156" s="33">
-        <v>44562</v>
-      </c>
-      <c r="L156" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="M156" s="27"/>
-      <c r="N156" s="28" t="s">
-        <v>748</v>
-      </c>
-      <c r="O156" s="29"/>
+      <c r="F156" s="18">
+        <v>20</v>
+      </c>
+      <c r="G156" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H156" s="18">
+        <v>260</v>
+      </c>
+      <c r="I156" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J156" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K156" s="10">
+        <v>44356</v>
+      </c>
+      <c r="L156" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="M156" s="11"/>
+      <c r="N156" s="19" t="s">
+        <v>833</v>
+      </c>
+      <c r="O156" s="7"/>
       <c r="P156" s="24"/>
       <c r="Q156" s="25"/>
       <c r="R156" s="7"/>
@@ -12058,16 +12073,16 @@
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
-        <v>721</v>
+        <v>745</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>723</v>
+        <v>746</v>
       </c>
       <c r="D157" s="13" t="s">
-        <v>724</v>
+        <v>747</v>
       </c>
       <c r="E157" s="14">
         <v>2021</v>
@@ -12088,14 +12103,14 @@
         <v>14</v>
       </c>
       <c r="K157" s="33">
-        <v>44563</v>
+        <v>44562</v>
       </c>
       <c r="L157" s="41" t="s">
         <v>274</v>
       </c>
       <c r="M157" s="27"/>
       <c r="N157" s="28" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="O157" s="29"/>
       <c r="P157" s="24"/>
@@ -12103,48 +12118,50 @@
       <c r="R157" s="7"/>
       <c r="S157" s="7"/>
       <c r="T157" s="7"/>
-      <c r="U157" s="7"/>
+      <c r="U157" s="7" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
-        <v>704</v>
+        <v>721</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>705</v>
+        <v>722</v>
       </c>
       <c r="C158" s="13" t="s">
-        <v>260</v>
+        <v>723</v>
       </c>
       <c r="D158" s="13" t="s">
-        <v>263</v>
+        <v>724</v>
       </c>
       <c r="E158" s="14">
         <v>2021</v>
       </c>
-      <c r="F158" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G158" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H158" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I158" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="J158" s="47" t="s">
+      <c r="F158" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G158" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H158" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I158" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J158" s="39" t="s">
         <v>14</v>
       </c>
       <c r="K158" s="33">
-        <v>44564</v>
-      </c>
-      <c r="L158" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="M158" s="49"/>
-      <c r="N158" s="48" t="s">
-        <v>780</v>
+        <v>44563</v>
+      </c>
+      <c r="L158" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="M158" s="27"/>
+      <c r="N158" s="28" t="s">
+        <v>756</v>
       </c>
       <c r="O158" s="29"/>
       <c r="P158" s="24"/>
@@ -12156,16 +12173,16 @@
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
-        <v>806</v>
+        <v>704</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>807</v>
+        <v>705</v>
       </c>
       <c r="C159" s="13" t="s">
-        <v>339</v>
+        <v>260</v>
       </c>
       <c r="D159" s="13" t="s">
-        <v>340</v>
+        <v>263</v>
       </c>
       <c r="E159" s="14">
         <v>2021</v>
@@ -12186,13 +12203,15 @@
         <v>14</v>
       </c>
       <c r="K159" s="33">
-        <v>44565</v>
+        <v>44564</v>
       </c>
       <c r="L159" s="33" t="s">
         <v>274</v>
       </c>
       <c r="M159" s="49"/>
-      <c r="N159" s="48"/>
+      <c r="N159" s="48" t="s">
+        <v>780</v>
+      </c>
       <c r="O159" s="29"/>
       <c r="P159" s="24"/>
       <c r="Q159" s="25"/>
@@ -12203,16 +12222,16 @@
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>800</v>
+        <v>806</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>801</v>
+        <v>807</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>799</v>
+        <v>339</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>802</v>
+        <v>340</v>
       </c>
       <c r="E160" s="14">
         <v>2021</v>
@@ -12233,7 +12252,7 @@
         <v>14</v>
       </c>
       <c r="K160" s="33">
-        <v>44566</v>
+        <v>44565</v>
       </c>
       <c r="L160" s="33" t="s">
         <v>274</v>
@@ -12250,16 +12269,16 @@
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>827</v>
+        <v>800</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>828</v>
+        <v>801</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>830</v>
+        <v>799</v>
       </c>
       <c r="D161" s="13" t="s">
-        <v>829</v>
+        <v>802</v>
       </c>
       <c r="E161" s="14">
         <v>2021</v>
@@ -12280,7 +12299,7 @@
         <v>14</v>
       </c>
       <c r="K161" s="33">
-        <v>44567</v>
+        <v>44566</v>
       </c>
       <c r="L161" s="33" t="s">
         <v>274</v>
@@ -12297,16 +12316,16 @@
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>711</v>
+        <v>827</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>712</v>
+        <v>828</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>268</v>
+        <v>830</v>
       </c>
       <c r="D162" s="13" t="s">
-        <v>269</v>
+        <v>829</v>
       </c>
       <c r="E162" s="14">
         <v>2021</v>
@@ -12327,7 +12346,7 @@
         <v>14</v>
       </c>
       <c r="K162" s="33">
-        <v>44568</v>
+        <v>44567</v>
       </c>
       <c r="L162" s="33" t="s">
         <v>274</v>
@@ -12344,16 +12363,16 @@
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>831</v>
+        <v>711</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>832</v>
+        <v>712</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>381</v>
+        <v>268</v>
       </c>
       <c r="D163" s="13" t="s">
-        <v>382</v>
+        <v>269</v>
       </c>
       <c r="E163" s="14">
         <v>2021</v>
@@ -12374,7 +12393,7 @@
         <v>14</v>
       </c>
       <c r="K163" s="33">
-        <v>44569</v>
+        <v>44568</v>
       </c>
       <c r="L163" s="33" t="s">
         <v>274</v>
@@ -12748,9 +12767,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12797,8 +12816,8 @@
         <v>44000</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F14" ca="1" si="0">TODAY()-E2</f>
-        <v>346</v>
+        <f t="shared" ref="F2:F15" ca="1" si="0">TODAY()-E2</f>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12819,7 +12838,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12840,7 +12859,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12861,7 +12880,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -12882,7 +12901,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -12903,7 +12922,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -12924,7 +12943,7 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -12945,7 +12964,7 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -12966,7 +12985,7 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -12987,7 +13006,7 @@
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -13008,7 +13027,7 @@
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -13029,7 +13048,7 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -13050,7 +13069,28 @@
       </c>
       <c r="F14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="E15" s="10">
+        <v>44356</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -13115,7 +13155,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>5.5835616438356164</v>
+        <v>5.6136986301369864</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -13136,7 +13176,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5835616438356164</v>
+        <v>5.6136986301369864</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -13157,7 +13197,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9616438356164387</v>
+        <v>4.9917808219178079</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -13178,7 +13218,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>3.3315068493150686</v>
+        <v>3.3616438356164382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
accepted and fully published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="839">
   <si>
     <t>title</t>
   </si>
@@ -2492,15 +2492,9 @@
     <t>Consumer and food product determinants of food wasting – a case study on chicken meat</t>
   </si>
   <si>
-    <t>Sustainable Production and Consumption</t>
-  </si>
-  <si>
     <t>Cooreman-Algoed, Margot; Minnens, Fien; Boone, Lieselot; Botterman, Kyara; Taelman, Sue Ellen; Verbeke, Wim; Devleesschauwer, Brecht; Hung, Yung; Dewulf, Jo</t>
   </si>
   <si>
-    <t>Sustain. Prod. Consum.</t>
-  </si>
-  <si>
     <t>10.1186/s13690-021-00599-z</t>
   </si>
   <si>
@@ -2538,6 +2532,15 @@
   </si>
   <si>
     <t>Cuschieri, Sarah; Calleja, Neville; Devleesschauwer, Brecht; Wyper, Grant M A</t>
+  </si>
+  <si>
+    <t>Sustainability</t>
+  </si>
+  <si>
+    <t>10.3390/su13137027</t>
+  </si>
+  <si>
+    <t>10.1186/s13690-021-00620-5</t>
   </si>
 </sst>
 </file>
@@ -2764,6 +2767,146 @@
   </cellStyles>
   <dxfs count="64">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2923,146 +3066,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -3077,73 +3080,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U163" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:U163"/>
-  <sortState ref="A2:U163">
-    <sortCondition ref="K1:K163"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U164" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A1:U164"/>
+  <sortState ref="A2:U164">
+    <sortCondition ref="K1:K164"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="47"/>
-    <tableColumn id="2" name="authors" dataDxfId="46"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
-    <tableColumn id="6" name="year" dataDxfId="43"/>
-    <tableColumn id="4" name="volume" dataDxfId="42"/>
-    <tableColumn id="5" name="issue" dataDxfId="41"/>
-    <tableColumn id="7" name="eID" dataDxfId="40"/>
-    <tableColumn id="8" name="from" dataDxfId="39"/>
-    <tableColumn id="9" name="to" dataDxfId="38"/>
-    <tableColumn id="10" name="date" dataDxfId="37"/>
-    <tableColumn id="14" name="classification" dataDxfId="36"/>
-    <tableColumn id="12" name="IF" dataDxfId="35"/>
-    <tableColumn id="13" name="DOI" dataDxfId="34"/>
-    <tableColumn id="15" name="WoS" dataDxfId="33"/>
-    <tableColumn id="16" name="rank" dataDxfId="32"/>
-    <tableColumn id="17" name="quartile" dataDxfId="31"/>
-    <tableColumn id="18" name="category" dataDxfId="30"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
-    <tableColumn id="20" name="SC" dataDxfId="28"/>
-    <tableColumn id="21" name="UGent" dataDxfId="27"/>
+    <tableColumn id="1" name="title" dataDxfId="61"/>
+    <tableColumn id="2" name="authors" dataDxfId="60"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="59"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="58"/>
+    <tableColumn id="6" name="year" dataDxfId="57"/>
+    <tableColumn id="4" name="volume" dataDxfId="56"/>
+    <tableColumn id="5" name="issue" dataDxfId="55"/>
+    <tableColumn id="7" name="eID" dataDxfId="54"/>
+    <tableColumn id="8" name="from" dataDxfId="53"/>
+    <tableColumn id="9" name="to" dataDxfId="52"/>
+    <tableColumn id="10" name="date" dataDxfId="51"/>
+    <tableColumn id="14" name="classification" dataDxfId="50"/>
+    <tableColumn id="12" name="IF" dataDxfId="49"/>
+    <tableColumn id="13" name="DOI" dataDxfId="48"/>
+    <tableColumn id="15" name="WoS" dataDxfId="47"/>
+    <tableColumn id="16" name="rank" dataDxfId="46"/>
+    <tableColumn id="17" name="quartile" dataDxfId="45"/>
+    <tableColumn id="18" name="category" dataDxfId="44"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="43"/>
+    <tableColumn id="20" name="SC" dataDxfId="42"/>
+    <tableColumn id="21" name="UGent" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J9" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J9" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A1:J9"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="25"/>
-    <tableColumn id="2" name="authors" dataDxfId="24"/>
-    <tableColumn id="3" name="editors" dataDxfId="23"/>
-    <tableColumn id="11" name="book" dataDxfId="22"/>
-    <tableColumn id="6" name="year" dataDxfId="21"/>
-    <tableColumn id="8" name="from" dataDxfId="20"/>
-    <tableColumn id="9" name="to" dataDxfId="19"/>
-    <tableColumn id="10" name="date" dataDxfId="18"/>
-    <tableColumn id="12" name="IF" dataDxfId="17"/>
-    <tableColumn id="13" name="DOI" dataDxfId="16"/>
+    <tableColumn id="1" name="title" dataDxfId="39"/>
+    <tableColumn id="2" name="authors" dataDxfId="38"/>
+    <tableColumn id="3" name="editors" dataDxfId="37"/>
+    <tableColumn id="11" name="book" dataDxfId="36"/>
+    <tableColumn id="6" name="year" dataDxfId="35"/>
+    <tableColumn id="8" name="from" dataDxfId="34"/>
+    <tableColumn id="9" name="to" dataDxfId="33"/>
+    <tableColumn id="10" name="date" dataDxfId="32"/>
+    <tableColumn id="12" name="IF" dataDxfId="31"/>
+    <tableColumn id="13" name="DOI" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F14" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:F14"/>
   <sortState ref="A2:F15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="13"/>
-    <tableColumn id="2" name="authors" dataDxfId="12"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
-    <tableColumn id="10" name="date" dataDxfId="9"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="8">
+    <tableColumn id="1" name="title" dataDxfId="27"/>
+    <tableColumn id="2" name="authors" dataDxfId="26"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="25"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="24"/>
+    <tableColumn id="10" name="date" dataDxfId="23"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="22">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3152,18 +3155,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="5"/>
-    <tableColumn id="2" name="authors" dataDxfId="4"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
-    <tableColumn id="10" name="date" dataDxfId="1"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="0">
+    <tableColumn id="1" name="title" dataDxfId="19"/>
+    <tableColumn id="2" name="authors" dataDxfId="18"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="17"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="16"/>
+    <tableColumn id="10" name="date" dataDxfId="15"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="14">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3458,10 +3461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U163"/>
+  <dimension ref="A1:U164"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11920,7 +11923,7 @@
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B154" s="7" t="s">
         <v>694</v>
@@ -11957,7 +11960,7 @@
       </c>
       <c r="M154" s="11"/>
       <c r="N154" s="19" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="O154" s="7"/>
       <c r="P154" s="24"/>
@@ -12022,10 +12025,10 @@
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>381</v>
@@ -12059,7 +12062,7 @@
       </c>
       <c r="M156" s="11"/>
       <c r="N156" s="19" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="O156" s="7"/>
       <c r="P156" s="24"/>
@@ -12072,47 +12075,47 @@
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A157" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="B157" s="13" t="s">
-        <v>714</v>
-      </c>
-      <c r="C157" s="13" t="s">
-        <v>746</v>
-      </c>
-      <c r="D157" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="E157" s="14">
+      <c r="A157" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E157" s="18">
         <v>2021</v>
       </c>
-      <c r="F157" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G157" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H157" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I157" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J157" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K157" s="33">
-        <v>44562</v>
-      </c>
-      <c r="L157" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="M157" s="27"/>
-      <c r="N157" s="28" t="s">
-        <v>748</v>
-      </c>
-      <c r="O157" s="29"/>
+      <c r="F157" s="18">
+        <v>79</v>
+      </c>
+      <c r="G157" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H157" s="18">
+        <v>112</v>
+      </c>
+      <c r="I157" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J157" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K157" s="10">
+        <v>44370</v>
+      </c>
+      <c r="L157" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="M157" s="11"/>
+      <c r="N157" s="19" t="s">
+        <v>838</v>
+      </c>
+      <c r="O157" s="7"/>
       <c r="P157" s="24"/>
       <c r="Q157" s="25"/>
       <c r="R157" s="7"/>
@@ -12123,47 +12126,47 @@
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A158" s="13" t="s">
-        <v>721</v>
-      </c>
-      <c r="B158" s="13" t="s">
-        <v>722</v>
-      </c>
-      <c r="C158" s="13" t="s">
-        <v>723</v>
-      </c>
-      <c r="D158" s="13" t="s">
-        <v>724</v>
-      </c>
-      <c r="E158" s="14">
+      <c r="A158" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="D158" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="E158" s="18">
         <v>2021</v>
       </c>
-      <c r="F158" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G158" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H158" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I158" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J158" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K158" s="33">
-        <v>44563</v>
-      </c>
-      <c r="L158" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="M158" s="27"/>
-      <c r="N158" s="28" t="s">
-        <v>756</v>
-      </c>
-      <c r="O158" s="29"/>
+      <c r="F158" s="18">
+        <v>13</v>
+      </c>
+      <c r="G158" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H158" s="18">
+        <v>7027</v>
+      </c>
+      <c r="I158" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J158" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K158" s="46">
+        <v>44370</v>
+      </c>
+      <c r="L158" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="M158" s="11"/>
+      <c r="N158" s="19" t="s">
+        <v>837</v>
+      </c>
+      <c r="O158" s="7"/>
       <c r="P158" s="24"/>
       <c r="Q158" s="25"/>
       <c r="R158" s="7"/>
@@ -12173,44 +12176,44 @@
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
-        <v>704</v>
+        <v>745</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="C159" s="13" t="s">
-        <v>260</v>
+        <v>746</v>
       </c>
       <c r="D159" s="13" t="s">
-        <v>263</v>
+        <v>747</v>
       </c>
       <c r="E159" s="14">
         <v>2021</v>
       </c>
-      <c r="F159" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G159" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H159" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I159" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="J159" s="47" t="s">
+      <c r="F159" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G159" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H159" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I159" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J159" s="39" t="s">
         <v>14</v>
       </c>
       <c r="K159" s="33">
-        <v>44564</v>
-      </c>
-      <c r="L159" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="M159" s="49"/>
-      <c r="N159" s="48" t="s">
-        <v>780</v>
+        <v>44562</v>
+      </c>
+      <c r="L159" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="M159" s="27"/>
+      <c r="N159" s="28" t="s">
+        <v>748</v>
       </c>
       <c r="O159" s="29"/>
       <c r="P159" s="24"/>
@@ -12218,47 +12221,51 @@
       <c r="R159" s="7"/>
       <c r="S159" s="7"/>
       <c r="T159" s="7"/>
-      <c r="U159" s="7"/>
+      <c r="U159" s="7" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>806</v>
+        <v>721</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>807</v>
+        <v>722</v>
       </c>
       <c r="C160" s="13" t="s">
-        <v>339</v>
+        <v>723</v>
       </c>
       <c r="D160" s="13" t="s">
-        <v>340</v>
+        <v>724</v>
       </c>
       <c r="E160" s="14">
         <v>2021</v>
       </c>
-      <c r="F160" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="G160" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H160" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I160" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="J160" s="47" t="s">
+      <c r="F160" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H160" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I160" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J160" s="39" t="s">
         <v>14</v>
       </c>
       <c r="K160" s="33">
-        <v>44565</v>
-      </c>
-      <c r="L160" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="M160" s="49"/>
-      <c r="N160" s="48"/>
+        <v>44563</v>
+      </c>
+      <c r="L160" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="M160" s="27"/>
+      <c r="N160" s="28" t="s">
+        <v>756</v>
+      </c>
       <c r="O160" s="29"/>
       <c r="P160" s="24"/>
       <c r="Q160" s="25"/>
@@ -12269,16 +12276,16 @@
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>800</v>
+        <v>704</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>801</v>
+        <v>705</v>
       </c>
       <c r="C161" s="13" t="s">
-        <v>799</v>
+        <v>260</v>
       </c>
       <c r="D161" s="13" t="s">
-        <v>802</v>
+        <v>263</v>
       </c>
       <c r="E161" s="14">
         <v>2021</v>
@@ -12299,13 +12306,15 @@
         <v>14</v>
       </c>
       <c r="K161" s="33">
-        <v>44566</v>
+        <v>44564</v>
       </c>
       <c r="L161" s="33" t="s">
         <v>274</v>
       </c>
       <c r="M161" s="49"/>
-      <c r="N161" s="48"/>
+      <c r="N161" s="48" t="s">
+        <v>780</v>
+      </c>
       <c r="O161" s="29"/>
       <c r="P161" s="24"/>
       <c r="Q161" s="25"/>
@@ -12316,16 +12325,16 @@
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>827</v>
+        <v>806</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>828</v>
+        <v>807</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>830</v>
+        <v>339</v>
       </c>
       <c r="D162" s="13" t="s">
-        <v>829</v>
+        <v>340</v>
       </c>
       <c r="E162" s="14">
         <v>2021</v>
@@ -12346,7 +12355,7 @@
         <v>14</v>
       </c>
       <c r="K162" s="33">
-        <v>44567</v>
+        <v>44565</v>
       </c>
       <c r="L162" s="33" t="s">
         <v>274</v>
@@ -12363,16 +12372,16 @@
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>711</v>
+        <v>800</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>712</v>
+        <v>801</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>268</v>
+        <v>799</v>
       </c>
       <c r="D163" s="13" t="s">
-        <v>269</v>
+        <v>802</v>
       </c>
       <c r="E163" s="14">
         <v>2021</v>
@@ -12393,7 +12402,7 @@
         <v>14</v>
       </c>
       <c r="K163" s="33">
-        <v>44568</v>
+        <v>44566</v>
       </c>
       <c r="L163" s="33" t="s">
         <v>274</v>
@@ -12408,60 +12417,107 @@
       <c r="T163" s="7"/>
       <c r="U163" s="7"/>
     </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A164" s="13" t="s">
+        <v>825</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>826</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>828</v>
+      </c>
+      <c r="D164" s="13" t="s">
+        <v>827</v>
+      </c>
+      <c r="E164" s="14">
+        <v>2021</v>
+      </c>
+      <c r="F164" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G164" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="H164" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I164" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J164" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="K164" s="33">
+        <v>44567</v>
+      </c>
+      <c r="L164" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="M164" s="49"/>
+      <c r="N164" s="48"/>
+      <c r="O164" s="29"/>
+      <c r="P164" s="24"/>
+      <c r="Q164" s="25"/>
+      <c r="R164" s="7"/>
+      <c r="S164" s="7"/>
+      <c r="T164" s="7"/>
+      <c r="U164" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S136:U146 S148:U1048576">
-    <cfRule type="cellIs" dxfId="63" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12767,9 +12823,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12816,8 +12872,8 @@
         <v>44000</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F15" ca="1" si="0">TODAY()-E2</f>
-        <v>357</v>
+        <f ca="1">TODAY()-E2</f>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -12837,8 +12893,8 @@
         <v>44181</v>
       </c>
       <c r="F3" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <f ca="1">TODAY()-E3</f>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -12858,8 +12914,8 @@
         <v>44191</v>
       </c>
       <c r="F4" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>166</v>
+        <f ca="1">TODAY()-E4</f>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -12879,8 +12935,8 @@
         <v>44192</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <f ca="1">TODAY()-E5</f>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -12900,8 +12956,8 @@
         <v>44197</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <f ca="1">TODAY()-E6</f>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -12921,8 +12977,8 @@
         <v>44205</v>
       </c>
       <c r="F7" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>152</v>
+        <f ca="1">TODAY()-E7</f>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -12942,8 +12998,8 @@
         <v>44242</v>
       </c>
       <c r="F8" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>115</v>
+        <f ca="1">TODAY()-E8</f>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -12963,8 +13019,8 @@
         <v>44243</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <f ca="1">TODAY()-E9</f>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -12984,8 +13040,8 @@
         <v>44246</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>111</v>
+        <f ca="1">TODAY()-E10</f>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -13005,8 +13061,8 @@
         <v>44277</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <f ca="1">TODAY()-E11</f>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -13026,8 +13082,8 @@
         <v>44281</v>
       </c>
       <c r="F12" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <f ca="1">TODAY()-E12</f>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -13047,50 +13103,29 @@
         <v>44306</v>
       </c>
       <c r="F13" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <f ca="1">TODAY()-E13</f>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>821</v>
+        <v>832</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>823</v>
+        <v>835</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>822</v>
+        <v>833</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
       <c r="E14" s="10">
-        <v>44309</v>
+        <v>44356</v>
       </c>
       <c r="F14" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>837</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="E15" s="10">
-        <v>44356</v>
-      </c>
-      <c r="F15" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f ca="1">TODAY()-E14</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -13155,7 +13190,7 @@
       </c>
       <c r="F2" s="44">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>5.6136986301369864</v>
+        <v>5.6493150684931503</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -13176,7 +13211,7 @@
       </c>
       <c r="F3" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6136986301369864</v>
+        <v>5.6493150684931503</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -13197,7 +13232,7 @@
       </c>
       <c r="F4" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9917808219178079</v>
+        <v>5.0273972602739727</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -13218,7 +13253,7 @@
       </c>
       <c r="F5" s="44">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>3.3616438356164382</v>
+        <v>3.3972602739726026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new accepted and fully published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="901">
   <si>
     <t>title</t>
   </si>
@@ -2432,9 +2432,6 @@
     <t>10.3389/ijph.2021.619011</t>
   </si>
   <si>
-    <t>Setting up an ad hoc COVID-19 mortality surveillance in Belgium during the first wave of the epidemic, March 1st - June 21st 2020</t>
-  </si>
-  <si>
     <t>Renard, Françoise; Scohy, Aline; Van der Heyden, Johan; Peeters, Ilse; Dequeker, Sara; Vandael, Eline; Van Goethem, Nina; Dubourg, Dominique; De Viron, Louise; Kongs, Anne; Hammami, Naïma; Devleesschauwer, Brecht; Sasse, André; Rebolledo Gonzalez, Javiera; Bustos Sierra, Natalia</t>
   </si>
   <si>
@@ -2712,6 +2709,24 @@
   </si>
   <si>
     <t>Dupont, Fabian; Trevisan, Chiara; Kaducu, Joyce Moriku; Ovuga, Emilio; Schmidt, Veronika; Winkler, Andrea S; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Establishing an ad hoc COVID-19 mortality surveillance during the first epidemic wave in Belgium, 1 March to 21 June 2020</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>pii=2001402</t>
+  </si>
+  <si>
+    <t>10.2807/1560-7917.ES.2021.26.48.2001402</t>
+  </si>
+  <si>
+    <t>The association between area deprivation and COVID-19 incidence: a municipality-level spatio-temporal study in Belgium, 2020-2021</t>
+  </si>
+  <si>
+    <t>Meurisse, Marjan; Lajot, Adrien; Devleesschauwer, Brecht; Van Cauteren, Dieter; Van Oyen, Herman; Van den Borre, Laura; Brondeel, Ruben</t>
   </si>
 </sst>
 </file>
@@ -2929,6 +2944,166 @@
   </cellStyles>
   <dxfs count="66">
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -3088,166 +3263,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -3262,73 +3277,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U179" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U179" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:U179"/>
-  <sortState ref="A2:U178">
-    <sortCondition ref="K1:K178"/>
+  <sortState ref="A2:U179">
+    <sortCondition ref="K1:K179"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="63"/>
-    <tableColumn id="2" name="authors" dataDxfId="62"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="61"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="60"/>
-    <tableColumn id="6" name="year" dataDxfId="59"/>
-    <tableColumn id="4" name="volume" dataDxfId="58"/>
-    <tableColumn id="5" name="issue" dataDxfId="57"/>
-    <tableColumn id="7" name="eID" dataDxfId="56"/>
-    <tableColumn id="8" name="from" dataDxfId="55"/>
-    <tableColumn id="9" name="to" dataDxfId="54"/>
-    <tableColumn id="10" name="date" dataDxfId="53"/>
-    <tableColumn id="14" name="classification" dataDxfId="52"/>
-    <tableColumn id="12" name="IF" dataDxfId="51"/>
-    <tableColumn id="13" name="DOI" dataDxfId="50"/>
-    <tableColumn id="15" name="WoS" dataDxfId="49"/>
-    <tableColumn id="16" name="rank" dataDxfId="48"/>
-    <tableColumn id="17" name="quartile" dataDxfId="47"/>
-    <tableColumn id="18" name="category" dataDxfId="46"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="45"/>
-    <tableColumn id="20" name="SC" dataDxfId="44"/>
-    <tableColumn id="21" name="UGent" dataDxfId="43"/>
+    <tableColumn id="1" name="title" dataDxfId="47"/>
+    <tableColumn id="2" name="authors" dataDxfId="46"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
+    <tableColumn id="6" name="year" dataDxfId="43"/>
+    <tableColumn id="4" name="volume" dataDxfId="42"/>
+    <tableColumn id="5" name="issue" dataDxfId="41"/>
+    <tableColumn id="7" name="eID" dataDxfId="40"/>
+    <tableColumn id="8" name="from" dataDxfId="39"/>
+    <tableColumn id="9" name="to" dataDxfId="38"/>
+    <tableColumn id="10" name="date" dataDxfId="37"/>
+    <tableColumn id="14" name="classification" dataDxfId="36"/>
+    <tableColumn id="12" name="IF" dataDxfId="35"/>
+    <tableColumn id="13" name="DOI" dataDxfId="34"/>
+    <tableColumn id="15" name="WoS" dataDxfId="33"/>
+    <tableColumn id="16" name="rank" dataDxfId="32"/>
+    <tableColumn id="17" name="quartile" dataDxfId="31"/>
+    <tableColumn id="18" name="category" dataDxfId="30"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
+    <tableColumn id="20" name="SC" dataDxfId="28"/>
+    <tableColumn id="21" name="UGent" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J9" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J9" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:J9"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="41"/>
-    <tableColumn id="2" name="authors" dataDxfId="40"/>
-    <tableColumn id="3" name="editors" dataDxfId="39"/>
-    <tableColumn id="11" name="book" dataDxfId="38"/>
-    <tableColumn id="6" name="year" dataDxfId="37"/>
-    <tableColumn id="8" name="from" dataDxfId="36"/>
-    <tableColumn id="9" name="to" dataDxfId="35"/>
-    <tableColumn id="10" name="date" dataDxfId="34"/>
-    <tableColumn id="12" name="IF" dataDxfId="33"/>
-    <tableColumn id="13" name="DOI" dataDxfId="32"/>
+    <tableColumn id="1" name="title" dataDxfId="25"/>
+    <tableColumn id="2" name="authors" dataDxfId="24"/>
+    <tableColumn id="3" name="editors" dataDxfId="23"/>
+    <tableColumn id="11" name="book" dataDxfId="22"/>
+    <tableColumn id="6" name="year" dataDxfId="21"/>
+    <tableColumn id="8" name="from" dataDxfId="20"/>
+    <tableColumn id="9" name="to" dataDxfId="19"/>
+    <tableColumn id="10" name="date" dataDxfId="18"/>
+    <tableColumn id="12" name="IF" dataDxfId="17"/>
+    <tableColumn id="13" name="DOI" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F15" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F16"/>
   <sortState ref="A2:F15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="29"/>
-    <tableColumn id="2" name="authors" dataDxfId="28"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="27"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="26"/>
-    <tableColumn id="10" name="date" dataDxfId="25"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="24">
+    <tableColumn id="1" name="title" dataDxfId="13"/>
+    <tableColumn id="2" name="authors" dataDxfId="12"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
+    <tableColumn id="10" name="date" dataDxfId="9"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="8">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3337,18 +3352,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="21"/>
-    <tableColumn id="2" name="authors" dataDxfId="20"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="19"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="18"/>
-    <tableColumn id="10" name="date" dataDxfId="17"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="16">
+    <tableColumn id="1" name="title" dataDxfId="5"/>
+    <tableColumn id="2" name="authors" dataDxfId="4"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
+    <tableColumn id="10" name="date" dataDxfId="1"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="0">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3645,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView topLeftCell="A144" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11850,16 +11865,16 @@
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="B149" s="7" t="s">
         <v>819</v>
       </c>
-      <c r="B149" s="7" t="s">
+      <c r="C149" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="D149" s="7" t="s">
         <v>820</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>822</v>
-      </c>
-      <c r="D149" s="7" t="s">
-        <v>821</v>
       </c>
       <c r="E149" s="18">
         <v>2021</v>
@@ -11887,7 +11902,7 @@
       </c>
       <c r="M149" s="11"/>
       <c r="N149" s="19" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="O149" s="7"/>
       <c r="P149" s="24"/>
@@ -11919,7 +11934,7 @@
         <v>397</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H150" s="18" t="s">
         <v>14</v>
@@ -12027,10 +12042,10 @@
         <v>14</v>
       </c>
       <c r="I152" s="18" t="s">
+        <v>804</v>
+      </c>
+      <c r="J152" s="18" t="s">
         <v>805</v>
-      </c>
-      <c r="J152" s="18" t="s">
-        <v>806</v>
       </c>
       <c r="K152" s="42">
         <v>44287</v>
@@ -12142,7 +12157,7 @@
       </c>
       <c r="M154" s="11"/>
       <c r="N154" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="O154" s="7"/>
       <c r="P154" s="24"/>
@@ -12156,7 +12171,7 @@
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B155" s="7" t="s">
         <v>694</v>
@@ -12193,7 +12208,7 @@
       </c>
       <c r="M155" s="11"/>
       <c r="N155" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="O155" s="7"/>
       <c r="P155" s="24"/>
@@ -12258,10 +12273,10 @@
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="B157" s="7" t="s">
         <v>823</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>824</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>381</v>
@@ -12295,7 +12310,7 @@
       </c>
       <c r="M157" s="11"/>
       <c r="N157" s="19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="O157" s="7"/>
       <c r="P157" s="24"/>
@@ -12346,7 +12361,7 @@
       </c>
       <c r="M158" s="11"/>
       <c r="N158" s="19" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="O158" s="7"/>
       <c r="P158" s="24"/>
@@ -12360,16 +12375,16 @@
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="B159" s="7" t="s">
         <v>815</v>
       </c>
-      <c r="B159" s="7" t="s">
-        <v>816</v>
-      </c>
       <c r="C159" s="7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E159" s="18">
         <v>2021</v>
@@ -12397,7 +12412,7 @@
       </c>
       <c r="M159" s="11"/>
       <c r="N159" s="19" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="O159" s="7"/>
       <c r="P159" s="24"/>
@@ -12448,7 +12463,7 @@
       </c>
       <c r="M160" s="11"/>
       <c r="N160" s="19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="O160" s="7"/>
       <c r="P160" s="24"/>
@@ -12513,10 +12528,10 @@
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>842</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>843</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>268</v>
@@ -12550,7 +12565,7 @@
       </c>
       <c r="M162" s="11"/>
       <c r="N162" s="19" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="O162" s="7"/>
       <c r="P162" s="24"/>
@@ -12652,7 +12667,7 @@
       </c>
       <c r="M164" s="11"/>
       <c r="N164" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="O164" s="7"/>
       <c r="P164" s="24"/>
@@ -12669,7 +12684,7 @@
         <v>772</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>161</v>
@@ -12687,7 +12702,7 @@
         <v>426</v>
       </c>
       <c r="H165" s="32" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I165" s="32" t="s">
         <v>14</v>
@@ -12703,7 +12718,7 @@
       </c>
       <c r="M165" s="11"/>
       <c r="N165" s="19" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O165" s="7"/>
       <c r="P165" s="24"/>
@@ -12717,16 +12732,16 @@
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>867</v>
       </c>
-      <c r="B166" s="7" t="s">
+      <c r="D166" s="7" t="s">
         <v>871</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>868</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>872</v>
       </c>
       <c r="E166" s="18">
         <v>2021</v>
@@ -12738,7 +12753,7 @@
         <v>14</v>
       </c>
       <c r="H166" s="32" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="I166" s="32" t="s">
         <v>14</v>
@@ -12754,7 +12769,7 @@
       </c>
       <c r="M166" s="11"/>
       <c r="N166" s="19" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="O166" s="7"/>
       <c r="P166" s="24"/>
@@ -12819,10 +12834,10 @@
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>766</v>
@@ -12856,7 +12871,7 @@
       </c>
       <c r="M168" s="11"/>
       <c r="N168" s="19" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="O168" s="7"/>
       <c r="P168" s="24"/>
@@ -12870,10 +12885,10 @@
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="B169" s="7" t="s">
         <v>826</v>
-      </c>
-      <c r="B169" s="7" t="s">
-        <v>827</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>90</v>
@@ -12907,7 +12922,7 @@
       </c>
       <c r="M169" s="11"/>
       <c r="N169" s="19" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="O169" s="7"/>
       <c r="P169" s="24"/>
@@ -12958,7 +12973,7 @@
       </c>
       <c r="M170" s="11"/>
       <c r="N170" s="19" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="O170" s="7"/>
       <c r="P170" s="24"/>
@@ -12972,16 +12987,16 @@
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="B171" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>814</v>
-      </c>
       <c r="C171" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="D171" s="7" t="s">
         <v>881</v>
-      </c>
-      <c r="D171" s="7" t="s">
-        <v>882</v>
       </c>
       <c r="E171" s="18">
         <v>2021</v>
@@ -13009,7 +13024,7 @@
       </c>
       <c r="M171" s="11"/>
       <c r="N171" s="19" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="O171" s="7"/>
       <c r="P171" s="24"/>
@@ -13023,10 +13038,10 @@
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>725</v>
@@ -13044,7 +13059,7 @@
         <v>14</v>
       </c>
       <c r="H172" s="18" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I172" s="18" t="s">
         <v>14</v>
@@ -13060,7 +13075,7 @@
       </c>
       <c r="M172" s="11"/>
       <c r="N172" s="19" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="O172" s="7"/>
       <c r="P172" s="24"/>
@@ -13111,7 +13126,7 @@
       </c>
       <c r="M173" s="11"/>
       <c r="N173" s="19" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="O173" s="7"/>
       <c r="P173" s="24"/>
@@ -13124,66 +13139,68 @@
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A174" s="13" t="s">
-        <v>796</v>
-      </c>
-      <c r="B174" s="13" t="s">
-        <v>797</v>
-      </c>
-      <c r="C174" s="13" t="s">
-        <v>795</v>
-      </c>
-      <c r="D174" s="13" t="s">
-        <v>798</v>
-      </c>
-      <c r="E174" s="14">
+      <c r="A174" s="7" t="s">
+        <v>895</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E174" s="18">
         <v>2021</v>
       </c>
-      <c r="F174" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G174" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H174" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I174" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J174" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K174" s="31">
-        <v>44927</v>
-      </c>
-      <c r="L174" s="31" t="s">
-        <v>274</v>
-      </c>
-      <c r="M174" s="45"/>
-      <c r="N174" s="44" t="s">
-        <v>835</v>
-      </c>
-      <c r="O174" s="27"/>
+      <c r="F174" s="18">
+        <v>26</v>
+      </c>
+      <c r="G174" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="H174" s="18" t="s">
+        <v>897</v>
+      </c>
+      <c r="I174" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J174" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K174" s="42">
+        <v>44532</v>
+      </c>
+      <c r="L174" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="M174" s="11"/>
+      <c r="N174" s="19" t="s">
+        <v>898</v>
+      </c>
+      <c r="O174" s="7"/>
       <c r="P174" s="24"/>
       <c r="Q174" s="25"/>
       <c r="R174" s="7"/>
       <c r="S174" s="7"/>
       <c r="T174" s="7"/>
-      <c r="U174" s="7"/>
+      <c r="U174" s="7" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
-        <v>846</v>
+        <v>796</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>781</v>
+        <v>797</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>660</v>
+        <v>795</v>
       </c>
       <c r="D175" s="13" t="s">
-        <v>661</v>
+        <v>798</v>
       </c>
       <c r="E175" s="14">
         <v>2021</v>
@@ -13204,14 +13221,14 @@
         <v>14</v>
       </c>
       <c r="K175" s="31">
-        <v>44928</v>
+        <v>44927</v>
       </c>
       <c r="L175" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M175" s="45"/>
       <c r="N175" s="44" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="O175" s="27"/>
       <c r="P175" s="24"/>
@@ -13223,10 +13240,10 @@
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
-        <v>731</v>
+        <v>845</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>811</v>
+        <v>781</v>
       </c>
       <c r="C176" s="13" t="s">
         <v>660</v>
@@ -13253,14 +13270,14 @@
         <v>14</v>
       </c>
       <c r="K176" s="31">
-        <v>44929</v>
+        <v>44928</v>
       </c>
       <c r="L176" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M176" s="45"/>
       <c r="N176" s="44" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="O176" s="27"/>
       <c r="P176" s="24"/>
@@ -13272,16 +13289,16 @@
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
-        <v>802</v>
+        <v>731</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>339</v>
+        <v>660</v>
       </c>
       <c r="D177" s="13" t="s">
-        <v>340</v>
+        <v>661</v>
       </c>
       <c r="E177" s="14">
         <v>2021</v>
@@ -13302,13 +13319,15 @@
         <v>14</v>
       </c>
       <c r="K177" s="31">
-        <v>44930</v>
+        <v>44929</v>
       </c>
       <c r="L177" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M177" s="45"/>
-      <c r="N177" s="44"/>
+      <c r="N177" s="44" t="s">
+        <v>857</v>
+      </c>
       <c r="O177" s="27"/>
       <c r="P177" s="24"/>
       <c r="Q177" s="25"/>
@@ -13366,10 +13385,10 @@
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
+        <v>893</v>
+      </c>
+      <c r="B179" s="13" t="s">
         <v>894</v>
-      </c>
-      <c r="B179" s="13" t="s">
-        <v>895</v>
       </c>
       <c r="C179" s="13" t="s">
         <v>55</v>
@@ -13413,66 +13432,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S136:U146 S148:U175 S177:U1048576">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="15" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S176:U176">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13771,7 +13790,7 @@
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="19" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
   </sheetData>
@@ -13784,9 +13803,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13833,37 +13852,37 @@
         <v>44191</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F15" ca="1" si="0">TODAY()-E2</f>
-        <v>327</v>
+        <f t="shared" ref="F2:F16" ca="1" si="0">TODAY()-E2</f>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>807</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>810</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>808</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>809</v>
       </c>
       <c r="E3" s="10">
         <v>44281</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>237</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>831</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>832</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>288</v>
@@ -13876,57 +13895,57 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>839</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>841</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>840</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E5" s="10">
         <v>44383</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="B6" t="s">
         <v>848</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="7" t="s">
         <v>849</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>850</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>851</v>
       </c>
       <c r="E6" s="10">
         <v>44421</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>853</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>854</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>660</v>
@@ -13939,15 +13958,15 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>855</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>856</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>374</v>
@@ -13960,15 +13979,15 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>859</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>860</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>90</v>
@@ -13981,15 +14000,15 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>874</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>875</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>253</v>
@@ -14002,36 +14021,36 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>864</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>865</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E11" s="10">
         <v>44475</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>876</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>877</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>268</v>
@@ -14044,15 +14063,15 @@
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>879</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>880</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>268</v>
@@ -14065,15 +14084,15 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>268</v>
@@ -14086,28 +14105,49 @@
       </c>
       <c r="F14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>886</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>887</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>884</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>888</v>
       </c>
       <c r="E15" s="10">
         <v>44503</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" s="10">
+        <v>44532</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14172,7 +14212,7 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>6.0547945205479454</v>
+        <v>6.095890410958904</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14193,7 +14233,7 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0547945205479454</v>
+        <v>6.095890410958904</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14214,7 +14254,7 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4328767123287669</v>
+        <v>5.4739726027397264</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -14235,7 +14275,7 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>3.8027397260273972</v>
+        <v>3.8438356164383563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new book chapter published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="915">
   <si>
     <t>title</t>
   </si>
@@ -2402,9 +2402,6 @@
     <t>Risk factors and their contribution to population health in the European Union (EU-28) countries in 2007 and 2017</t>
   </si>
   <si>
-    <t>Estimates of global disease burden associated with foodborne pathogens</t>
-  </si>
-  <si>
     <t>Foodborne Infections and Intoxications, 5th ed.</t>
   </si>
   <si>
@@ -2754,6 +2751,24 @@
   </si>
   <si>
     <t>Otavova, Martina; Faes, Christel; Bouland, Catherine; De Clercq, Eva; Vandeninden, Bram; Eggerickx, Thierry; Sanderson, Jean-Paul; Devleesschauwer, Brecht; Masquelier, Bruno</t>
+  </si>
+  <si>
+    <t>Taenia solium Cysticercosis/Taeniosis in Europe and Central Asia</t>
+  </si>
+  <si>
+    <t>Trevisan, Chiara; Gabriël, Sarah; Dorny, Pierre; Devleesschauwer, Brecht</t>
+  </si>
+  <si>
+    <t>Steinmann, Peter; Utzinger, Jürg</t>
+  </si>
+  <si>
+    <t>Neglected Tropical Diseases - Europe and Central Asia</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-030-84224-6_4</t>
+  </si>
+  <si>
+    <t>Estimates of Global Disease Burden Associated with Foodborne Pathogens</t>
   </si>
 </sst>
 </file>
@@ -2829,7 +2844,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2963,6 +2978,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2970,6 +2988,166 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3170,166 +3348,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="d/mm/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -3344,73 +3362,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U182" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:U182" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:U182"/>
   <sortState ref="A2:U179">
     <sortCondition ref="K1:K179"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="title" dataDxfId="67"/>
-    <tableColumn id="2" name="authors" dataDxfId="66"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="65"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="64"/>
-    <tableColumn id="6" name="year" dataDxfId="63"/>
-    <tableColumn id="4" name="volume" dataDxfId="62"/>
-    <tableColumn id="5" name="issue" dataDxfId="61"/>
-    <tableColumn id="7" name="eID" dataDxfId="60"/>
-    <tableColumn id="8" name="from" dataDxfId="59"/>
-    <tableColumn id="9" name="to" dataDxfId="58"/>
-    <tableColumn id="10" name="date" dataDxfId="57"/>
-    <tableColumn id="14" name="classification" dataDxfId="56"/>
-    <tableColumn id="12" name="IF" dataDxfId="55"/>
-    <tableColumn id="13" name="DOI" dataDxfId="54"/>
-    <tableColumn id="15" name="WoS" dataDxfId="53"/>
-    <tableColumn id="16" name="rank" dataDxfId="52"/>
-    <tableColumn id="17" name="quartile" dataDxfId="51"/>
-    <tableColumn id="18" name="category" dataDxfId="50"/>
-    <tableColumn id="19" name="CBRA" dataDxfId="49"/>
-    <tableColumn id="20" name="SC" dataDxfId="48"/>
-    <tableColumn id="21" name="UGent" dataDxfId="47"/>
+    <tableColumn id="1" name="title" dataDxfId="47"/>
+    <tableColumn id="2" name="authors" dataDxfId="46"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="45"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="44"/>
+    <tableColumn id="6" name="year" dataDxfId="43"/>
+    <tableColumn id="4" name="volume" dataDxfId="42"/>
+    <tableColumn id="5" name="issue" dataDxfId="41"/>
+    <tableColumn id="7" name="eID" dataDxfId="40"/>
+    <tableColumn id="8" name="from" dataDxfId="39"/>
+    <tableColumn id="9" name="to" dataDxfId="38"/>
+    <tableColumn id="10" name="date" dataDxfId="37"/>
+    <tableColumn id="14" name="classification" dataDxfId="36"/>
+    <tableColumn id="12" name="IF" dataDxfId="35"/>
+    <tableColumn id="13" name="DOI" dataDxfId="34"/>
+    <tableColumn id="15" name="WoS" dataDxfId="33"/>
+    <tableColumn id="16" name="rank" dataDxfId="32"/>
+    <tableColumn id="17" name="quartile" dataDxfId="31"/>
+    <tableColumn id="18" name="category" dataDxfId="30"/>
+    <tableColumn id="19" name="CBRA" dataDxfId="29"/>
+    <tableColumn id="20" name="SC" dataDxfId="28"/>
+    <tableColumn id="21" name="UGent" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J9" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="A1:J9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:J10" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="A1:J10"/>
   <sortState ref="A2:N50">
     <sortCondition ref="H1:H50"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="title" dataDxfId="45"/>
-    <tableColumn id="2" name="authors" dataDxfId="44"/>
-    <tableColumn id="3" name="editors" dataDxfId="43"/>
-    <tableColumn id="11" name="book" dataDxfId="42"/>
-    <tableColumn id="6" name="year" dataDxfId="41"/>
-    <tableColumn id="8" name="from" dataDxfId="40"/>
-    <tableColumn id="9" name="to" dataDxfId="39"/>
-    <tableColumn id="10" name="date" dataDxfId="38"/>
-    <tableColumn id="12" name="IF" dataDxfId="37"/>
-    <tableColumn id="13" name="DOI" dataDxfId="36"/>
+    <tableColumn id="1" name="title" dataDxfId="25"/>
+    <tableColumn id="2" name="authors" dataDxfId="24"/>
+    <tableColumn id="3" name="editors" dataDxfId="23"/>
+    <tableColumn id="11" name="book" dataDxfId="22"/>
+    <tableColumn id="6" name="year" dataDxfId="21"/>
+    <tableColumn id="8" name="from" dataDxfId="20"/>
+    <tableColumn id="9" name="to" dataDxfId="19"/>
+    <tableColumn id="10" name="date" dataDxfId="18"/>
+    <tableColumn id="12" name="IF" dataDxfId="17"/>
+    <tableColumn id="13" name="DOI" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F17" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:F17"/>
   <sortState ref="A2:F15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="33"/>
-    <tableColumn id="2" name="authors" dataDxfId="32"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="31"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="30"/>
-    <tableColumn id="10" name="date" dataDxfId="29"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="28">
+    <tableColumn id="1" name="title" dataDxfId="13"/>
+    <tableColumn id="2" name="authors" dataDxfId="12"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="11"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="10"/>
+    <tableColumn id="10" name="date" dataDxfId="9"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="8">
       <calculatedColumnFormula>TODAY()-E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3419,18 +3437,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel135" displayName="Tabel135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F5"/>
   <sortState ref="A2:K14">
     <sortCondition ref="E1:E14"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="title" dataDxfId="25"/>
-    <tableColumn id="2" name="authors" dataDxfId="24"/>
-    <tableColumn id="3" name="journal_full" dataDxfId="23"/>
-    <tableColumn id="11" name="journal_short" dataDxfId="22"/>
-    <tableColumn id="10" name="date" dataDxfId="21"/>
-    <tableColumn id="12" name="COUNT" dataDxfId="20">
+    <tableColumn id="1" name="title" dataDxfId="5"/>
+    <tableColumn id="2" name="authors" dataDxfId="4"/>
+    <tableColumn id="3" name="journal_full" dataDxfId="3"/>
+    <tableColumn id="11" name="journal_short" dataDxfId="2"/>
+    <tableColumn id="10" name="date" dataDxfId="1"/>
+    <tableColumn id="12" name="COUNT" dataDxfId="0">
       <calculatedColumnFormula>(TODAY()-E2)/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3727,7 +3745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A144" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
@@ -11952,16 +11970,16 @@
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B149" s="7" t="s">
         <v>818</v>
       </c>
-      <c r="B149" s="7" t="s">
+      <c r="C149" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="D149" s="7" t="s">
         <v>819</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>821</v>
-      </c>
-      <c r="D149" s="7" t="s">
-        <v>820</v>
       </c>
       <c r="E149" s="18">
         <v>2021</v>
@@ -11989,7 +12007,7 @@
       </c>
       <c r="M149" s="11"/>
       <c r="N149" s="19" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="O149" s="7"/>
       <c r="P149" s="24"/>
@@ -12023,7 +12041,7 @@
         <v>397</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H150" s="18" t="s">
         <v>14</v>
@@ -12095,7 +12113,7 @@
       </c>
       <c r="M151" s="11"/>
       <c r="N151" s="19" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="O151" s="7"/>
       <c r="P151" s="24"/>
@@ -12135,10 +12153,10 @@
         <v>14</v>
       </c>
       <c r="I152" s="18" t="s">
+        <v>803</v>
+      </c>
+      <c r="J152" s="18" t="s">
         <v>804</v>
-      </c>
-      <c r="J152" s="18" t="s">
-        <v>805</v>
       </c>
       <c r="K152" s="42">
         <v>44287</v>
@@ -12254,7 +12272,7 @@
       </c>
       <c r="M154" s="11"/>
       <c r="N154" s="19" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="O154" s="7"/>
       <c r="P154" s="24"/>
@@ -12270,7 +12288,7 @@
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B155" s="7" t="s">
         <v>694</v>
@@ -12307,7 +12325,7 @@
       </c>
       <c r="M155" s="11"/>
       <c r="N155" s="19" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="O155" s="7"/>
       <c r="P155" s="24"/>
@@ -12376,10 +12394,10 @@
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="B157" s="7" t="s">
         <v>822</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>823</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>381</v>
@@ -12413,7 +12431,7 @@
       </c>
       <c r="M157" s="11"/>
       <c r="N157" s="19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O157" s="7"/>
       <c r="P157" s="24"/>
@@ -12466,7 +12484,7 @@
       </c>
       <c r="M158" s="11"/>
       <c r="N158" s="19" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="O158" s="7"/>
       <c r="P158" s="24"/>
@@ -12482,16 +12500,16 @@
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="B159" s="7" t="s">
         <v>814</v>
       </c>
-      <c r="B159" s="7" t="s">
-        <v>815</v>
-      </c>
       <c r="C159" s="7" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E159" s="18">
         <v>2021</v>
@@ -12519,7 +12537,7 @@
       </c>
       <c r="M159" s="11"/>
       <c r="N159" s="19" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="O159" s="7"/>
       <c r="P159" s="24"/>
@@ -12535,10 +12553,10 @@
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="B160" s="7" t="s">
         <v>799</v>
-      </c>
-      <c r="B160" s="7" t="s">
-        <v>800</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>268</v>
@@ -12572,7 +12590,7 @@
       </c>
       <c r="M160" s="11"/>
       <c r="N160" s="19" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="O160" s="7"/>
       <c r="P160" s="24"/>
@@ -12641,10 +12659,10 @@
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>841</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>842</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>268</v>
@@ -12678,7 +12696,7 @@
       </c>
       <c r="M162" s="11"/>
       <c r="N162" s="19" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="O162" s="7"/>
       <c r="P162" s="24"/>
@@ -12784,7 +12802,7 @@
       </c>
       <c r="M164" s="11"/>
       <c r="N164" s="19" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="O164" s="7"/>
       <c r="P164" s="24"/>
@@ -12803,7 +12821,7 @@
         <v>772</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>161</v>
@@ -12821,7 +12839,7 @@
         <v>426</v>
       </c>
       <c r="H165" s="32" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I165" s="32" t="s">
         <v>14</v>
@@ -12837,7 +12855,7 @@
       </c>
       <c r="M165" s="11"/>
       <c r="N165" s="19" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O165" s="7"/>
       <c r="P165" s="24"/>
@@ -12853,16 +12871,16 @@
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>869</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>866</v>
       </c>
-      <c r="B166" s="7" t="s">
+      <c r="D166" s="7" t="s">
         <v>870</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>867</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>871</v>
       </c>
       <c r="E166" s="18">
         <v>2021</v>
@@ -12874,7 +12892,7 @@
         <v>14</v>
       </c>
       <c r="H166" s="32" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I166" s="32" t="s">
         <v>14</v>
@@ -12890,7 +12908,7 @@
       </c>
       <c r="M166" s="11"/>
       <c r="N166" s="19" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O166" s="7"/>
       <c r="P166" s="24"/>
@@ -12959,10 +12977,10 @@
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>766</v>
@@ -12996,7 +13014,7 @@
       </c>
       <c r="M168" s="11"/>
       <c r="N168" s="19" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="O168" s="7"/>
       <c r="P168" s="24"/>
@@ -13012,10 +13030,10 @@
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="B169" s="7" t="s">
         <v>825</v>
-      </c>
-      <c r="B169" s="7" t="s">
-        <v>826</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>90</v>
@@ -13049,7 +13067,7 @@
       </c>
       <c r="M169" s="11"/>
       <c r="N169" s="19" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O169" s="7"/>
       <c r="P169" s="24"/>
@@ -13102,7 +13120,7 @@
       </c>
       <c r="M170" s="11"/>
       <c r="N170" s="19" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="O170" s="7"/>
       <c r="P170" s="24"/>
@@ -13118,16 +13136,16 @@
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="B171" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>813</v>
-      </c>
       <c r="C171" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="D171" s="7" t="s">
         <v>880</v>
-      </c>
-      <c r="D171" s="7" t="s">
-        <v>881</v>
       </c>
       <c r="E171" s="18">
         <v>2021</v>
@@ -13155,7 +13173,7 @@
       </c>
       <c r="M171" s="11"/>
       <c r="N171" s="19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="O171" s="7"/>
       <c r="P171" s="24"/>
@@ -13171,10 +13189,10 @@
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>725</v>
@@ -13192,7 +13210,7 @@
         <v>14</v>
       </c>
       <c r="H172" s="18" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I172" s="18" t="s">
         <v>14</v>
@@ -13208,7 +13226,7 @@
       </c>
       <c r="M172" s="11"/>
       <c r="N172" s="19" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="O172" s="7"/>
       <c r="P172" s="24"/>
@@ -13261,7 +13279,7 @@
       </c>
       <c r="M173" s="11"/>
       <c r="N173" s="19" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="O173" s="7"/>
       <c r="P173" s="24"/>
@@ -13277,10 +13295,10 @@
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C174" s="7" t="s">
         <v>339</v>
@@ -13295,10 +13313,10 @@
         <v>26</v>
       </c>
       <c r="G174" s="19" t="s">
+        <v>895</v>
+      </c>
+      <c r="H174" s="18" t="s">
         <v>896</v>
-      </c>
-      <c r="H174" s="18" t="s">
-        <v>897</v>
       </c>
       <c r="I174" s="18" t="s">
         <v>14</v>
@@ -13314,7 +13332,7 @@
       </c>
       <c r="M174" s="11"/>
       <c r="N174" s="19" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="O174" s="7"/>
       <c r="P174" s="24"/>
@@ -13330,16 +13348,16 @@
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
+        <v>795</v>
+      </c>
+      <c r="B175" s="13" t="s">
         <v>796</v>
       </c>
-      <c r="B175" s="13" t="s">
+      <c r="C175" s="13" t="s">
+        <v>794</v>
+      </c>
+      <c r="D175" s="13" t="s">
         <v>797</v>
-      </c>
-      <c r="C175" s="13" t="s">
-        <v>795</v>
-      </c>
-      <c r="D175" s="13" t="s">
-        <v>798</v>
       </c>
       <c r="E175" s="14">
         <v>2022</v>
@@ -13367,7 +13385,7 @@
       </c>
       <c r="M175" s="45"/>
       <c r="N175" s="44" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="O175" s="27"/>
       <c r="P175" s="24"/>
@@ -13379,7 +13397,7 @@
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B176" s="13" t="s">
         <v>781</v>
@@ -13416,7 +13434,7 @@
       </c>
       <c r="M176" s="45"/>
       <c r="N176" s="44" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="O176" s="27"/>
       <c r="P176" s="24"/>
@@ -13431,7 +13449,7 @@
         <v>731</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C177" s="13" t="s">
         <v>660</v>
@@ -13465,7 +13483,7 @@
       </c>
       <c r="M177" s="45"/>
       <c r="N177" s="44" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="O177" s="27"/>
       <c r="P177" s="24"/>
@@ -13477,10 +13495,10 @@
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
+        <v>892</v>
+      </c>
+      <c r="B178" s="13" t="s">
         <v>893</v>
-      </c>
-      <c r="B178" s="13" t="s">
-        <v>894</v>
       </c>
       <c r="C178" s="13" t="s">
         <v>55</v>
@@ -13514,7 +13532,7 @@
       </c>
       <c r="M178" s="45"/>
       <c r="N178" s="44" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="O178" s="27"/>
       <c r="P178" s="24"/>
@@ -13573,16 +13591,16 @@
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
+        <v>837</v>
+      </c>
+      <c r="B180" s="13" t="s">
+        <v>839</v>
+      </c>
+      <c r="C180" s="13" t="s">
         <v>838</v>
       </c>
-      <c r="B180" s="13" t="s">
-        <v>840</v>
-      </c>
-      <c r="C180" s="13" t="s">
-        <v>839</v>
-      </c>
       <c r="D180" s="13" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E180" s="14">
         <v>2022</v>
@@ -13620,10 +13638,10 @@
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
+        <v>829</v>
+      </c>
+      <c r="B181" s="13" t="s">
         <v>830</v>
-      </c>
-      <c r="B181" s="13" t="s">
-        <v>831</v>
       </c>
       <c r="C181" s="13" t="s">
         <v>288</v>
@@ -13667,16 +13685,16 @@
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
+        <v>846</v>
+      </c>
+      <c r="B182" s="13" t="s">
         <v>847</v>
       </c>
-      <c r="B182" s="13" t="s">
+      <c r="C182" s="13" t="s">
         <v>848</v>
       </c>
-      <c r="C182" s="13" t="s">
+      <c r="D182" s="13" t="s">
         <v>849</v>
-      </c>
-      <c r="D182" s="13" t="s">
-        <v>850</v>
       </c>
       <c r="E182" s="14">
         <v>2022</v>
@@ -13714,82 +13732,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S1:U112 S114:U122 S124:U125 S127:U134 U126 S148:U175 S177:U179 S182:U1048576 S136:U146">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="19" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T113:U113">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="17" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="15" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S123:U123">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="13" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S126:T126">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S135:U135">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S147:U147">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S176:U176">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S180:U180">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S181:U181">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13803,9 +13821,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14063,16 +14081,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>792</v>
+        <v>914</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>789</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E9" s="18">
         <v>2021</v>
@@ -14088,7 +14106,37 @@
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="19" t="s">
-        <v>833</v>
+        <v>832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>911</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>912</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2022</v>
+      </c>
+      <c r="F10" s="18">
+        <v>69</v>
+      </c>
+      <c r="G10" s="18">
+        <v>82</v>
+      </c>
+      <c r="H10" s="42">
+        <v>44562</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="19" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -14151,36 +14199,36 @@
       </c>
       <c r="F2" s="12">
         <f t="shared" ref="F2:F17" ca="1" si="0">TODAY()-E2</f>
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>808</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>806</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>809</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>807</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>808</v>
       </c>
       <c r="E3" s="10">
         <v>44281</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>852</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>853</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>660</v>
@@ -14193,15 +14241,15 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>854</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>855</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>374</v>
@@ -14214,15 +14262,15 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>858</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>859</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>90</v>
@@ -14235,15 +14283,15 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>873</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>874</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>253</v>
@@ -14256,36 +14304,36 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>863</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>864</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E8" s="10">
         <v>44475</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>875</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>876</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>268</v>
@@ -14298,15 +14346,15 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>878</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>879</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>268</v>
@@ -14319,15 +14367,15 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>268</v>
@@ -14340,36 +14388,36 @@
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>884</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>885</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
+        <v>882</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>886</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>883</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>887</v>
       </c>
       <c r="E12" s="10">
         <v>44503</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>899</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>900</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>268</v>
@@ -14382,15 +14430,15 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>902</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>903</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>109</v>
@@ -14403,15 +14451,15 @@
       </c>
       <c r="F14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>904</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>905</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>161</v>
@@ -14424,15 +14472,15 @@
       </c>
       <c r="F15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>12</v>
@@ -14445,15 +14493,15 @@
       </c>
       <c r="F16" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>908</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>909</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>576</v>
@@ -14466,7 +14514,7 @@
       </c>
       <c r="F17" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -14531,7 +14579,7 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>6.183561643835616</v>
+        <v>6.1890410958904107</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14552,7 +14600,7 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6.183561643835616</v>
+        <v>6.1890410958904107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14573,7 +14621,7 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5616438356164384</v>
+        <v>5.5671232876712331</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -14594,7 +14642,7 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>3.9315068493150687</v>
+        <v>3.9369863013698629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new submission & fully published
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="935">
   <si>
     <t>title</t>
   </si>
@@ -2817,6 +2817,18 @@
   </si>
   <si>
     <t>10.1016/j.envres.2022.113014</t>
+  </si>
+  <si>
+    <t>Environmental nitrogen enrichment and the increasing burden of allergic disease: a trait modification hypothesis</t>
+  </si>
+  <si>
+    <t>Environmental Health</t>
+  </si>
+  <si>
+    <t>Environ. Health</t>
+  </si>
+  <si>
+    <t>Ceulemans, Tobias; Verscheure, Paulien; Shadouh, Caroline; Van Acker, Kasper; Devleesschauwer, Brecht; Linard, Catherine; Dendoncker, Nicolas; Speybroeck, Niko; Bruffaerts, Nicolas; Honnay, Olivier; Schrijvers, Rik; Aerts, Raf</t>
   </si>
 </sst>
 </file>
@@ -3465,8 +3477,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:F17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel13" displayName="Tabel13" ref="A1:F18" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:F18"/>
   <sortState ref="A2:F15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
@@ -3793,8 +3805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13819,47 +13831,47 @@
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A183" s="13" t="s">
-        <v>795</v>
-      </c>
-      <c r="B183" s="13" t="s">
-        <v>796</v>
-      </c>
-      <c r="C183" s="13" t="s">
-        <v>794</v>
-      </c>
-      <c r="D183" s="13" t="s">
-        <v>797</v>
-      </c>
-      <c r="E183" s="14">
+      <c r="A183" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="E183" s="18">
         <v>2022</v>
       </c>
-      <c r="F183" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G183" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H183" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I183" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J183" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="K183" s="31">
-        <v>44927</v>
-      </c>
-      <c r="L183" s="31" t="s">
-        <v>274</v>
-      </c>
-      <c r="M183" s="45"/>
-      <c r="N183" s="44" t="s">
-        <v>831</v>
-      </c>
-      <c r="O183" s="27"/>
+      <c r="F183" s="18">
+        <v>210</v>
+      </c>
+      <c r="G183" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H183" s="18">
+        <v>113014</v>
+      </c>
+      <c r="I183" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J183" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K183" s="42">
+        <v>44743</v>
+      </c>
+      <c r="L183" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="M183" s="11"/>
+      <c r="N183" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="O183" s="7"/>
       <c r="P183" s="24"/>
       <c r="Q183" s="25"/>
       <c r="R183" s="7"/>
@@ -13869,16 +13881,16 @@
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="13" t="s">
-        <v>827</v>
+        <v>795</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>828</v>
+        <v>796</v>
       </c>
       <c r="C184" s="13" t="s">
-        <v>288</v>
+        <v>794</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>331</v>
+        <v>797</v>
       </c>
       <c r="E184" s="14">
         <v>2022</v>
@@ -13899,14 +13911,14 @@
         <v>14</v>
       </c>
       <c r="K184" s="31">
-        <v>44928</v>
+        <v>44927</v>
       </c>
       <c r="L184" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M184" s="45"/>
       <c r="N184" s="44" t="s">
-        <v>911</v>
+        <v>831</v>
       </c>
       <c r="O184" s="27"/>
       <c r="P184" s="24"/>
@@ -13918,16 +13930,16 @@
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>844</v>
+        <v>827</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>845</v>
+        <v>828</v>
       </c>
       <c r="C185" s="13" t="s">
-        <v>846</v>
+        <v>288</v>
       </c>
       <c r="D185" s="13" t="s">
-        <v>847</v>
+        <v>331</v>
       </c>
       <c r="E185" s="14">
         <v>2022</v>
@@ -13948,14 +13960,14 @@
         <v>14</v>
       </c>
       <c r="K185" s="31">
-        <v>44929</v>
+        <v>44928</v>
       </c>
       <c r="L185" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M185" s="45"/>
       <c r="N185" s="44" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="O185" s="27"/>
       <c r="P185" s="24"/>
@@ -13967,16 +13979,16 @@
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" s="13" t="s">
-        <v>928</v>
+        <v>844</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>929</v>
+        <v>845</v>
       </c>
       <c r="C186" s="13" t="s">
-        <v>512</v>
+        <v>846</v>
       </c>
       <c r="D186" s="13" t="s">
-        <v>513</v>
+        <v>847</v>
       </c>
       <c r="E186" s="14">
         <v>2022</v>
@@ -13997,14 +14009,14 @@
         <v>14</v>
       </c>
       <c r="K186" s="31">
-        <v>44930</v>
+        <v>44929</v>
       </c>
       <c r="L186" s="31" t="s">
         <v>274</v>
       </c>
       <c r="M186" s="45"/>
       <c r="N186" s="44" t="s">
-        <v>930</v>
+        <v>915</v>
       </c>
       <c r="O186" s="27"/>
       <c r="P186" s="24"/>
@@ -14480,7 +14492,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -14529,8 +14541,8 @@
         <v>44191</v>
       </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2:F17" ca="1" si="0">TODAY()-E2</f>
-        <v>425</v>
+        <f t="shared" ref="F2:F18" ca="1" si="0">TODAY()-E2</f>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14551,7 +14563,7 @@
       </c>
       <c r="F3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14572,7 +14584,7 @@
       </c>
       <c r="F4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -14593,7 +14605,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -14614,7 +14626,7 @@
       </c>
       <c r="F6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -14635,7 +14647,7 @@
       </c>
       <c r="F7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -14656,7 +14668,7 @@
       </c>
       <c r="F8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -14677,7 +14689,7 @@
       </c>
       <c r="F9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -14698,7 +14710,7 @@
       </c>
       <c r="F10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -14719,7 +14731,7 @@
       </c>
       <c r="F11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -14740,7 +14752,7 @@
       </c>
       <c r="F12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -14761,7 +14773,7 @@
       </c>
       <c r="F13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -14782,7 +14794,7 @@
       </c>
       <c r="F14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -14803,7 +14815,7 @@
       </c>
       <c r="F15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -14824,7 +14836,7 @@
       </c>
       <c r="F16" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -14845,7 +14857,28 @@
       </c>
       <c r="F17" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>933</v>
+      </c>
+      <c r="E18" s="10">
+        <v>44622</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14910,7 +14943,7 @@
       </c>
       <c r="F2" s="40">
         <f t="shared" ref="F2:F4" ca="1" si="0">(TODAY()-E2)/365</f>
-        <v>6.3232876712328769</v>
+        <v>6.3397260273972602</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14931,7 +14964,7 @@
       </c>
       <c r="F3" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3232876712328769</v>
+        <v>6.3397260273972602</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14952,7 +14985,7 @@
       </c>
       <c r="F4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7013698630136984</v>
+        <v>5.7178082191780826</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -14973,7 +15006,7 @@
       </c>
       <c r="F5" s="40">
         <f ca="1">(TODAY()-E5)/365</f>
-        <v>4.0712328767123287</v>
+        <v>4.087671232876712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>